<commit_message>
FPT Index testing Data push from IMIS
</commit_message>
<xml_diff>
--- a/web/hca.xlsx
+++ b/web/hca.xlsx
@@ -2429,6 +2429,18 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="72" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2597,41 +2609,29 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="72" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -3610,114 +3610,114 @@
       <pane xSplit="3" ySplit="10" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="O11" sqref="O11"/>
+      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="89.42578125" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="155.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.59765625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="89.3984375" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.59765625" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="155.1328125" style="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="164" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.73046875" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.265625" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.3984375" style="17" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.73046875" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.265625" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.3984375" style="15" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.73046875" style="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.265625" style="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.3984375" style="15" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18" style="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.85546875" style="15"/>
+    <col min="18" max="16384" width="8.86328125" style="15"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:17" s="1" customFormat="1">
-      <c r="A2" s="204"/>
-      <c r="B2" s="204"/>
-      <c r="C2" s="204"/>
-      <c r="D2" s="204"/>
-      <c r="E2" s="204"/>
-      <c r="F2" s="204"/>
-      <c r="G2" s="204"/>
-      <c r="H2" s="204"/>
-      <c r="I2" s="204"/>
+      <c r="A2" s="208"/>
+      <c r="B2" s="208"/>
+      <c r="C2" s="208"/>
+      <c r="D2" s="208"/>
+      <c r="E2" s="208"/>
+      <c r="F2" s="208"/>
+      <c r="G2" s="208"/>
+      <c r="H2" s="208"/>
+      <c r="I2" s="208"/>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1">
-      <c r="A3" s="204"/>
-      <c r="B3" s="204"/>
-      <c r="C3" s="204"/>
-      <c r="D3" s="204"/>
-      <c r="E3" s="204"/>
-      <c r="F3" s="204"/>
-      <c r="G3" s="204"/>
-      <c r="H3" s="204"/>
-      <c r="I3" s="204"/>
+      <c r="A3" s="208"/>
+      <c r="B3" s="208"/>
+      <c r="C3" s="208"/>
+      <c r="D3" s="208"/>
+      <c r="E3" s="208"/>
+      <c r="F3" s="208"/>
+      <c r="G3" s="208"/>
+      <c r="H3" s="208"/>
+      <c r="I3" s="208"/>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1">
-      <c r="A4" s="204"/>
-      <c r="B4" s="204"/>
-      <c r="C4" s="204"/>
-      <c r="D4" s="204"/>
-      <c r="E4" s="204"/>
-      <c r="F4" s="204"/>
-      <c r="G4" s="204"/>
-      <c r="H4" s="204"/>
-      <c r="I4" s="204"/>
-    </row>
-    <row r="6" spans="1:17" ht="26.25">
-      <c r="A6" s="211" t="s">
+      <c r="A4" s="208"/>
+      <c r="B4" s="208"/>
+      <c r="C4" s="208"/>
+      <c r="D4" s="208"/>
+      <c r="E4" s="208"/>
+      <c r="F4" s="208"/>
+      <c r="G4" s="208"/>
+      <c r="H4" s="208"/>
+      <c r="I4" s="208"/>
+    </row>
+    <row r="6" spans="1:17" ht="25.15">
+      <c r="A6" s="215" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="211"/>
-      <c r="C6" s="211"/>
-      <c r="D6" s="211"/>
-      <c r="E6" s="211"/>
-      <c r="F6" s="211"/>
-      <c r="G6" s="211"/>
-      <c r="H6" s="211"/>
-      <c r="I6" s="211"/>
-      <c r="J6" s="211"/>
-      <c r="K6" s="211"/>
-      <c r="L6" s="211"/>
-      <c r="M6" s="211"/>
-      <c r="N6" s="211"/>
-      <c r="O6" s="211"/>
-      <c r="P6" s="211"/>
-      <c r="Q6" s="211"/>
-    </row>
-    <row r="7" spans="1:17" ht="15.75" thickBot="1"/>
+      <c r="B6" s="215"/>
+      <c r="C6" s="215"/>
+      <c r="D6" s="215"/>
+      <c r="E6" s="215"/>
+      <c r="F6" s="215"/>
+      <c r="G6" s="215"/>
+      <c r="H6" s="215"/>
+      <c r="I6" s="215"/>
+      <c r="J6" s="215"/>
+      <c r="K6" s="215"/>
+      <c r="L6" s="215"/>
+      <c r="M6" s="215"/>
+      <c r="N6" s="215"/>
+      <c r="O6" s="215"/>
+      <c r="P6" s="215"/>
+      <c r="Q6" s="215"/>
+    </row>
+    <row r="7" spans="1:17" ht="15.4" thickBot="1"/>
     <row r="8" spans="1:17" s="18" customFormat="1" ht="25.15" customHeight="1" thickTop="1">
       <c r="A8" s="25"/>
-      <c r="B8" s="212" t="s">
+      <c r="B8" s="216" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="212"/>
-      <c r="D8" s="212"/>
-      <c r="E8" s="212"/>
-      <c r="F8" s="213" t="s">
+      <c r="C8" s="216"/>
+      <c r="D8" s="216"/>
+      <c r="E8" s="216"/>
+      <c r="F8" s="217" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="213"/>
-      <c r="H8" s="213"/>
-      <c r="I8" s="213"/>
-      <c r="J8" s="213" t="s">
+      <c r="G8" s="217"/>
+      <c r="H8" s="217"/>
+      <c r="I8" s="217"/>
+      <c r="J8" s="217" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="213"/>
-      <c r="L8" s="213"/>
-      <c r="M8" s="213"/>
-      <c r="N8" s="213" t="s">
+      <c r="K8" s="217"/>
+      <c r="L8" s="217"/>
+      <c r="M8" s="217"/>
+      <c r="N8" s="217" t="s">
         <v>33</v>
       </c>
-      <c r="O8" s="213"/>
-      <c r="P8" s="213"/>
-      <c r="Q8" s="221"/>
-    </row>
-    <row r="9" spans="1:17" s="24" customFormat="1" ht="15.75">
+      <c r="O8" s="217"/>
+      <c r="P8" s="217"/>
+      <c r="Q8" s="225"/>
+    </row>
+    <row r="9" spans="1:17" s="24" customFormat="1">
       <c r="A9" s="19" t="s">
         <v>17</v>
       </c>
@@ -3771,31 +3771,31 @@
       </c>
     </row>
     <row r="10" spans="1:17" s="32" customFormat="1" ht="58.15" customHeight="1">
-      <c r="A10" s="214" t="s">
+      <c r="A10" s="218" t="s">
         <v>89</v>
       </c>
-      <c r="B10" s="215"/>
-      <c r="C10" s="215"/>
-      <c r="D10" s="215"/>
-      <c r="E10" s="215"/>
-      <c r="F10" s="216" t="s">
+      <c r="B10" s="219"/>
+      <c r="C10" s="219"/>
+      <c r="D10" s="219"/>
+      <c r="E10" s="219"/>
+      <c r="F10" s="220" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="216"/>
-      <c r="H10" s="216"/>
-      <c r="I10" s="216"/>
-      <c r="J10" s="216" t="s">
+      <c r="G10" s="220"/>
+      <c r="H10" s="220"/>
+      <c r="I10" s="220"/>
+      <c r="J10" s="220" t="s">
         <v>39</v>
       </c>
-      <c r="K10" s="216"/>
-      <c r="L10" s="216"/>
-      <c r="M10" s="216"/>
-      <c r="N10" s="216" t="s">
+      <c r="K10" s="220"/>
+      <c r="L10" s="220"/>
+      <c r="M10" s="220"/>
+      <c r="N10" s="220" t="s">
         <v>40</v>
       </c>
-      <c r="O10" s="216"/>
-      <c r="P10" s="216"/>
-      <c r="Q10" s="217"/>
+      <c r="O10" s="220"/>
+      <c r="P10" s="220"/>
+      <c r="Q10" s="221"/>
     </row>
     <row r="11" spans="1:17" s="38" customFormat="1" ht="43.9" customHeight="1">
       <c r="A11" s="34">
@@ -3959,7 +3959,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="38" customFormat="1" ht="36">
+    <row r="15" spans="1:17" s="38" customFormat="1" ht="34.5">
       <c r="A15" s="34">
         <v>5</v>
       </c>
@@ -3998,7 +3998,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="38" customFormat="1" ht="36">
+    <row r="16" spans="1:17" s="38" customFormat="1" ht="17.25">
       <c r="A16" s="39">
         <v>6</v>
       </c>
@@ -4070,7 +4070,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="38" customFormat="1" ht="36">
+    <row r="18" spans="1:17" s="38" customFormat="1" ht="17.25">
       <c r="A18" s="39">
         <v>8</v>
       </c>
@@ -4103,7 +4103,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="38" customFormat="1" ht="36">
+    <row r="19" spans="1:17" s="38" customFormat="1" ht="17.25">
       <c r="A19" s="34">
         <v>9</v>
       </c>
@@ -4142,7 +4142,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="38" customFormat="1" ht="36">
+    <row r="20" spans="1:17" s="38" customFormat="1" ht="35.25">
       <c r="A20" s="34">
         <v>10</v>
       </c>
@@ -4181,7 +4181,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="33" customFormat="1" ht="20.25">
+    <row r="21" spans="1:17" s="33" customFormat="1" ht="20.65">
       <c r="A21" s="29">
         <v>11</v>
       </c>
@@ -4189,24 +4189,24 @@
         <v>48</v>
       </c>
       <c r="C21" s="31"/>
-      <c r="D21" s="189" t="s">
+      <c r="D21" s="193" t="s">
         <v>93</v>
       </c>
-      <c r="E21" s="190"/>
-      <c r="F21" s="190"/>
-      <c r="G21" s="190"/>
-      <c r="H21" s="190"/>
-      <c r="I21" s="190"/>
-      <c r="J21" s="190"/>
-      <c r="K21" s="190"/>
-      <c r="L21" s="190"/>
-      <c r="M21" s="190"/>
-      <c r="N21" s="190"/>
-      <c r="O21" s="190"/>
-      <c r="P21" s="190"/>
-      <c r="Q21" s="191"/>
-    </row>
-    <row r="22" spans="1:17" s="14" customFormat="1" ht="18">
+      <c r="E21" s="194"/>
+      <c r="F21" s="194"/>
+      <c r="G21" s="194"/>
+      <c r="H21" s="194"/>
+      <c r="I21" s="194"/>
+      <c r="J21" s="194"/>
+      <c r="K21" s="194"/>
+      <c r="L21" s="194"/>
+      <c r="M21" s="194"/>
+      <c r="N21" s="194"/>
+      <c r="O21" s="194"/>
+      <c r="P21" s="194"/>
+      <c r="Q21" s="195"/>
+    </row>
+    <row r="22" spans="1:17" s="14" customFormat="1" ht="17.25">
       <c r="A22" s="69">
         <v>11.1</v>
       </c>
@@ -4217,7 +4217,7 @@
       <c r="D22" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="201" t="s">
+      <c r="E22" s="205" t="s">
         <v>56</v>
       </c>
       <c r="F22" s="35"/>
@@ -4245,7 +4245,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="14" customFormat="1" ht="18">
+    <row r="23" spans="1:17" s="14" customFormat="1" ht="17.25">
       <c r="A23" s="69">
         <v>11.2</v>
       </c>
@@ -4256,7 +4256,7 @@
       <c r="D23" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="202"/>
+      <c r="E23" s="206"/>
       <c r="F23" s="40" t="s">
         <v>44</v>
       </c>
@@ -4288,7 +4288,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="14" customFormat="1" ht="18">
+    <row r="24" spans="1:17" s="14" customFormat="1" ht="17.25">
       <c r="A24" s="69">
         <v>11.3</v>
       </c>
@@ -4299,7 +4299,7 @@
       <c r="D24" s="69" t="s">
         <v>82</v>
       </c>
-      <c r="E24" s="203"/>
+      <c r="E24" s="207"/>
       <c r="F24" s="35"/>
       <c r="G24" s="35" t="s">
         <v>41</v>
@@ -4325,7 +4325,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="14" customFormat="1" ht="36">
+    <row r="25" spans="1:17" s="14" customFormat="1" ht="17.25">
       <c r="A25" s="69">
         <v>11.4</v>
       </c>
@@ -4336,7 +4336,7 @@
       <c r="D25" s="69" t="s">
         <v>83</v>
       </c>
-      <c r="E25" s="201" t="s">
+      <c r="E25" s="205" t="s">
         <v>80</v>
       </c>
       <c r="F25" s="40"/>
@@ -4364,7 +4364,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="14" customFormat="1" ht="18.75" thickBot="1">
+    <row r="26" spans="1:17" s="14" customFormat="1" ht="17.649999999999999" thickBot="1">
       <c r="A26" s="69">
         <v>11.5</v>
       </c>
@@ -4375,7 +4375,7 @@
       <c r="D26" s="69" t="s">
         <v>84</v>
       </c>
-      <c r="E26" s="203"/>
+      <c r="E26" s="207"/>
       <c r="F26" s="45"/>
       <c r="G26" s="45" t="s">
         <v>41</v>
@@ -4401,51 +4401,51 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A27" s="218"/>
-      <c r="B27" s="219"/>
-      <c r="C27" s="219"/>
-      <c r="D27" s="219"/>
-      <c r="E27" s="219"/>
-      <c r="F27" s="219"/>
-      <c r="G27" s="219"/>
-      <c r="H27" s="219"/>
-      <c r="I27" s="219"/>
-      <c r="J27" s="219"/>
-      <c r="K27" s="219"/>
-      <c r="L27" s="219"/>
-      <c r="M27" s="219"/>
-      <c r="N27" s="219"/>
-      <c r="O27" s="219"/>
-      <c r="P27" s="219"/>
-      <c r="Q27" s="220"/>
+    <row r="27" spans="1:17" ht="15.75" thickTop="1" thickBot="1">
+      <c r="A27" s="222"/>
+      <c r="B27" s="223"/>
+      <c r="C27" s="223"/>
+      <c r="D27" s="223"/>
+      <c r="E27" s="223"/>
+      <c r="F27" s="223"/>
+      <c r="G27" s="223"/>
+      <c r="H27" s="223"/>
+      <c r="I27" s="223"/>
+      <c r="J27" s="223"/>
+      <c r="K27" s="223"/>
+      <c r="L27" s="223"/>
+      <c r="M27" s="223"/>
+      <c r="N27" s="223"/>
+      <c r="O27" s="223"/>
+      <c r="P27" s="223"/>
+      <c r="Q27" s="224"/>
     </row>
     <row r="28" spans="1:17" s="32" customFormat="1" ht="21" thickTop="1">
-      <c r="A28" s="208" t="s">
+      <c r="A28" s="212" t="s">
         <v>90</v>
       </c>
-      <c r="B28" s="209"/>
-      <c r="C28" s="209"/>
-      <c r="D28" s="209"/>
-      <c r="E28" s="210"/>
-      <c r="F28" s="198" t="s">
+      <c r="B28" s="213"/>
+      <c r="C28" s="213"/>
+      <c r="D28" s="213"/>
+      <c r="E28" s="214"/>
+      <c r="F28" s="202" t="s">
         <v>45</v>
       </c>
-      <c r="G28" s="199"/>
-      <c r="H28" s="199"/>
-      <c r="I28" s="200"/>
-      <c r="J28" s="195" t="s">
+      <c r="G28" s="203"/>
+      <c r="H28" s="203"/>
+      <c r="I28" s="204"/>
+      <c r="J28" s="199" t="s">
         <v>45</v>
       </c>
-      <c r="K28" s="196"/>
-      <c r="L28" s="196"/>
-      <c r="M28" s="197"/>
-      <c r="N28" s="192" t="s">
+      <c r="K28" s="200"/>
+      <c r="L28" s="200"/>
+      <c r="M28" s="201"/>
+      <c r="N28" s="196" t="s">
         <v>45</v>
       </c>
-      <c r="O28" s="193"/>
-      <c r="P28" s="193"/>
-      <c r="Q28" s="194"/>
+      <c r="O28" s="197"/>
+      <c r="P28" s="197"/>
+      <c r="Q28" s="198"/>
     </row>
     <row r="29" spans="1:17" s="38" customFormat="1" ht="55.5" customHeight="1">
       <c r="A29" s="69">
@@ -4630,7 +4630,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="13" customFormat="1" ht="20.25">
+    <row r="34" spans="1:17" s="13" customFormat="1" ht="20.65">
       <c r="A34" s="29">
         <v>17</v>
       </c>
@@ -4638,22 +4638,22 @@
         <v>23</v>
       </c>
       <c r="C34" s="31"/>
-      <c r="D34" s="189" t="s">
+      <c r="D34" s="193" t="s">
         <v>93</v>
       </c>
-      <c r="E34" s="190"/>
-      <c r="F34" s="190"/>
-      <c r="G34" s="190"/>
-      <c r="H34" s="190"/>
-      <c r="I34" s="190"/>
-      <c r="J34" s="190"/>
-      <c r="K34" s="190"/>
-      <c r="L34" s="190"/>
-      <c r="M34" s="190"/>
-      <c r="N34" s="190"/>
-      <c r="O34" s="190"/>
-      <c r="P34" s="190"/>
-      <c r="Q34" s="191"/>
+      <c r="E34" s="194"/>
+      <c r="F34" s="194"/>
+      <c r="G34" s="194"/>
+      <c r="H34" s="194"/>
+      <c r="I34" s="194"/>
+      <c r="J34" s="194"/>
+      <c r="K34" s="194"/>
+      <c r="L34" s="194"/>
+      <c r="M34" s="194"/>
+      <c r="N34" s="194"/>
+      <c r="O34" s="194"/>
+      <c r="P34" s="194"/>
+      <c r="Q34" s="195"/>
     </row>
     <row r="35" spans="1:17" s="14" customFormat="1" ht="41.65" customHeight="1">
       <c r="A35" s="69">
@@ -4666,7 +4666,7 @@
       <c r="D35" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="205" t="s">
+      <c r="E35" s="209" t="s">
         <v>116</v>
       </c>
       <c r="F35" s="59"/>
@@ -4705,7 +4705,7 @@
       <c r="D36" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="E36" s="206"/>
+      <c r="E36" s="210"/>
       <c r="F36" s="61"/>
       <c r="G36" s="40" t="s">
         <v>77</v>
@@ -4742,7 +4742,7 @@
       <c r="D37" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="207"/>
+      <c r="E37" s="211"/>
       <c r="F37" s="59" t="s">
         <v>47</v>
       </c>
@@ -4785,7 +4785,7 @@
       <c r="D38" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="E38" s="205" t="s">
+      <c r="E38" s="209" t="s">
         <v>79</v>
       </c>
       <c r="F38" s="61"/>
@@ -4824,7 +4824,7 @@
       <c r="D39" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="E39" s="206"/>
+      <c r="E39" s="210"/>
       <c r="F39" s="59"/>
       <c r="G39" s="35" t="s">
         <v>77</v>
@@ -4861,7 +4861,7 @@
       <c r="D40" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="E40" s="207"/>
+      <c r="E40" s="211"/>
       <c r="F40" s="63"/>
       <c r="G40" s="64" t="s">
         <v>77</v>
@@ -4887,7 +4887,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="15.75" thickTop="1"/>
+    <row r="41" spans="1:17" ht="15.4" thickTop="1"/>
   </sheetData>
   <mergeCells count="21">
     <mergeCell ref="A2:I4"/>
@@ -4936,27 +4936,27 @@
       <pane xSplit="3" ySplit="7" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="12.5703125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="129.28515625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="72" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="71" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.5703125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="37.140625" style="1" customWidth="1"/>
-    <col min="12" max="15" width="9.140625" style="1"/>
-    <col min="16" max="16" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1328125" style="1"/>
+    <col min="2" max="2" width="12.59765625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="129.265625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="17.86328125" style="72" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.73046875" style="71" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.3984375" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.59765625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="6.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37.1328125" style="1" customWidth="1"/>
+    <col min="12" max="15" width="9.1328125" style="1"/>
+    <col min="16" max="16" width="15.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.73046875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="15.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:23" s="75" customFormat="1" ht="34.35" hidden="1" customHeight="1" thickBot="1">
@@ -4985,12 +4985,12 @@
         <v>2020</v>
       </c>
       <c r="J1" s="88"/>
-      <c r="K1" s="222" t="s">
+      <c r="K1" s="226" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="223"/>
-      <c r="M1" s="223"/>
-      <c r="N1" s="224"/>
+      <c r="L1" s="227"/>
+      <c r="M1" s="227"/>
+      <c r="N1" s="228"/>
       <c r="O1" s="89"/>
       <c r="P1" s="90">
         <f>DATE(I1,G1,"01")</f>
@@ -5013,25 +5013,25 @@
       <c r="W1" s="74"/>
     </row>
     <row r="2" spans="2:23" s="77" customFormat="1" ht="34.35" hidden="1" customHeight="1" thickBot="1">
-      <c r="B2" s="231" t="s">
+      <c r="B2" s="235" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="232"/>
-      <c r="D2" s="232"/>
-      <c r="E2" s="232"/>
-      <c r="F2" s="232"/>
-      <c r="G2" s="232"/>
-      <c r="H2" s="232"/>
-      <c r="I2" s="232"/>
-      <c r="J2" s="232"/>
-      <c r="K2" s="232"/>
-      <c r="L2" s="232"/>
-      <c r="M2" s="232"/>
-      <c r="N2" s="232"/>
-      <c r="O2" s="232"/>
-      <c r="P2" s="232"/>
-      <c r="Q2" s="232"/>
-      <c r="R2" s="233"/>
+      <c r="C2" s="236"/>
+      <c r="D2" s="236"/>
+      <c r="E2" s="236"/>
+      <c r="F2" s="236"/>
+      <c r="G2" s="236"/>
+      <c r="H2" s="236"/>
+      <c r="I2" s="236"/>
+      <c r="J2" s="236"/>
+      <c r="K2" s="236"/>
+      <c r="L2" s="236"/>
+      <c r="M2" s="236"/>
+      <c r="N2" s="236"/>
+      <c r="O2" s="236"/>
+      <c r="P2" s="236"/>
+      <c r="Q2" s="236"/>
+      <c r="R2" s="237"/>
       <c r="S2" s="76"/>
       <c r="V2" s="73">
         <v>1</v>
@@ -5061,14 +5061,14 @@
       <c r="W3" s="78"/>
     </row>
     <row r="4" spans="2:23" s="77" customFormat="1" ht="24" customHeight="1" thickBot="1">
-      <c r="B4" s="228" t="str">
+      <c r="B4" s="232" t="str">
         <f>B1&amp;" : "&amp;C1&amp;"                                                           MFLCode : "&amp;E1&amp;"                                                    Reporting Month :   "&amp;G1&amp;"                                             Reporting Year: "&amp;I1</f>
         <v>Health Facility : Likii Dispensary                                                           MFLCode : 15035                                                    Reporting Month :   02                                             Reporting Year: 2020</v>
       </c>
-      <c r="C4" s="229"/>
-      <c r="D4" s="229"/>
-      <c r="E4" s="229"/>
-      <c r="F4" s="230"/>
+      <c r="C4" s="233"/>
+      <c r="D4" s="233"/>
+      <c r="E4" s="233"/>
+      <c r="F4" s="234"/>
       <c r="G4" s="93"/>
       <c r="H4" s="94"/>
       <c r="I4" s="94"/>
@@ -5094,15 +5094,15 @@
       <c r="W4" s="78"/>
     </row>
     <row r="5" spans="2:23" s="81" customFormat="1" ht="30.75" customHeight="1" thickBot="1">
-      <c r="B5" s="234" t="s">
+      <c r="B5" s="238" t="s">
         <v>110</v>
       </c>
-      <c r="C5" s="235"/>
-      <c r="D5" s="225" t="s">
+      <c r="C5" s="239"/>
+      <c r="D5" s="229" t="s">
         <v>111</v>
       </c>
-      <c r="E5" s="226"/>
-      <c r="F5" s="227"/>
+      <c r="E5" s="230"/>
+      <c r="F5" s="231"/>
       <c r="G5" s="97"/>
       <c r="H5" s="97"/>
       <c r="I5" s="97"/>
@@ -5124,10 +5124,10 @@
       <c r="W5" s="80"/>
     </row>
     <row r="6" spans="2:23" s="2" customFormat="1" ht="27.75" customHeight="1" thickBot="1">
-      <c r="B6" s="240" t="s">
+      <c r="B6" s="244" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="241"/>
+      <c r="C6" s="245"/>
       <c r="D6" s="98" t="s">
         <v>115</v>
       </c>
@@ -5136,12 +5136,12 @@
         <v>43497</v>
       </c>
       <c r="F6" s="100"/>
-      <c r="G6" s="244"/>
-      <c r="H6" s="236" t="s">
+      <c r="G6" s="248"/>
+      <c r="H6" s="240" t="s">
         <v>86</v>
       </c>
-      <c r="I6" s="237"/>
-      <c r="J6" s="238"/>
+      <c r="I6" s="241"/>
+      <c r="J6" s="242"/>
       <c r="K6" s="101"/>
       <c r="L6" s="101"/>
       <c r="M6" s="101"/>
@@ -5167,7 +5167,7 @@
       <c r="F7" s="106" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="244"/>
+      <c r="G7" s="248"/>
       <c r="H7" s="107" t="s">
         <v>0</v>
       </c>
@@ -5199,7 +5199,7 @@
         <f>IFERROR(D8/E8,)</f>
         <v>0</v>
       </c>
-      <c r="G8" s="244"/>
+      <c r="G8" s="248"/>
       <c r="H8" s="115"/>
       <c r="I8" s="116" t="s">
         <v>41</v>
@@ -5233,7 +5233,7 @@
         <f t="shared" ref="F9:F23" si="0">IFERROR(D9/E9,)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="244"/>
+      <c r="G9" s="248"/>
       <c r="H9" s="115"/>
       <c r="I9" s="116" t="s">
         <v>41</v>
@@ -5267,7 +5267,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G10" s="244"/>
+      <c r="G10" s="248"/>
       <c r="H10" s="121" t="s">
         <v>43</v>
       </c>
@@ -5303,7 +5303,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G11" s="244"/>
+      <c r="G11" s="248"/>
       <c r="H11" s="115"/>
       <c r="I11" s="122" t="s">
         <v>43</v>
@@ -5337,7 +5337,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G12" s="244"/>
+      <c r="G12" s="248"/>
       <c r="H12" s="125" t="s">
         <v>91</v>
       </c>
@@ -5370,7 +5370,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G13" s="244"/>
+      <c r="G13" s="248"/>
       <c r="H13" s="126"/>
       <c r="I13" s="127"/>
       <c r="J13" s="117"/>
@@ -5402,7 +5402,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G14" s="244"/>
+      <c r="G14" s="248"/>
       <c r="H14" s="128" t="s">
         <v>44</v>
       </c>
@@ -5435,7 +5435,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G15" s="244"/>
+      <c r="G15" s="248"/>
       <c r="H15" s="115"/>
       <c r="I15" s="127"/>
       <c r="J15" s="117"/>
@@ -5467,7 +5467,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G16" s="244"/>
+      <c r="G16" s="248"/>
       <c r="H16" s="115"/>
       <c r="I16" s="129" t="s">
         <v>44</v>
@@ -5501,7 +5501,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G17" s="244"/>
+      <c r="G17" s="248"/>
       <c r="H17" s="115"/>
       <c r="I17" s="129" t="s">
         <v>44</v>
@@ -5529,7 +5529,7 @@
       <c r="D18" s="174"/>
       <c r="E18" s="174"/>
       <c r="F18" s="175"/>
-      <c r="G18" s="244"/>
+      <c r="G18" s="248"/>
       <c r="H18" s="130"/>
       <c r="I18" s="131"/>
       <c r="J18" s="132"/>
@@ -5558,7 +5558,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G19" s="244"/>
+      <c r="G19" s="248"/>
       <c r="H19" s="115"/>
       <c r="I19" s="116" t="s">
         <v>41</v>
@@ -5595,7 +5595,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G20" s="244"/>
+      <c r="G20" s="248"/>
       <c r="H20" s="128" t="s">
         <v>44</v>
       </c>
@@ -5631,7 +5631,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G21" s="244"/>
+      <c r="G21" s="248"/>
       <c r="H21" s="115"/>
       <c r="I21" s="116" t="s">
         <v>41</v>
@@ -5665,7 +5665,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G22" s="244"/>
+      <c r="G22" s="248"/>
       <c r="H22" s="115"/>
       <c r="I22" s="116" t="s">
         <v>41</v>
@@ -5684,22 +5684,22 @@
       <c r="R22" s="118"/>
     </row>
     <row r="23" spans="2:18" s="3" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B23" s="247">
+      <c r="B23" s="189">
         <v>11.5</v>
       </c>
-      <c r="C23" s="248" t="s">
+      <c r="C23" s="190" t="s">
         <v>16</v>
       </c>
       <c r="D23" s="181"/>
-      <c r="E23" s="249">
+      <c r="E23" s="191">
         <f>E8</f>
         <v>0</v>
       </c>
-      <c r="F23" s="250">
+      <c r="F23" s="192">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="244"/>
+      <c r="G23" s="248"/>
       <c r="H23" s="139"/>
       <c r="I23" s="140" t="s">
         <v>41</v>
@@ -5718,17 +5718,17 @@
       <c r="R23" s="118"/>
     </row>
     <row r="24" spans="2:18" ht="16.5" customHeight="1">
-      <c r="B24" s="251" t="s">
+      <c r="B24" s="249" t="s">
         <v>80</v>
       </c>
-      <c r="C24" s="252"/>
-      <c r="D24" s="252"/>
-      <c r="E24" s="252"/>
-      <c r="F24" s="253"/>
-      <c r="G24" s="244"/>
-      <c r="H24" s="245"/>
-      <c r="I24" s="245"/>
-      <c r="J24" s="245"/>
+      <c r="C24" s="250"/>
+      <c r="D24" s="250"/>
+      <c r="E24" s="250"/>
+      <c r="F24" s="251"/>
+      <c r="G24" s="248"/>
+      <c r="H24" s="255"/>
+      <c r="I24" s="255"/>
+      <c r="J24" s="255"/>
       <c r="K24" s="133"/>
       <c r="L24" s="133"/>
       <c r="M24" s="133"/>
@@ -5739,15 +5739,15 @@
       <c r="R24" s="133"/>
     </row>
     <row r="25" spans="2:18" ht="9.75" customHeight="1" thickBot="1">
-      <c r="B25" s="254"/>
-      <c r="C25" s="255"/>
-      <c r="D25" s="255"/>
-      <c r="E25" s="255"/>
-      <c r="F25" s="256"/>
-      <c r="G25" s="244"/>
-      <c r="H25" s="245"/>
-      <c r="I25" s="245"/>
-      <c r="J25" s="245"/>
+      <c r="B25" s="252"/>
+      <c r="C25" s="253"/>
+      <c r="D25" s="253"/>
+      <c r="E25" s="253"/>
+      <c r="F25" s="254"/>
+      <c r="G25" s="248"/>
+      <c r="H25" s="255"/>
+      <c r="I25" s="255"/>
+      <c r="J25" s="255"/>
       <c r="K25" s="133"/>
       <c r="L25" s="133"/>
       <c r="M25" s="133"/>
@@ -5758,10 +5758,10 @@
       <c r="R25" s="133"/>
     </row>
     <row r="26" spans="2:18" s="5" customFormat="1" ht="32.25" customHeight="1" thickBot="1">
-      <c r="B26" s="242" t="s">
+      <c r="B26" s="246" t="s">
         <v>90</v>
       </c>
-      <c r="C26" s="243"/>
+      <c r="C26" s="247"/>
       <c r="D26" s="142" t="s">
         <v>115</v>
       </c>
@@ -5770,12 +5770,12 @@
         <v>43132</v>
       </c>
       <c r="F26" s="144"/>
-      <c r="G26" s="244"/>
-      <c r="H26" s="236" t="s">
+      <c r="G26" s="248"/>
+      <c r="H26" s="240" t="s">
         <v>86</v>
       </c>
-      <c r="I26" s="237"/>
-      <c r="J26" s="238"/>
+      <c r="I26" s="241"/>
+      <c r="J26" s="242"/>
       <c r="K26" s="145"/>
       <c r="L26" s="145"/>
       <c r="M26" s="145"/>
@@ -5801,7 +5801,7 @@
       <c r="F27" s="149" t="s">
         <v>2</v>
       </c>
-      <c r="G27" s="244"/>
+      <c r="G27" s="248"/>
       <c r="H27" s="107" t="s">
         <v>0</v>
       </c>
@@ -5833,7 +5833,7 @@
         <f t="shared" ref="F28:F39" si="2">IFERROR(D28/E28,)</f>
         <v>0</v>
       </c>
-      <c r="G28" s="244"/>
+      <c r="G28" s="248"/>
       <c r="H28" s="115" t="s">
         <v>46</v>
       </c>
@@ -5867,7 +5867,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G29" s="244"/>
+      <c r="G29" s="248"/>
       <c r="H29" s="115"/>
       <c r="I29" s="152" t="s">
         <v>46</v>
@@ -5898,7 +5898,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G30" s="244"/>
+      <c r="G30" s="248"/>
       <c r="H30" s="115"/>
       <c r="I30" s="152"/>
       <c r="J30" s="134"/>
@@ -5927,7 +5927,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G31" s="244"/>
+      <c r="G31" s="248"/>
       <c r="H31" s="155"/>
       <c r="I31" s="156"/>
       <c r="J31" s="134"/>
@@ -5956,7 +5956,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G32" s="244"/>
+      <c r="G32" s="248"/>
       <c r="H32" s="115"/>
       <c r="I32" s="152" t="s">
         <v>47</v>
@@ -5984,7 +5984,7 @@
       <c r="D33" s="160"/>
       <c r="E33" s="187"/>
       <c r="F33" s="161"/>
-      <c r="G33" s="244"/>
+      <c r="G33" s="248"/>
       <c r="H33" s="162"/>
       <c r="I33" s="163"/>
       <c r="J33" s="164"/>
@@ -6010,7 +6010,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G34" s="244"/>
+      <c r="G34" s="248"/>
       <c r="H34" s="165"/>
       <c r="I34" s="166" t="s">
         <v>77</v>
@@ -6044,7 +6044,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G35" s="244"/>
+      <c r="G35" s="248"/>
       <c r="H35" s="168"/>
       <c r="I35" s="166" t="s">
         <v>77</v>
@@ -6081,7 +6081,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G36" s="244"/>
+      <c r="G36" s="248"/>
       <c r="H36" s="169" t="s">
         <v>47</v>
       </c>
@@ -6117,7 +6117,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G37" s="244"/>
+      <c r="G37" s="248"/>
       <c r="H37" s="115"/>
       <c r="I37" s="166" t="s">
         <v>77</v>
@@ -6151,7 +6151,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G38" s="244"/>
+      <c r="G38" s="248"/>
       <c r="H38" s="155"/>
       <c r="I38" s="166" t="s">
         <v>77</v>
@@ -6185,7 +6185,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G39" s="244"/>
+      <c r="G39" s="248"/>
       <c r="H39" s="139"/>
       <c r="I39" s="170" t="s">
         <v>77</v>
@@ -6204,17 +6204,17 @@
       <c r="R39" s="167"/>
     </row>
     <row r="40" spans="2:18" s="8" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B40" s="246" t="s">
+      <c r="B40" s="256" t="s">
         <v>79</v>
       </c>
-      <c r="C40" s="246"/>
-      <c r="D40" s="246"/>
-      <c r="E40" s="246"/>
-      <c r="F40" s="246"/>
-      <c r="G40" s="244"/>
-      <c r="H40" s="239"/>
-      <c r="I40" s="239"/>
-      <c r="J40" s="239"/>
+      <c r="C40" s="256"/>
+      <c r="D40" s="256"/>
+      <c r="E40" s="256"/>
+      <c r="F40" s="256"/>
+      <c r="G40" s="248"/>
+      <c r="H40" s="243"/>
+      <c r="I40" s="243"/>
+      <c r="J40" s="243"/>
       <c r="K40" s="171"/>
       <c r="L40" s="171"/>
       <c r="M40" s="171"/>

</xml_diff>

<commit_message>
IMIOS Revisions with Consolidated Prep Module
</commit_message>
<xml_diff>
--- a/web/hca.xlsx
+++ b/web/hca.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="118">
   <si>
     <t>Num</t>
   </si>
@@ -482,6 +482,9 @@
   <si>
     <t># HEI registered in birth cohort  (Col a)</t>
   </si>
+  <si>
+    <t>Data Error Checks</t>
+  </si>
 </sst>
 </file>
 
@@ -492,7 +495,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="yyyy/mmm"/>
   </numFmts>
-  <fonts count="43">
+  <fonts count="46">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -763,6 +766,25 @@
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="19">
     <fill>
@@ -874,7 +896,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="76">
+  <borders count="96">
     <border>
       <left/>
       <right/>
@@ -1857,6 +1879,246 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="8"/>
+      </left>
+      <right style="medium">
+        <color theme="8"/>
+      </right>
+      <top style="medium">
+        <color theme="8"/>
+      </top>
+      <bottom style="medium">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="8"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="8"/>
+      </right>
+      <top style="medium">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="8"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="8"/>
+      </left>
+      <right style="medium">
+        <color theme="8"/>
+      </right>
+      <top style="medium">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="8"/>
+      </left>
+      <right style="medium">
+        <color theme="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="8"/>
+      </left>
+      <right style="medium">
+        <color theme="8"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="4"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="8"/>
+      </top>
+      <bottom style="medium">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="8"/>
+      </top>
+      <bottom style="medium">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="8"/>
+      </right>
+      <top style="medium">
+        <color theme="8"/>
+      </top>
+      <bottom style="medium">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1865,7 +2127,7 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="257">
+  <cellXfs count="287">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2154,9 +2416,6 @@
     <xf numFmtId="165" fontId="33" fillId="18" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="18" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2197,9 +2456,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2227,10 +2483,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2289,9 +2541,6 @@
     <xf numFmtId="165" fontId="33" fillId="17" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="33" fillId="17" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2341,9 +2590,6 @@
     <xf numFmtId="0" fontId="40" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="17" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="41" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2383,9 +2629,6 @@
     <xf numFmtId="0" fontId="37" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2438,8 +2681,65 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="72" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="14" fillId="17" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="14" fillId="17" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2477,68 +2777,59 @@
     <xf numFmtId="0" fontId="20" fillId="4" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="33" fillId="18" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="18" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="39" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="39" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="14" fillId="17" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="14" fillId="17" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2582,56 +2873,117 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="18" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="18" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="18" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="39" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="39" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="72" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="33" fillId="17" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="17" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="51" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="94" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="95" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2641,7 +2993,167 @@
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="43">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.59996337778862885"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.59996337778862885"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -2724,11 +3236,11 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="4" tint="0.59996337778862885"/>
+        <color theme="0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2794,6 +3306,16 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="4" tint="0.59996337778862885"/>
       </font>
       <fill>
@@ -2814,11 +3336,11 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="4" tint="0.59996337778862885"/>
+        <color theme="0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3216,7 +3738,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
+      <xdr:colOff>952501</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>537883</xdr:rowOff>
     </xdr:to>
@@ -3263,7 +3785,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>69409</xdr:colOff>
+      <xdr:colOff>170613</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>424465</xdr:rowOff>
     </xdr:to>
@@ -3613,111 +4135,111 @@
       <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="89.42578125" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="155.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.59765625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="89.3984375" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.59765625" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="155.1328125" style="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="164" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.73046875" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.265625" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.3984375" style="17" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.73046875" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.265625" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.3984375" style="15" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.73046875" style="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.265625" style="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.3984375" style="15" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18" style="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.85546875" style="15"/>
+    <col min="18" max="16384" width="8.86328125" style="15"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:17" s="1" customFormat="1">
-      <c r="A2" s="208"/>
-      <c r="B2" s="208"/>
-      <c r="C2" s="208"/>
-      <c r="D2" s="208"/>
-      <c r="E2" s="208"/>
-      <c r="F2" s="208"/>
-      <c r="G2" s="208"/>
-      <c r="H2" s="208"/>
-      <c r="I2" s="208"/>
+      <c r="A2" s="186"/>
+      <c r="B2" s="186"/>
+      <c r="C2" s="186"/>
+      <c r="D2" s="186"/>
+      <c r="E2" s="186"/>
+      <c r="F2" s="186"/>
+      <c r="G2" s="186"/>
+      <c r="H2" s="186"/>
+      <c r="I2" s="186"/>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1">
-      <c r="A3" s="208"/>
-      <c r="B3" s="208"/>
-      <c r="C3" s="208"/>
-      <c r="D3" s="208"/>
-      <c r="E3" s="208"/>
-      <c r="F3" s="208"/>
-      <c r="G3" s="208"/>
-      <c r="H3" s="208"/>
-      <c r="I3" s="208"/>
+      <c r="A3" s="186"/>
+      <c r="B3" s="186"/>
+      <c r="C3" s="186"/>
+      <c r="D3" s="186"/>
+      <c r="E3" s="186"/>
+      <c r="F3" s="186"/>
+      <c r="G3" s="186"/>
+      <c r="H3" s="186"/>
+      <c r="I3" s="186"/>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1">
-      <c r="A4" s="208"/>
-      <c r="B4" s="208"/>
-      <c r="C4" s="208"/>
-      <c r="D4" s="208"/>
-      <c r="E4" s="208"/>
-      <c r="F4" s="208"/>
-      <c r="G4" s="208"/>
-      <c r="H4" s="208"/>
-      <c r="I4" s="208"/>
-    </row>
-    <row r="6" spans="1:17" ht="26.25">
-      <c r="A6" s="215" t="s">
+      <c r="A4" s="186"/>
+      <c r="B4" s="186"/>
+      <c r="C4" s="186"/>
+      <c r="D4" s="186"/>
+      <c r="E4" s="186"/>
+      <c r="F4" s="186"/>
+      <c r="G4" s="186"/>
+      <c r="H4" s="186"/>
+      <c r="I4" s="186"/>
+    </row>
+    <row r="6" spans="1:17" ht="25.15">
+      <c r="A6" s="195" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="215"/>
-      <c r="C6" s="215"/>
-      <c r="D6" s="215"/>
-      <c r="E6" s="215"/>
-      <c r="F6" s="215"/>
-      <c r="G6" s="215"/>
-      <c r="H6" s="215"/>
-      <c r="I6" s="215"/>
-      <c r="J6" s="215"/>
-      <c r="K6" s="215"/>
-      <c r="L6" s="215"/>
-      <c r="M6" s="215"/>
-      <c r="N6" s="215"/>
-      <c r="O6" s="215"/>
-      <c r="P6" s="215"/>
-      <c r="Q6" s="215"/>
-    </row>
-    <row r="7" spans="1:17" ht="15.75" thickBot="1"/>
+      <c r="B6" s="195"/>
+      <c r="C6" s="195"/>
+      <c r="D6" s="195"/>
+      <c r="E6" s="195"/>
+      <c r="F6" s="195"/>
+      <c r="G6" s="195"/>
+      <c r="H6" s="195"/>
+      <c r="I6" s="195"/>
+      <c r="J6" s="195"/>
+      <c r="K6" s="195"/>
+      <c r="L6" s="195"/>
+      <c r="M6" s="195"/>
+      <c r="N6" s="195"/>
+      <c r="O6" s="195"/>
+      <c r="P6" s="195"/>
+      <c r="Q6" s="195"/>
+    </row>
+    <row r="7" spans="1:17" ht="15.4" thickBot="1"/>
     <row r="8" spans="1:17" s="18" customFormat="1" ht="25.15" customHeight="1" thickTop="1">
       <c r="A8" s="25"/>
-      <c r="B8" s="216" t="s">
+      <c r="B8" s="196" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="216"/>
-      <c r="D8" s="216"/>
-      <c r="E8" s="216"/>
-      <c r="F8" s="217" t="s">
+      <c r="C8" s="196"/>
+      <c r="D8" s="196"/>
+      <c r="E8" s="196"/>
+      <c r="F8" s="197" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="217"/>
-      <c r="H8" s="217"/>
-      <c r="I8" s="217"/>
-      <c r="J8" s="217" t="s">
+      <c r="G8" s="197"/>
+      <c r="H8" s="197"/>
+      <c r="I8" s="197"/>
+      <c r="J8" s="197" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="217"/>
-      <c r="L8" s="217"/>
-      <c r="M8" s="217"/>
-      <c r="N8" s="217" t="s">
+      <c r="K8" s="197"/>
+      <c r="L8" s="197"/>
+      <c r="M8" s="197"/>
+      <c r="N8" s="197" t="s">
         <v>33</v>
       </c>
-      <c r="O8" s="217"/>
-      <c r="P8" s="217"/>
-      <c r="Q8" s="225"/>
-    </row>
-    <row r="9" spans="1:17" s="24" customFormat="1" ht="15.75">
+      <c r="O8" s="197"/>
+      <c r="P8" s="197"/>
+      <c r="Q8" s="205"/>
+    </row>
+    <row r="9" spans="1:17" s="24" customFormat="1">
       <c r="A9" s="19" t="s">
         <v>17</v>
       </c>
@@ -3771,31 +4293,31 @@
       </c>
     </row>
     <row r="10" spans="1:17" s="32" customFormat="1" ht="58.15" customHeight="1">
-      <c r="A10" s="218" t="s">
+      <c r="A10" s="198" t="s">
         <v>89</v>
       </c>
-      <c r="B10" s="219"/>
-      <c r="C10" s="219"/>
-      <c r="D10" s="219"/>
-      <c r="E10" s="219"/>
-      <c r="F10" s="220" t="s">
+      <c r="B10" s="199"/>
+      <c r="C10" s="199"/>
+      <c r="D10" s="199"/>
+      <c r="E10" s="199"/>
+      <c r="F10" s="200" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="220"/>
-      <c r="H10" s="220"/>
-      <c r="I10" s="220"/>
-      <c r="J10" s="220" t="s">
+      <c r="G10" s="200"/>
+      <c r="H10" s="200"/>
+      <c r="I10" s="200"/>
+      <c r="J10" s="200" t="s">
         <v>39</v>
       </c>
-      <c r="K10" s="220"/>
-      <c r="L10" s="220"/>
-      <c r="M10" s="220"/>
-      <c r="N10" s="220" t="s">
+      <c r="K10" s="200"/>
+      <c r="L10" s="200"/>
+      <c r="M10" s="200"/>
+      <c r="N10" s="200" t="s">
         <v>40</v>
       </c>
-      <c r="O10" s="220"/>
-      <c r="P10" s="220"/>
-      <c r="Q10" s="221"/>
+      <c r="O10" s="200"/>
+      <c r="P10" s="200"/>
+      <c r="Q10" s="201"/>
     </row>
     <row r="11" spans="1:17" s="38" customFormat="1" ht="43.9" customHeight="1">
       <c r="A11" s="34">
@@ -3959,7 +4481,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="38" customFormat="1" ht="36">
+    <row r="15" spans="1:17" s="38" customFormat="1" ht="34.5">
       <c r="A15" s="34">
         <v>5</v>
       </c>
@@ -3998,7 +4520,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="38" customFormat="1" ht="36">
+    <row r="16" spans="1:17" s="38" customFormat="1" ht="17.25">
       <c r="A16" s="39">
         <v>6</v>
       </c>
@@ -4070,7 +4592,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="38" customFormat="1" ht="36">
+    <row r="18" spans="1:17" s="38" customFormat="1" ht="17.25">
       <c r="A18" s="39">
         <v>8</v>
       </c>
@@ -4103,7 +4625,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="38" customFormat="1" ht="36">
+    <row r="19" spans="1:17" s="38" customFormat="1" ht="17.25">
       <c r="A19" s="34">
         <v>9</v>
       </c>
@@ -4142,7 +4664,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="38" customFormat="1" ht="36">
+    <row r="20" spans="1:17" s="38" customFormat="1" ht="35.25">
       <c r="A20" s="34">
         <v>10</v>
       </c>
@@ -4181,7 +4703,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="33" customFormat="1" ht="20.25">
+    <row r="21" spans="1:17" s="33" customFormat="1" ht="20.65">
       <c r="A21" s="29">
         <v>11</v>
       </c>
@@ -4189,24 +4711,24 @@
         <v>48</v>
       </c>
       <c r="C21" s="31"/>
-      <c r="D21" s="193" t="s">
+      <c r="D21" s="206" t="s">
         <v>93</v>
       </c>
-      <c r="E21" s="194"/>
-      <c r="F21" s="194"/>
-      <c r="G21" s="194"/>
-      <c r="H21" s="194"/>
-      <c r="I21" s="194"/>
-      <c r="J21" s="194"/>
-      <c r="K21" s="194"/>
-      <c r="L21" s="194"/>
-      <c r="M21" s="194"/>
-      <c r="N21" s="194"/>
-      <c r="O21" s="194"/>
-      <c r="P21" s="194"/>
-      <c r="Q21" s="195"/>
-    </row>
-    <row r="22" spans="1:17" s="14" customFormat="1" ht="18">
+      <c r="E21" s="207"/>
+      <c r="F21" s="207"/>
+      <c r="G21" s="207"/>
+      <c r="H21" s="207"/>
+      <c r="I21" s="207"/>
+      <c r="J21" s="207"/>
+      <c r="K21" s="207"/>
+      <c r="L21" s="207"/>
+      <c r="M21" s="207"/>
+      <c r="N21" s="207"/>
+      <c r="O21" s="207"/>
+      <c r="P21" s="207"/>
+      <c r="Q21" s="208"/>
+    </row>
+    <row r="22" spans="1:17" s="14" customFormat="1" ht="17.25">
       <c r="A22" s="69">
         <v>11.1</v>
       </c>
@@ -4217,7 +4739,7 @@
       <c r="D22" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="205" t="s">
+      <c r="E22" s="187" t="s">
         <v>56</v>
       </c>
       <c r="F22" s="35"/>
@@ -4245,7 +4767,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="14" customFormat="1" ht="18">
+    <row r="23" spans="1:17" s="14" customFormat="1" ht="17.25">
       <c r="A23" s="69">
         <v>11.2</v>
       </c>
@@ -4256,7 +4778,7 @@
       <c r="D23" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="206"/>
+      <c r="E23" s="218"/>
       <c r="F23" s="40" t="s">
         <v>44</v>
       </c>
@@ -4288,7 +4810,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="14" customFormat="1" ht="18">
+    <row r="24" spans="1:17" s="14" customFormat="1" ht="17.25">
       <c r="A24" s="69">
         <v>11.3</v>
       </c>
@@ -4299,7 +4821,7 @@
       <c r="D24" s="69" t="s">
         <v>82</v>
       </c>
-      <c r="E24" s="207"/>
+      <c r="E24" s="188"/>
       <c r="F24" s="35"/>
       <c r="G24" s="35" t="s">
         <v>41</v>
@@ -4325,7 +4847,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="14" customFormat="1" ht="36">
+    <row r="25" spans="1:17" s="14" customFormat="1" ht="17.25">
       <c r="A25" s="69">
         <v>11.4</v>
       </c>
@@ -4336,7 +4858,7 @@
       <c r="D25" s="69" t="s">
         <v>83</v>
       </c>
-      <c r="E25" s="205" t="s">
+      <c r="E25" s="187" t="s">
         <v>80</v>
       </c>
       <c r="F25" s="40"/>
@@ -4364,7 +4886,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="14" customFormat="1" ht="18.75" thickBot="1">
+    <row r="26" spans="1:17" s="14" customFormat="1" ht="17.649999999999999" thickBot="1">
       <c r="A26" s="69">
         <v>11.5</v>
       </c>
@@ -4375,7 +4897,7 @@
       <c r="D26" s="69" t="s">
         <v>84</v>
       </c>
-      <c r="E26" s="207"/>
+      <c r="E26" s="188"/>
       <c r="F26" s="45"/>
       <c r="G26" s="45" t="s">
         <v>41</v>
@@ -4401,51 +4923,51 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A27" s="222"/>
-      <c r="B27" s="223"/>
-      <c r="C27" s="223"/>
-      <c r="D27" s="223"/>
-      <c r="E27" s="223"/>
-      <c r="F27" s="223"/>
-      <c r="G27" s="223"/>
-      <c r="H27" s="223"/>
-      <c r="I27" s="223"/>
-      <c r="J27" s="223"/>
-      <c r="K27" s="223"/>
-      <c r="L27" s="223"/>
-      <c r="M27" s="223"/>
-      <c r="N27" s="223"/>
-      <c r="O27" s="223"/>
-      <c r="P27" s="223"/>
-      <c r="Q27" s="224"/>
+    <row r="27" spans="1:17" ht="15.75" thickTop="1" thickBot="1">
+      <c r="A27" s="202"/>
+      <c r="B27" s="203"/>
+      <c r="C27" s="203"/>
+      <c r="D27" s="203"/>
+      <c r="E27" s="203"/>
+      <c r="F27" s="203"/>
+      <c r="G27" s="203"/>
+      <c r="H27" s="203"/>
+      <c r="I27" s="203"/>
+      <c r="J27" s="203"/>
+      <c r="K27" s="203"/>
+      <c r="L27" s="203"/>
+      <c r="M27" s="203"/>
+      <c r="N27" s="203"/>
+      <c r="O27" s="203"/>
+      <c r="P27" s="203"/>
+      <c r="Q27" s="204"/>
     </row>
     <row r="28" spans="1:17" s="32" customFormat="1" ht="21" thickTop="1">
-      <c r="A28" s="212" t="s">
+      <c r="A28" s="192" t="s">
         <v>90</v>
       </c>
-      <c r="B28" s="213"/>
-      <c r="C28" s="213"/>
-      <c r="D28" s="213"/>
-      <c r="E28" s="214"/>
-      <c r="F28" s="202" t="s">
+      <c r="B28" s="193"/>
+      <c r="C28" s="193"/>
+      <c r="D28" s="193"/>
+      <c r="E28" s="194"/>
+      <c r="F28" s="215" t="s">
         <v>45</v>
       </c>
-      <c r="G28" s="203"/>
-      <c r="H28" s="203"/>
-      <c r="I28" s="204"/>
-      <c r="J28" s="199" t="s">
+      <c r="G28" s="216"/>
+      <c r="H28" s="216"/>
+      <c r="I28" s="217"/>
+      <c r="J28" s="212" t="s">
         <v>45</v>
       </c>
-      <c r="K28" s="200"/>
-      <c r="L28" s="200"/>
-      <c r="M28" s="201"/>
-      <c r="N28" s="196" t="s">
+      <c r="K28" s="213"/>
+      <c r="L28" s="213"/>
+      <c r="M28" s="214"/>
+      <c r="N28" s="209" t="s">
         <v>45</v>
       </c>
-      <c r="O28" s="197"/>
-      <c r="P28" s="197"/>
-      <c r="Q28" s="198"/>
+      <c r="O28" s="210"/>
+      <c r="P28" s="210"/>
+      <c r="Q28" s="211"/>
     </row>
     <row r="29" spans="1:17" s="38" customFormat="1" ht="55.5" customHeight="1">
       <c r="A29" s="69">
@@ -4630,7 +5152,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="13" customFormat="1" ht="20.25">
+    <row r="34" spans="1:17" s="13" customFormat="1" ht="20.65">
       <c r="A34" s="29">
         <v>17</v>
       </c>
@@ -4638,22 +5160,22 @@
         <v>23</v>
       </c>
       <c r="C34" s="31"/>
-      <c r="D34" s="193" t="s">
+      <c r="D34" s="206" t="s">
         <v>93</v>
       </c>
-      <c r="E34" s="194"/>
-      <c r="F34" s="194"/>
-      <c r="G34" s="194"/>
-      <c r="H34" s="194"/>
-      <c r="I34" s="194"/>
-      <c r="J34" s="194"/>
-      <c r="K34" s="194"/>
-      <c r="L34" s="194"/>
-      <c r="M34" s="194"/>
-      <c r="N34" s="194"/>
-      <c r="O34" s="194"/>
-      <c r="P34" s="194"/>
-      <c r="Q34" s="195"/>
+      <c r="E34" s="207"/>
+      <c r="F34" s="207"/>
+      <c r="G34" s="207"/>
+      <c r="H34" s="207"/>
+      <c r="I34" s="207"/>
+      <c r="J34" s="207"/>
+      <c r="K34" s="207"/>
+      <c r="L34" s="207"/>
+      <c r="M34" s="207"/>
+      <c r="N34" s="207"/>
+      <c r="O34" s="207"/>
+      <c r="P34" s="207"/>
+      <c r="Q34" s="208"/>
     </row>
     <row r="35" spans="1:17" s="14" customFormat="1" ht="41.65" customHeight="1">
       <c r="A35" s="69">
@@ -4666,7 +5188,7 @@
       <c r="D35" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="209" t="s">
+      <c r="E35" s="189" t="s">
         <v>116</v>
       </c>
       <c r="F35" s="59"/>
@@ -4705,7 +5227,7 @@
       <c r="D36" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="E36" s="210"/>
+      <c r="E36" s="190"/>
       <c r="F36" s="61"/>
       <c r="G36" s="40" t="s">
         <v>77</v>
@@ -4742,7 +5264,7 @@
       <c r="D37" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="211"/>
+      <c r="E37" s="191"/>
       <c r="F37" s="59" t="s">
         <v>47</v>
       </c>
@@ -4785,7 +5307,7 @@
       <c r="D38" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="E38" s="209" t="s">
+      <c r="E38" s="189" t="s">
         <v>79</v>
       </c>
       <c r="F38" s="61"/>
@@ -4824,7 +5346,7 @@
       <c r="D39" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="E39" s="210"/>
+      <c r="E39" s="190"/>
       <c r="F39" s="59"/>
       <c r="G39" s="35" t="s">
         <v>77</v>
@@ -4861,7 +5383,7 @@
       <c r="D40" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="E40" s="211"/>
+      <c r="E40" s="191"/>
       <c r="F40" s="63"/>
       <c r="G40" s="64" t="s">
         <v>77</v>
@@ -4887,9 +5409,14 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="15.75" thickTop="1"/>
+    <row r="41" spans="1:17" ht="15.4" thickTop="1"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D34:Q34"/>
+    <mergeCell ref="N28:Q28"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="F28:I28"/>
+    <mergeCell ref="E22:E24"/>
     <mergeCell ref="A2:I4"/>
     <mergeCell ref="E25:E26"/>
     <mergeCell ref="E35:E37"/>
@@ -4906,11 +5433,6 @@
     <mergeCell ref="A27:Q27"/>
     <mergeCell ref="N8:Q8"/>
     <mergeCell ref="D21:Q21"/>
-    <mergeCell ref="D34:Q34"/>
-    <mergeCell ref="N28:Q28"/>
-    <mergeCell ref="J28:M28"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="E22:E24"/>
   </mergeCells>
   <pageMargins left="0.37037037037037002" right="0.51136363636363602" top="0.43154761904761901" bottom="0.64583333333333304" header="0.5" footer="0.5"/>
   <pageSetup paperSize="256" scale="74" fitToHeight="0" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -4936,27 +5458,28 @@
       <pane xSplit="3" ySplit="7" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="12.5703125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="129.28515625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="72" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="71" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.5703125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="37.140625" style="1" customWidth="1"/>
-    <col min="12" max="15" width="9.140625" style="1"/>
-    <col min="16" max="16" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="5.53125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.59765625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="129.265625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="17.86328125" style="72" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" style="71" customWidth="1"/>
+    <col min="6" max="6" width="12" style="257" customWidth="1"/>
+    <col min="7" max="7" width="5.59765625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.1328125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="2.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="77.265625" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="39.9296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="9.1328125" style="1"/>
+    <col min="16" max="16" width="15.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.73046875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="15.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:23" s="75" customFormat="1" ht="34.35" hidden="1" customHeight="1" thickBot="1">
@@ -4972,7 +5495,7 @@
       <c r="E1" s="87" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="86" t="s">
+      <c r="F1" s="250" t="s">
         <v>101</v>
       </c>
       <c r="G1" s="87" t="s">
@@ -4985,12 +5508,12 @@
         <v>2020</v>
       </c>
       <c r="J1" s="88"/>
-      <c r="K1" s="226" t="s">
+      <c r="K1" s="236" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="227"/>
-      <c r="M1" s="227"/>
-      <c r="N1" s="228"/>
+      <c r="L1" s="237"/>
+      <c r="M1" s="237"/>
+      <c r="N1" s="238"/>
       <c r="O1" s="89"/>
       <c r="P1" s="90">
         <f>DATE(I1,G1,"01")</f>
@@ -5013,25 +5536,25 @@
       <c r="W1" s="74"/>
     </row>
     <row r="2" spans="2:23" s="77" customFormat="1" ht="34.35" hidden="1" customHeight="1" thickBot="1">
-      <c r="B2" s="235" t="s">
+      <c r="B2" s="245" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="236"/>
-      <c r="D2" s="236"/>
-      <c r="E2" s="236"/>
-      <c r="F2" s="236"/>
-      <c r="G2" s="236"/>
-      <c r="H2" s="236"/>
-      <c r="I2" s="236"/>
-      <c r="J2" s="236"/>
-      <c r="K2" s="236"/>
-      <c r="L2" s="236"/>
-      <c r="M2" s="236"/>
-      <c r="N2" s="236"/>
-      <c r="O2" s="236"/>
-      <c r="P2" s="236"/>
-      <c r="Q2" s="236"/>
-      <c r="R2" s="237"/>
+      <c r="C2" s="246"/>
+      <c r="D2" s="246"/>
+      <c r="E2" s="246"/>
+      <c r="F2" s="246"/>
+      <c r="G2" s="246"/>
+      <c r="H2" s="246"/>
+      <c r="I2" s="246"/>
+      <c r="J2" s="246"/>
+      <c r="K2" s="246"/>
+      <c r="L2" s="246"/>
+      <c r="M2" s="246"/>
+      <c r="N2" s="246"/>
+      <c r="O2" s="246"/>
+      <c r="P2" s="246"/>
+      <c r="Q2" s="246"/>
+      <c r="R2" s="247"/>
       <c r="S2" s="76"/>
       <c r="V2" s="73">
         <v>1</v>
@@ -5039,15 +5562,18 @@
       <c r="W2" s="78"/>
     </row>
     <row r="3" spans="2:23" s="77" customFormat="1" ht="48" customHeight="1" thickBot="1">
-      <c r="B3" s="176"/>
-      <c r="C3" s="177"/>
-      <c r="D3" s="177"/>
-      <c r="E3" s="177"/>
-      <c r="F3" s="178"/>
+      <c r="B3" s="170"/>
+      <c r="C3" s="171"/>
+      <c r="D3" s="171"/>
+      <c r="E3" s="171"/>
+      <c r="F3" s="172"/>
       <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
+      <c r="H3" s="258" t="str">
+        <f>IF(LEN(L8&amp;L26)&lt;1,"","Form Has Data Errors, Please correct before submitting or uploading")</f>
+        <v/>
+      </c>
+      <c r="I3" s="259"/>
+      <c r="J3" s="260"/>
       <c r="K3" s="92"/>
       <c r="L3" s="92"/>
       <c r="M3" s="92"/>
@@ -5061,18 +5587,18 @@
       <c r="W3" s="78"/>
     </row>
     <row r="4" spans="2:23" s="77" customFormat="1" ht="24" customHeight="1" thickBot="1">
-      <c r="B4" s="232" t="str">
+      <c r="B4" s="242" t="str">
         <f>B1&amp;" : "&amp;C1&amp;"                                                           MFLCode : "&amp;E1&amp;"                                                    Reporting Month :   "&amp;G1&amp;"                                             Reporting Year: "&amp;I1</f>
         <v>Health Facility : Likii Dispensary                                                           MFLCode : 15035                                                    Reporting Month :   02                                             Reporting Year: 2020</v>
       </c>
-      <c r="C4" s="233"/>
-      <c r="D4" s="233"/>
-      <c r="E4" s="233"/>
-      <c r="F4" s="234"/>
+      <c r="C4" s="243"/>
+      <c r="D4" s="243"/>
+      <c r="E4" s="243"/>
+      <c r="F4" s="244"/>
       <c r="G4" s="93"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="94"/>
-      <c r="J4" s="94"/>
+      <c r="H4" s="261"/>
+      <c r="I4" s="262"/>
+      <c r="J4" s="263"/>
       <c r="K4" s="94"/>
       <c r="L4" s="94"/>
       <c r="M4" s="94"/>
@@ -5094,19 +5620,19 @@
       <c r="W4" s="78"/>
     </row>
     <row r="5" spans="2:23" s="81" customFormat="1" ht="30.75" customHeight="1" thickBot="1">
-      <c r="B5" s="238" t="s">
+      <c r="B5" s="248" t="s">
         <v>110</v>
       </c>
-      <c r="C5" s="239"/>
-      <c r="D5" s="229" t="s">
+      <c r="C5" s="249"/>
+      <c r="D5" s="239" t="s">
         <v>111</v>
       </c>
-      <c r="E5" s="230"/>
-      <c r="F5" s="231"/>
+      <c r="E5" s="240"/>
+      <c r="F5" s="241"/>
       <c r="G5" s="97"/>
-      <c r="H5" s="97"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="97"/>
+      <c r="H5" s="264"/>
+      <c r="I5" s="265"/>
+      <c r="J5" s="266"/>
       <c r="K5" s="97"/>
       <c r="L5" s="97"/>
       <c r="M5" s="97"/>
@@ -5124,10 +5650,10 @@
       <c r="W5" s="80"/>
     </row>
     <row r="6" spans="2:23" s="2" customFormat="1" ht="27.75" customHeight="1" thickBot="1">
-      <c r="B6" s="244" t="s">
+      <c r="B6" s="223" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="245"/>
+      <c r="C6" s="224"/>
       <c r="D6" s="98" t="s">
         <v>115</v>
       </c>
@@ -5135,1098 +5661,1120 @@
         <f>Q1</f>
         <v>43497</v>
       </c>
-      <c r="F6" s="100"/>
-      <c r="G6" s="248"/>
-      <c r="H6" s="240" t="s">
+      <c r="F6" s="251"/>
+      <c r="G6" s="227"/>
+      <c r="H6" s="275" t="s">
         <v>86</v>
       </c>
-      <c r="I6" s="241"/>
-      <c r="J6" s="242"/>
-      <c r="K6" s="101"/>
-      <c r="L6" s="101"/>
-      <c r="M6" s="101"/>
-      <c r="N6" s="101"/>
-      <c r="O6" s="101"/>
-      <c r="P6" s="101"/>
-      <c r="Q6" s="101"/>
-      <c r="R6" s="101"/>
-    </row>
-    <row r="7" spans="2:23" s="70" customFormat="1" ht="19.5" customHeight="1">
-      <c r="B7" s="102" t="s">
+      <c r="I6" s="276"/>
+      <c r="J6" s="277"/>
+      <c r="K6" s="100"/>
+      <c r="L6" s="100"/>
+      <c r="M6" s="100"/>
+      <c r="N6" s="100"/>
+      <c r="O6" s="100"/>
+      <c r="P6" s="100"/>
+      <c r="Q6" s="100"/>
+      <c r="R6" s="100"/>
+    </row>
+    <row r="7" spans="2:23" s="70" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
+      <c r="B7" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="103" t="s">
+      <c r="C7" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="104" t="s">
+      <c r="D7" s="103" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="105" t="s">
+      <c r="E7" s="104" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="106" t="s">
+      <c r="F7" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="248"/>
-      <c r="H7" s="107" t="s">
+      <c r="G7" s="227"/>
+      <c r="H7" s="282" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="108" t="s">
+      <c r="I7" s="283" t="s">
         <v>1</v>
       </c>
-      <c r="J7" s="109" t="s">
+      <c r="J7" s="281" t="s">
         <v>2</v>
       </c>
-      <c r="K7" s="110"/>
-      <c r="L7" s="110"/>
-      <c r="M7" s="110"/>
-      <c r="N7" s="110"/>
-      <c r="O7" s="110"/>
-      <c r="P7" s="110"/>
-      <c r="Q7" s="110"/>
-      <c r="R7" s="110"/>
+      <c r="K7" s="109"/>
+      <c r="L7" s="274" t="s">
+        <v>117</v>
+      </c>
+      <c r="M7" s="109"/>
+      <c r="N7" s="109"/>
+      <c r="O7" s="109"/>
+      <c r="P7" s="109"/>
+      <c r="Q7" s="109"/>
+      <c r="R7" s="109"/>
     </row>
     <row r="8" spans="2:23" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B8" s="111">
+      <c r="B8" s="110">
         <v>1</v>
       </c>
-      <c r="C8" s="112" t="s">
+      <c r="C8" s="111" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="113"/>
-      <c r="E8" s="113"/>
-      <c r="F8" s="114">
+      <c r="D8" s="112"/>
+      <c r="E8" s="112"/>
+      <c r="F8" s="252">
         <f>IFERROR(D8/E8,)</f>
         <v>0</v>
       </c>
-      <c r="G8" s="248"/>
-      <c r="H8" s="115"/>
-      <c r="I8" s="116" t="s">
+      <c r="G8" s="227"/>
+      <c r="H8" s="278"/>
+      <c r="I8" s="279" t="s">
         <v>41</v>
       </c>
-      <c r="J8" s="117"/>
-      <c r="K8" s="118" t="str">
-        <f>IF(D8&gt;E8,"Numerator Cannot be more than Denominator","")</f>
+      <c r="J8" s="280"/>
+      <c r="K8" s="116" t="str">
+        <f>IF(D8&gt;E8,"*Numerator for "&amp;C8&amp;" Cannot be more than Denominator"&amp;CHAR(10),"")</f>
         <v/>
       </c>
-      <c r="L8" s="118"/>
-      <c r="M8" s="118"/>
-      <c r="N8" s="118"/>
-      <c r="O8" s="118"/>
-      <c r="P8" s="118"/>
-      <c r="Q8" s="118"/>
-      <c r="R8" s="118"/>
+      <c r="L8" s="268" t="str">
+        <f>CONCATENATE(K8,K9,K10,K11,K12,K13,K14,K15,K16,K17,K18,K19,K20,K21,K22,K23,K24)</f>
+        <v/>
+      </c>
+      <c r="M8" s="116"/>
+      <c r="N8" s="116"/>
+      <c r="O8" s="116"/>
+      <c r="P8" s="116"/>
+      <c r="Q8" s="116"/>
+      <c r="R8" s="116"/>
     </row>
     <row r="9" spans="2:23" s="4" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B9" s="111">
+      <c r="B9" s="110">
         <v>2</v>
       </c>
-      <c r="C9" s="112" t="s">
+      <c r="C9" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="181"/>
-      <c r="E9" s="119">
+      <c r="D9" s="175"/>
+      <c r="E9" s="185">
         <f>E8</f>
         <v>0</v>
       </c>
-      <c r="F9" s="114">
+      <c r="F9" s="252">
         <f t="shared" ref="F9:F23" si="0">IFERROR(D9/E9,)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="248"/>
-      <c r="H9" s="115"/>
-      <c r="I9" s="116" t="s">
+      <c r="G9" s="227"/>
+      <c r="H9" s="113"/>
+      <c r="I9" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="J9" s="117"/>
-      <c r="K9" s="118" t="str">
-        <f t="shared" ref="K9:K23" si="1">IF(D9&gt;E9,"Numerator Cannot be more than Denominator","")</f>
+      <c r="J9" s="115"/>
+      <c r="K9" s="116" t="str">
+        <f t="shared" ref="K9:K23" si="1">IF(D9&gt;E9,"*Numerator for "&amp;C9&amp;" Cannot be more than Denominator"&amp;CHAR(10),"")</f>
         <v/>
       </c>
-      <c r="L9" s="120"/>
-      <c r="M9" s="120"/>
-      <c r="N9" s="120"/>
-      <c r="O9" s="120"/>
-      <c r="P9" s="120"/>
-      <c r="Q9" s="120"/>
-      <c r="R9" s="120"/>
+      <c r="L9" s="269"/>
+      <c r="M9" s="118"/>
+      <c r="N9" s="118"/>
+      <c r="O9" s="118"/>
+      <c r="P9" s="118"/>
+      <c r="Q9" s="118"/>
+      <c r="R9" s="118"/>
     </row>
     <row r="10" spans="2:23" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B10" s="111">
+      <c r="B10" s="110">
         <v>3</v>
       </c>
-      <c r="C10" s="179" t="s">
+      <c r="C10" s="173" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="182"/>
-      <c r="E10" s="180">
+      <c r="D10" s="284"/>
+      <c r="E10" s="286">
         <f>E8</f>
         <v>0</v>
       </c>
-      <c r="F10" s="114">
+      <c r="F10" s="285">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G10" s="248"/>
-      <c r="H10" s="121" t="s">
+      <c r="G10" s="227"/>
+      <c r="H10" s="119" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="116" t="s">
+      <c r="I10" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="J10" s="117"/>
-      <c r="K10" s="118" t="str">
+      <c r="J10" s="115"/>
+      <c r="K10" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="L10" s="118"/>
-      <c r="M10" s="118"/>
-      <c r="N10" s="118"/>
-      <c r="O10" s="118"/>
-      <c r="P10" s="118"/>
-      <c r="Q10" s="118"/>
-      <c r="R10" s="118"/>
+      <c r="L10" s="269"/>
+      <c r="M10" s="116"/>
+      <c r="N10" s="116"/>
+      <c r="O10" s="116"/>
+      <c r="P10" s="116"/>
+      <c r="Q10" s="116"/>
+      <c r="R10" s="116"/>
     </row>
     <row r="11" spans="2:23" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B11" s="111">
+      <c r="B11" s="110">
         <v>4</v>
       </c>
-      <c r="C11" s="112" t="s">
+      <c r="C11" s="111" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="151"/>
-      <c r="E11" s="119">
+      <c r="D11" s="147"/>
+      <c r="E11" s="182">
         <f>D10</f>
         <v>0</v>
       </c>
-      <c r="F11" s="114">
+      <c r="F11" s="252">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G11" s="248"/>
-      <c r="H11" s="115"/>
-      <c r="I11" s="122" t="s">
+      <c r="G11" s="227"/>
+      <c r="H11" s="113"/>
+      <c r="I11" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="J11" s="117"/>
-      <c r="K11" s="118" t="str">
+      <c r="J11" s="115"/>
+      <c r="K11" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="L11" s="118"/>
-      <c r="M11" s="118"/>
-      <c r="N11" s="118"/>
-      <c r="O11" s="118"/>
-      <c r="P11" s="118"/>
-      <c r="Q11" s="118"/>
-      <c r="R11" s="118"/>
+      <c r="L11" s="269"/>
+      <c r="M11" s="116"/>
+      <c r="N11" s="116"/>
+      <c r="O11" s="116"/>
+      <c r="P11" s="116"/>
+      <c r="Q11" s="116"/>
+      <c r="R11" s="116"/>
     </row>
     <row r="12" spans="2:23" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B12" s="111">
+      <c r="B12" s="110">
         <v>5</v>
       </c>
-      <c r="C12" s="123" t="s">
+      <c r="C12" s="121" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="124"/>
-      <c r="E12" s="119">
+      <c r="D12" s="112"/>
+      <c r="E12" s="117">
         <f>E8</f>
         <v>0</v>
       </c>
-      <c r="F12" s="114">
+      <c r="F12" s="252">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G12" s="248"/>
-      <c r="H12" s="125" t="s">
+      <c r="G12" s="227"/>
+      <c r="H12" s="122" t="s">
         <v>91</v>
       </c>
-      <c r="I12" s="116" t="s">
+      <c r="I12" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="J12" s="117"/>
-      <c r="K12" s="118" t="str">
+      <c r="J12" s="115"/>
+      <c r="K12" s="116" t="str">
+        <f>IF(D12&gt;E12,"*Numerator for HEI tested with First DNA PCR at 6-8wks or at First contact and results available between 0 and 12 months Cannot be more than Denominator"&amp;CHAR(10)&amp;CHAR(10),"")</f>
+        <v/>
+      </c>
+      <c r="L12" s="269"/>
+      <c r="M12" s="116"/>
+      <c r="N12" s="116"/>
+      <c r="O12" s="116"/>
+      <c r="P12" s="116"/>
+      <c r="Q12" s="116"/>
+      <c r="R12" s="116"/>
+    </row>
+    <row r="13" spans="2:23" s="3" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B13" s="110">
+        <v>6</v>
+      </c>
+      <c r="C13" s="111" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="175"/>
+      <c r="E13" s="112"/>
+      <c r="F13" s="252">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="227"/>
+      <c r="H13" s="123"/>
+      <c r="I13" s="124"/>
+      <c r="J13" s="115"/>
+      <c r="K13" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="L12" s="118"/>
-      <c r="M12" s="118"/>
-      <c r="N12" s="118"/>
-      <c r="O12" s="118"/>
-      <c r="P12" s="118"/>
-      <c r="Q12" s="118"/>
-      <c r="R12" s="118"/>
-    </row>
-    <row r="13" spans="2:23" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B13" s="111">
-        <v>6</v>
-      </c>
-      <c r="C13" s="112" t="s">
+      <c r="L13" s="269"/>
+      <c r="M13" s="116"/>
+      <c r="N13" s="116"/>
+      <c r="O13" s="116"/>
+      <c r="P13" s="116"/>
+      <c r="Q13" s="116"/>
+      <c r="R13" s="116"/>
+    </row>
+    <row r="14" spans="2:23" s="3" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B14" s="110">
         <v>7</v>
       </c>
-      <c r="D13" s="181"/>
-      <c r="E13" s="113"/>
-      <c r="F13" s="114">
+      <c r="C14" s="173" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="176"/>
+      <c r="E14" s="174">
+        <f>E8</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="252">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G13" s="248"/>
-      <c r="H13" s="126"/>
-      <c r="I13" s="127"/>
-      <c r="J13" s="117"/>
-      <c r="K13" s="118" t="str">
+      <c r="G14" s="227"/>
+      <c r="H14" s="125" t="s">
+        <v>44</v>
+      </c>
+      <c r="I14" s="114" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" s="115"/>
+      <c r="K14" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="L13" s="118"/>
-      <c r="M13" s="118"/>
-      <c r="N13" s="118"/>
-      <c r="O13" s="118"/>
-      <c r="P13" s="118"/>
-      <c r="Q13" s="118"/>
-      <c r="R13" s="118"/>
-    </row>
-    <row r="14" spans="2:23" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B14" s="111">
-        <v>7</v>
-      </c>
-      <c r="C14" s="179" t="s">
+      <c r="L14" s="269"/>
+      <c r="M14" s="116"/>
+      <c r="N14" s="116"/>
+      <c r="O14" s="116"/>
+      <c r="P14" s="116"/>
+      <c r="Q14" s="116"/>
+      <c r="R14" s="116"/>
+    </row>
+    <row r="15" spans="2:23" s="3" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B15" s="110">
         <v>8</v>
       </c>
-      <c r="D14" s="182"/>
-      <c r="E14" s="180">
+      <c r="C15" s="111" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="147"/>
+      <c r="E15" s="112"/>
+      <c r="F15" s="252">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="227"/>
+      <c r="H15" s="113"/>
+      <c r="I15" s="124"/>
+      <c r="J15" s="115"/>
+      <c r="K15" s="116" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L15" s="269"/>
+      <c r="M15" s="116"/>
+      <c r="N15" s="116"/>
+      <c r="O15" s="116"/>
+      <c r="P15" s="116"/>
+      <c r="Q15" s="116"/>
+      <c r="R15" s="116"/>
+    </row>
+    <row r="16" spans="2:23" s="3" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B16" s="110">
+        <v>9</v>
+      </c>
+      <c r="C16" s="111" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="112"/>
+      <c r="E16" s="117">
+        <f>D14</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="252">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="227"/>
+      <c r="H16" s="113"/>
+      <c r="I16" s="126" t="s">
+        <v>44</v>
+      </c>
+      <c r="J16" s="115"/>
+      <c r="K16" s="116" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L16" s="269"/>
+      <c r="M16" s="116"/>
+      <c r="N16" s="116"/>
+      <c r="O16" s="116"/>
+      <c r="P16" s="116"/>
+      <c r="Q16" s="116"/>
+      <c r="R16" s="116"/>
+    </row>
+    <row r="17" spans="2:18" s="3" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B17" s="110">
+        <v>10</v>
+      </c>
+      <c r="C17" s="111" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="112"/>
+      <c r="E17" s="117">
+        <f>D14</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="252">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="227"/>
+      <c r="H17" s="113"/>
+      <c r="I17" s="126" t="s">
+        <v>44</v>
+      </c>
+      <c r="J17" s="115"/>
+      <c r="K17" s="116" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="L17" s="269"/>
+      <c r="M17" s="116"/>
+      <c r="N17" s="116"/>
+      <c r="O17" s="116"/>
+      <c r="P17" s="116"/>
+      <c r="Q17" s="116"/>
+      <c r="R17" s="116"/>
+    </row>
+    <row r="18" spans="2:18" ht="18.75" customHeight="1">
+      <c r="B18" s="167">
+        <v>11</v>
+      </c>
+      <c r="C18" s="168" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="169"/>
+      <c r="E18" s="169"/>
+      <c r="F18" s="253"/>
+      <c r="G18" s="227"/>
+      <c r="H18" s="127"/>
+      <c r="I18" s="128"/>
+      <c r="J18" s="129"/>
+      <c r="K18" s="116" t="str">
+        <f>IF(D12&lt;E11,"*Numerator for "&amp;C12&amp;" Cannot be less than Denominator for "&amp;C11&amp;CHAR(10)&amp;CHAR(10),"")</f>
+        <v/>
+      </c>
+      <c r="L18" s="269"/>
+      <c r="M18" s="130"/>
+      <c r="N18" s="130"/>
+      <c r="O18" s="130"/>
+      <c r="P18" s="130"/>
+      <c r="Q18" s="130"/>
+      <c r="R18" s="130"/>
+    </row>
+    <row r="19" spans="2:18" s="3" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B19" s="110">
+        <v>11.1</v>
+      </c>
+      <c r="C19" s="111" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="112"/>
+      <c r="E19" s="117">
         <f>E8</f>
         <v>0</v>
       </c>
-      <c r="F14" s="114">
+      <c r="F19" s="252">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G14" s="248"/>
-      <c r="H14" s="128" t="s">
-        <v>44</v>
-      </c>
-      <c r="I14" s="116" t="s">
+      <c r="G19" s="227"/>
+      <c r="H19" s="113"/>
+      <c r="I19" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="J14" s="117"/>
-      <c r="K14" s="118" t="str">
+      <c r="J19" s="131"/>
+      <c r="K19" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="L14" s="118"/>
-      <c r="M14" s="118"/>
-      <c r="N14" s="118"/>
-      <c r="O14" s="118"/>
-      <c r="P14" s="118"/>
-      <c r="Q14" s="118"/>
-      <c r="R14" s="118"/>
-    </row>
-    <row r="15" spans="2:23" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B15" s="111">
-        <v>8</v>
-      </c>
-      <c r="C15" s="112" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="151"/>
-      <c r="E15" s="113"/>
-      <c r="F15" s="114">
+      <c r="L19" s="269"/>
+      <c r="M19" s="116"/>
+      <c r="N19" s="116"/>
+      <c r="O19" s="116"/>
+      <c r="P19" s="116"/>
+      <c r="Q19" s="116"/>
+      <c r="R19" s="116"/>
+    </row>
+    <row r="20" spans="2:18" s="3" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B20" s="110">
+        <v>11.2</v>
+      </c>
+      <c r="C20" s="111" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="117">
+        <f>D14</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="117">
+        <f>E8</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="252">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G15" s="248"/>
-      <c r="H15" s="115"/>
-      <c r="I15" s="127"/>
-      <c r="J15" s="117"/>
-      <c r="K15" s="118" t="str">
+      <c r="G20" s="227"/>
+      <c r="H20" s="125" t="s">
+        <v>44</v>
+      </c>
+      <c r="I20" s="114" t="s">
+        <v>41</v>
+      </c>
+      <c r="J20" s="131"/>
+      <c r="K20" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="L15" s="118"/>
-      <c r="M15" s="118"/>
-      <c r="N15" s="118"/>
-      <c r="O15" s="118"/>
-      <c r="P15" s="118"/>
-      <c r="Q15" s="118"/>
-      <c r="R15" s="118"/>
-    </row>
-    <row r="16" spans="2:23" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B16" s="111">
-        <v>9</v>
-      </c>
-      <c r="C16" s="112" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="113"/>
-      <c r="E16" s="119">
-        <f>D14</f>
+      <c r="L20" s="269"/>
+      <c r="M20" s="116"/>
+      <c r="N20" s="116"/>
+      <c r="O20" s="116"/>
+      <c r="P20" s="116"/>
+      <c r="Q20" s="116"/>
+      <c r="R20" s="116"/>
+    </row>
+    <row r="21" spans="2:18" s="3" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B21" s="110">
+        <v>11.3</v>
+      </c>
+      <c r="C21" s="111" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="112"/>
+      <c r="E21" s="117">
+        <f>E8</f>
         <v>0</v>
       </c>
-      <c r="F16" s="114">
+      <c r="F21" s="252">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G16" s="248"/>
-      <c r="H16" s="115"/>
-      <c r="I16" s="129" t="s">
-        <v>44</v>
-      </c>
-      <c r="J16" s="117"/>
-      <c r="K16" s="118" t="str">
+      <c r="G21" s="227"/>
+      <c r="H21" s="113"/>
+      <c r="I21" s="114" t="s">
+        <v>41</v>
+      </c>
+      <c r="J21" s="131"/>
+      <c r="K21" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="L16" s="118"/>
-      <c r="M16" s="118"/>
-      <c r="N16" s="118"/>
-      <c r="O16" s="118"/>
-      <c r="P16" s="118"/>
-      <c r="Q16" s="118"/>
-      <c r="R16" s="118"/>
-    </row>
-    <row r="17" spans="2:18" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B17" s="111">
-        <v>10</v>
-      </c>
-      <c r="C17" s="112" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="113"/>
-      <c r="E17" s="119">
-        <f>D14</f>
+      <c r="L21" s="269"/>
+      <c r="M21" s="116"/>
+      <c r="N21" s="116"/>
+      <c r="O21" s="116"/>
+      <c r="P21" s="116"/>
+      <c r="Q21" s="116"/>
+      <c r="R21" s="116"/>
+    </row>
+    <row r="22" spans="2:18" s="3" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B22" s="110">
+        <v>11.4</v>
+      </c>
+      <c r="C22" s="111" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="112"/>
+      <c r="E22" s="117">
+        <f>E8</f>
         <v>0</v>
       </c>
-      <c r="F17" s="114">
+      <c r="F22" s="252">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G17" s="248"/>
-      <c r="H17" s="115"/>
-      <c r="I17" s="129" t="s">
-        <v>44</v>
-      </c>
-      <c r="J17" s="117"/>
-      <c r="K17" s="118" t="str">
+      <c r="G22" s="227"/>
+      <c r="H22" s="113"/>
+      <c r="I22" s="114" t="s">
+        <v>41</v>
+      </c>
+      <c r="J22" s="131"/>
+      <c r="K22" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="L17" s="118"/>
-      <c r="M17" s="118"/>
-      <c r="N17" s="118"/>
-      <c r="O17" s="118"/>
-      <c r="P17" s="118"/>
-      <c r="Q17" s="118"/>
-      <c r="R17" s="118"/>
-    </row>
-    <row r="18" spans="2:18" ht="18.75" customHeight="1">
-      <c r="B18" s="172">
-        <v>11</v>
-      </c>
-      <c r="C18" s="173" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="174"/>
-      <c r="E18" s="174"/>
-      <c r="F18" s="175"/>
-      <c r="G18" s="248"/>
-      <c r="H18" s="130"/>
-      <c r="I18" s="131"/>
-      <c r="J18" s="132"/>
-      <c r="K18" s="133"/>
-      <c r="L18" s="133"/>
-      <c r="M18" s="133"/>
-      <c r="N18" s="133"/>
-      <c r="O18" s="133"/>
-      <c r="P18" s="133"/>
-      <c r="Q18" s="133"/>
-      <c r="R18" s="133"/>
-    </row>
-    <row r="19" spans="2:18" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B19" s="111">
-        <v>11.1</v>
-      </c>
-      <c r="C19" s="112" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="113"/>
-      <c r="E19" s="119">
+      <c r="L22" s="269"/>
+      <c r="M22" s="116"/>
+      <c r="N22" s="116"/>
+      <c r="O22" s="116"/>
+      <c r="P22" s="116"/>
+      <c r="Q22" s="116"/>
+      <c r="R22" s="116"/>
+    </row>
+    <row r="23" spans="2:18" s="3" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
+      <c r="B23" s="183">
+        <v>11.5</v>
+      </c>
+      <c r="C23" s="184" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="175"/>
+      <c r="E23" s="185">
         <f>E8</f>
         <v>0</v>
       </c>
-      <c r="F19" s="114">
+      <c r="F23" s="254">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G19" s="248"/>
-      <c r="H19" s="115"/>
-      <c r="I19" s="116" t="s">
+      <c r="G23" s="227"/>
+      <c r="H23" s="136"/>
+      <c r="I23" s="137" t="s">
         <v>41</v>
       </c>
-      <c r="J19" s="134"/>
-      <c r="K19" s="118" t="str">
+      <c r="J23" s="138"/>
+      <c r="K23" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="L19" s="118"/>
-      <c r="M19" s="118"/>
-      <c r="N19" s="118"/>
-      <c r="O19" s="118"/>
-      <c r="P19" s="118"/>
-      <c r="Q19" s="118"/>
-      <c r="R19" s="118"/>
-    </row>
-    <row r="20" spans="2:18" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B20" s="111">
-        <v>11.2</v>
-      </c>
-      <c r="C20" s="112" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" s="119">
-        <f>D14</f>
-        <v>0</v>
-      </c>
-      <c r="E20" s="119">
-        <f>E8</f>
-        <v>0</v>
-      </c>
-      <c r="F20" s="114">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="248"/>
-      <c r="H20" s="128" t="s">
-        <v>44</v>
-      </c>
-      <c r="I20" s="116" t="s">
-        <v>41</v>
-      </c>
-      <c r="J20" s="134"/>
-      <c r="K20" s="118" t="str">
-        <f t="shared" si="1"/>
+      <c r="L23" s="270"/>
+      <c r="M23" s="116"/>
+      <c r="N23" s="116"/>
+      <c r="O23" s="116"/>
+      <c r="P23" s="116"/>
+      <c r="Q23" s="116"/>
+      <c r="R23" s="116"/>
+    </row>
+    <row r="24" spans="2:18" ht="16.5" customHeight="1">
+      <c r="B24" s="228" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="229"/>
+      <c r="D24" s="229"/>
+      <c r="E24" s="229"/>
+      <c r="F24" s="230"/>
+      <c r="G24" s="227"/>
+      <c r="H24" s="234"/>
+      <c r="I24" s="234"/>
+      <c r="J24" s="234"/>
+      <c r="K24" s="130" t="str">
+        <f>IF(SUM(D19:D23)&lt;&gt;E19,"* Sum of Numerator  11.1,11.2,11.3,11.4 and 11.5 should be equal to Denominator for 11.1","")</f>
         <v/>
       </c>
-      <c r="L20" s="118"/>
-      <c r="M20" s="118"/>
-      <c r="N20" s="118"/>
-      <c r="O20" s="118"/>
-      <c r="P20" s="118"/>
-      <c r="Q20" s="118"/>
-      <c r="R20" s="118"/>
-    </row>
-    <row r="21" spans="2:18" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B21" s="111">
-        <v>11.3</v>
-      </c>
-      <c r="C21" s="112" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="113"/>
-      <c r="E21" s="119">
-        <f>E8</f>
-        <v>0</v>
-      </c>
-      <c r="F21" s="114">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="248"/>
-      <c r="H21" s="115"/>
-      <c r="I21" s="116" t="s">
-        <v>41</v>
-      </c>
-      <c r="J21" s="134"/>
-      <c r="K21" s="118" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L21" s="118"/>
-      <c r="M21" s="118"/>
-      <c r="N21" s="118"/>
-      <c r="O21" s="118"/>
-      <c r="P21" s="118"/>
-      <c r="Q21" s="118"/>
-      <c r="R21" s="118"/>
-    </row>
-    <row r="22" spans="2:18" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B22" s="111">
-        <v>11.4</v>
-      </c>
-      <c r="C22" s="112" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="113"/>
-      <c r="E22" s="119">
-        <f>E8</f>
-        <v>0</v>
-      </c>
-      <c r="F22" s="114">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="248"/>
-      <c r="H22" s="115"/>
-      <c r="I22" s="116" t="s">
-        <v>41</v>
-      </c>
-      <c r="J22" s="134"/>
-      <c r="K22" s="118" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L22" s="118"/>
-      <c r="M22" s="118"/>
-      <c r="N22" s="118"/>
-      <c r="O22" s="118"/>
-      <c r="P22" s="118"/>
-      <c r="Q22" s="118"/>
-      <c r="R22" s="118"/>
-    </row>
-    <row r="23" spans="2:18" s="3" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B23" s="189">
-        <v>11.5</v>
-      </c>
-      <c r="C23" s="190" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="181"/>
-      <c r="E23" s="191">
-        <f>E8</f>
-        <v>0</v>
-      </c>
-      <c r="F23" s="192">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="248"/>
-      <c r="H23" s="139"/>
-      <c r="I23" s="140" t="s">
-        <v>41</v>
-      </c>
-      <c r="J23" s="141"/>
-      <c r="K23" s="118" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="L23" s="118"/>
-      <c r="M23" s="118"/>
-      <c r="N23" s="118"/>
-      <c r="O23" s="118"/>
-      <c r="P23" s="118"/>
-      <c r="Q23" s="118"/>
-      <c r="R23" s="118"/>
-    </row>
-    <row r="24" spans="2:18" ht="16.5" customHeight="1">
-      <c r="B24" s="249" t="s">
-        <v>80</v>
-      </c>
-      <c r="C24" s="250"/>
-      <c r="D24" s="250"/>
-      <c r="E24" s="250"/>
-      <c r="F24" s="251"/>
-      <c r="G24" s="248"/>
-      <c r="H24" s="255"/>
-      <c r="I24" s="255"/>
-      <c r="J24" s="255"/>
-      <c r="K24" s="133"/>
-      <c r="L24" s="133"/>
-      <c r="M24" s="133"/>
-      <c r="N24" s="133"/>
-      <c r="O24" s="133"/>
-      <c r="P24" s="133"/>
-      <c r="Q24" s="133"/>
-      <c r="R24" s="133"/>
+      <c r="L24" s="130"/>
+      <c r="M24" s="130"/>
+      <c r="N24" s="130"/>
+      <c r="O24" s="130"/>
+      <c r="P24" s="130"/>
+      <c r="Q24" s="130"/>
+      <c r="R24" s="130"/>
     </row>
     <row r="25" spans="2:18" ht="9.75" customHeight="1" thickBot="1">
-      <c r="B25" s="252"/>
-      <c r="C25" s="253"/>
-      <c r="D25" s="253"/>
-      <c r="E25" s="253"/>
-      <c r="F25" s="254"/>
-      <c r="G25" s="248"/>
-      <c r="H25" s="255"/>
-      <c r="I25" s="255"/>
-      <c r="J25" s="255"/>
-      <c r="K25" s="133"/>
-      <c r="L25" s="133"/>
-      <c r="M25" s="133"/>
-      <c r="N25" s="133"/>
-      <c r="O25" s="133"/>
-      <c r="P25" s="133"/>
-      <c r="Q25" s="133"/>
-      <c r="R25" s="133"/>
+      <c r="B25" s="231"/>
+      <c r="C25" s="232"/>
+      <c r="D25" s="232"/>
+      <c r="E25" s="232"/>
+      <c r="F25" s="233"/>
+      <c r="G25" s="227"/>
+      <c r="H25" s="234"/>
+      <c r="I25" s="234"/>
+      <c r="J25" s="234"/>
+      <c r="K25" s="130"/>
+      <c r="L25" s="130"/>
+      <c r="M25" s="130"/>
+      <c r="N25" s="130"/>
+      <c r="O25" s="130"/>
+      <c r="P25" s="130"/>
+      <c r="Q25" s="130"/>
+      <c r="R25" s="130"/>
     </row>
     <row r="26" spans="2:18" s="5" customFormat="1" ht="32.25" customHeight="1" thickBot="1">
-      <c r="B26" s="246" t="s">
+      <c r="B26" s="225" t="s">
         <v>90</v>
       </c>
-      <c r="C26" s="247"/>
-      <c r="D26" s="142" t="s">
+      <c r="C26" s="226"/>
+      <c r="D26" s="139" t="s">
         <v>115</v>
       </c>
-      <c r="E26" s="143">
+      <c r="E26" s="140">
         <f>R1</f>
         <v>43132</v>
       </c>
-      <c r="F26" s="144"/>
-      <c r="G26" s="248"/>
-      <c r="H26" s="240" t="s">
+      <c r="F26" s="255"/>
+      <c r="G26" s="227"/>
+      <c r="H26" s="219" t="s">
         <v>86</v>
       </c>
-      <c r="I26" s="241"/>
-      <c r="J26" s="242"/>
-      <c r="K26" s="145"/>
-      <c r="L26" s="145"/>
-      <c r="M26" s="145"/>
-      <c r="N26" s="145"/>
-      <c r="O26" s="145"/>
-      <c r="P26" s="145"/>
-      <c r="Q26" s="145"/>
-      <c r="R26" s="145"/>
+      <c r="I26" s="220"/>
+      <c r="J26" s="221"/>
+      <c r="K26" s="141"/>
+      <c r="L26" s="271" t="str">
+        <f>CONCATENATE(K28,K29,K30,K31,K32,K33,K34,K35,K36,K37,K38,K39)</f>
+        <v/>
+      </c>
+      <c r="M26" s="141"/>
+      <c r="N26" s="141"/>
+      <c r="O26" s="141"/>
+      <c r="P26" s="141"/>
+      <c r="Q26" s="141"/>
+      <c r="R26" s="141"/>
     </row>
     <row r="27" spans="2:18" s="70" customFormat="1" ht="22.9" customHeight="1" thickBot="1">
-      <c r="B27" s="146" t="s">
+      <c r="B27" s="142" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="147" t="s">
+      <c r="C27" s="143" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="185" t="s">
+      <c r="D27" s="179" t="s">
         <v>19</v>
       </c>
-      <c r="E27" s="148" t="s">
+      <c r="E27" s="144" t="s">
         <v>20</v>
       </c>
-      <c r="F27" s="149" t="s">
+      <c r="F27" s="145" t="s">
         <v>2</v>
       </c>
-      <c r="G27" s="248"/>
-      <c r="H27" s="107" t="s">
+      <c r="G27" s="227"/>
+      <c r="H27" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="108" t="s">
+      <c r="I27" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="J27" s="109" t="s">
+      <c r="J27" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="K27" s="110"/>
-      <c r="L27" s="110"/>
-      <c r="M27" s="110"/>
-      <c r="N27" s="110"/>
-      <c r="O27" s="110"/>
-      <c r="P27" s="110"/>
-      <c r="Q27" s="110"/>
-      <c r="R27" s="110"/>
+      <c r="K27" s="109"/>
+      <c r="L27" s="272"/>
+      <c r="M27" s="109"/>
+      <c r="N27" s="109"/>
+      <c r="O27" s="109"/>
+      <c r="P27" s="109"/>
+      <c r="Q27" s="109"/>
+      <c r="R27" s="109"/>
     </row>
     <row r="28" spans="2:18" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B28" s="150">
+      <c r="B28" s="146">
         <v>12</v>
       </c>
-      <c r="C28" s="183" t="s">
+      <c r="C28" s="177" t="s">
         <v>92</v>
       </c>
-      <c r="D28" s="182"/>
-      <c r="E28" s="184"/>
-      <c r="F28" s="114">
+      <c r="D28" s="176"/>
+      <c r="E28" s="178"/>
+      <c r="F28" s="252">
         <f t="shared" ref="F28:F39" si="2">IFERROR(D28/E28,)</f>
         <v>0</v>
       </c>
-      <c r="G28" s="248"/>
-      <c r="H28" s="115" t="s">
+      <c r="G28" s="227"/>
+      <c r="H28" s="113" t="s">
         <v>46</v>
       </c>
-      <c r="I28" s="152"/>
-      <c r="J28" s="134"/>
-      <c r="K28" s="118" t="str">
-        <f t="shared" ref="K28:K39" si="3">IF(D28&gt;E28,"Numerator Cannot be more than Denominator","")</f>
+      <c r="I28" s="148"/>
+      <c r="J28" s="131"/>
+      <c r="K28" s="116" t="str">
+        <f>IF(D28&gt;E28,"*Numerator for "&amp;C28&amp;" Cannot be more than Denominator"&amp;CHAR(10),"")</f>
         <v/>
       </c>
-      <c r="L28" s="153"/>
-      <c r="M28" s="153"/>
-      <c r="N28" s="153"/>
-      <c r="O28" s="153"/>
-      <c r="P28" s="153"/>
-      <c r="Q28" s="153"/>
-      <c r="R28" s="153"/>
+      <c r="L28" s="272"/>
+      <c r="M28" s="149"/>
+      <c r="N28" s="149"/>
+      <c r="O28" s="149"/>
+      <c r="P28" s="149"/>
+      <c r="Q28" s="149"/>
+      <c r="R28" s="149"/>
     </row>
     <row r="29" spans="2:18" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B29" s="111">
+      <c r="B29" s="110">
         <v>13</v>
       </c>
-      <c r="C29" s="154" t="s">
+      <c r="C29" s="150" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="151"/>
-      <c r="E29" s="119">
+      <c r="D29" s="147"/>
+      <c r="E29" s="117">
         <f>D28</f>
         <v>0</v>
       </c>
-      <c r="F29" s="114">
+      <c r="F29" s="252">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G29" s="248"/>
-      <c r="H29" s="115"/>
-      <c r="I29" s="152" t="s">
+      <c r="G29" s="227"/>
+      <c r="H29" s="113"/>
+      <c r="I29" s="148" t="s">
         <v>46</v>
       </c>
-      <c r="J29" s="134"/>
-      <c r="K29" s="118" t="str">
+      <c r="J29" s="131"/>
+      <c r="K29" s="116" t="str">
+        <f t="shared" ref="K29:K32" si="3">IF(D29&gt;E29,"*Numerator for "&amp;C29&amp;" Cannot be more than Denominator"&amp;CHAR(10),"")</f>
+        <v/>
+      </c>
+      <c r="L29" s="272"/>
+      <c r="M29" s="149"/>
+      <c r="N29" s="149"/>
+      <c r="O29" s="149"/>
+      <c r="P29" s="149"/>
+      <c r="Q29" s="149"/>
+      <c r="R29" s="149"/>
+    </row>
+    <row r="30" spans="2:18" s="11" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B30" s="110">
+        <v>14</v>
+      </c>
+      <c r="C30" s="150" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="112"/>
+      <c r="E30" s="112"/>
+      <c r="F30" s="252">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G30" s="227"/>
+      <c r="H30" s="113"/>
+      <c r="I30" s="148"/>
+      <c r="J30" s="131"/>
+      <c r="K30" s="116" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L29" s="153"/>
-      <c r="M29" s="153"/>
-      <c r="N29" s="153"/>
-      <c r="O29" s="153"/>
-      <c r="P29" s="153"/>
-      <c r="Q29" s="153"/>
-      <c r="R29" s="153"/>
-    </row>
-    <row r="30" spans="2:18" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B30" s="111">
-        <v>14</v>
-      </c>
-      <c r="C30" s="154" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="113"/>
-      <c r="E30" s="113"/>
-      <c r="F30" s="114">
+      <c r="L30" s="272"/>
+      <c r="M30" s="149"/>
+      <c r="N30" s="149"/>
+      <c r="O30" s="149"/>
+      <c r="P30" s="149"/>
+      <c r="Q30" s="149"/>
+      <c r="R30" s="149"/>
+    </row>
+    <row r="31" spans="2:18" s="11" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B31" s="110">
+        <v>15</v>
+      </c>
+      <c r="C31" s="150" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="112"/>
+      <c r="E31" s="175"/>
+      <c r="F31" s="252">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G30" s="248"/>
-      <c r="H30" s="115"/>
-      <c r="I30" s="152"/>
-      <c r="J30" s="134"/>
-      <c r="K30" s="118" t="str">
+      <c r="G31" s="227"/>
+      <c r="H31" s="151"/>
+      <c r="I31" s="152"/>
+      <c r="J31" s="131"/>
+      <c r="K31" s="116" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L30" s="153"/>
-      <c r="M30" s="153"/>
-      <c r="N30" s="153"/>
-      <c r="O30" s="153"/>
-      <c r="P30" s="153"/>
-      <c r="Q30" s="153"/>
-      <c r="R30" s="153"/>
-    </row>
-    <row r="31" spans="2:18" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B31" s="111">
-        <v>15</v>
-      </c>
-      <c r="C31" s="154" t="s">
-        <v>88</v>
-      </c>
-      <c r="D31" s="113"/>
-      <c r="E31" s="181"/>
-      <c r="F31" s="114">
+      <c r="L31" s="272"/>
+      <c r="M31" s="149"/>
+      <c r="N31" s="149"/>
+      <c r="O31" s="149"/>
+      <c r="P31" s="149"/>
+      <c r="Q31" s="149"/>
+      <c r="R31" s="149"/>
+    </row>
+    <row r="32" spans="2:18" s="12" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B32" s="110">
+        <v>16</v>
+      </c>
+      <c r="C32" s="150" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="180"/>
+      <c r="E32" s="176"/>
+      <c r="F32" s="252">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G31" s="248"/>
-      <c r="H31" s="155"/>
-      <c r="I31" s="156"/>
-      <c r="J31" s="134"/>
-      <c r="K31" s="118" t="str">
+      <c r="G32" s="227"/>
+      <c r="H32" s="113"/>
+      <c r="I32" s="148" t="s">
+        <v>47</v>
+      </c>
+      <c r="J32" s="131"/>
+      <c r="K32" s="116" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L31" s="153"/>
-      <c r="M31" s="153"/>
-      <c r="N31" s="153"/>
-      <c r="O31" s="153"/>
-      <c r="P31" s="153"/>
-      <c r="Q31" s="153"/>
-      <c r="R31" s="153"/>
-    </row>
-    <row r="32" spans="2:18" s="12" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B32" s="111">
-        <v>16</v>
-      </c>
-      <c r="C32" s="154" t="s">
-        <v>49</v>
-      </c>
-      <c r="D32" s="186"/>
-      <c r="E32" s="182"/>
-      <c r="F32" s="114">
+      <c r="L32" s="272"/>
+      <c r="M32" s="153"/>
+      <c r="N32" s="153"/>
+      <c r="O32" s="153"/>
+      <c r="P32" s="153"/>
+      <c r="Q32" s="153"/>
+      <c r="R32" s="153"/>
+    </row>
+    <row r="33" spans="2:18" s="5" customFormat="1" ht="15" customHeight="1">
+      <c r="B33" s="154">
+        <v>17</v>
+      </c>
+      <c r="C33" s="155" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" s="156"/>
+      <c r="E33" s="181"/>
+      <c r="F33" s="256"/>
+      <c r="G33" s="227"/>
+      <c r="H33" s="157"/>
+      <c r="I33" s="158"/>
+      <c r="J33" s="159"/>
+      <c r="K33" s="141"/>
+      <c r="L33" s="272"/>
+      <c r="M33" s="141"/>
+      <c r="N33" s="141"/>
+      <c r="O33" s="141"/>
+      <c r="P33" s="141"/>
+      <c r="Q33" s="141"/>
+      <c r="R33" s="141"/>
+    </row>
+    <row r="34" spans="2:18" s="6" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B34" s="110">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="C34" s="111" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="180"/>
+      <c r="E34" s="176"/>
+      <c r="F34" s="252">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G32" s="248"/>
-      <c r="H32" s="115"/>
-      <c r="I32" s="152" t="s">
-        <v>47</v>
-      </c>
-      <c r="J32" s="134"/>
-      <c r="K32" s="118" t="str">
-        <f t="shared" si="3"/>
+      <c r="G34" s="227"/>
+      <c r="H34" s="160"/>
+      <c r="I34" s="161" t="s">
+        <v>77</v>
+      </c>
+      <c r="J34" s="131"/>
+      <c r="K34" s="267" t="str">
+        <f>IF(SUM(D34:D39)&lt;&gt;E34,"*Sum of Numerator  17.1,17.2,17.3,17.4,17.5 and 17.6 should be equal to Denominator for 17.1","")</f>
         <v/>
       </c>
-      <c r="L32" s="157"/>
-      <c r="M32" s="157"/>
-      <c r="N32" s="157"/>
-      <c r="O32" s="157"/>
-      <c r="P32" s="157"/>
-      <c r="Q32" s="157"/>
-      <c r="R32" s="157"/>
-    </row>
-    <row r="33" spans="2:18" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="B33" s="158">
-        <v>17</v>
-      </c>
-      <c r="C33" s="159" t="s">
-        <v>23</v>
-      </c>
-      <c r="D33" s="160"/>
-      <c r="E33" s="187"/>
-      <c r="F33" s="161"/>
-      <c r="G33" s="248"/>
-      <c r="H33" s="162"/>
-      <c r="I33" s="163"/>
-      <c r="J33" s="164"/>
-      <c r="K33" s="145"/>
-      <c r="L33" s="145"/>
-      <c r="M33" s="145"/>
-      <c r="N33" s="145"/>
-      <c r="O33" s="145"/>
-      <c r="P33" s="145"/>
-      <c r="Q33" s="145"/>
-      <c r="R33" s="145"/>
-    </row>
-    <row r="34" spans="2:18" s="6" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B34" s="111">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="C34" s="112" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="186"/>
-      <c r="E34" s="182"/>
-      <c r="F34" s="114">
+      <c r="L34" s="272"/>
+      <c r="M34" s="162"/>
+      <c r="N34" s="162"/>
+      <c r="O34" s="162"/>
+      <c r="P34" s="162"/>
+      <c r="Q34" s="162"/>
+      <c r="R34" s="162"/>
+    </row>
+    <row r="35" spans="2:18" s="6" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B35" s="110">
+        <v>17.2</v>
+      </c>
+      <c r="C35" s="111" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="112"/>
+      <c r="E35" s="182">
+        <f>E34</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="252">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G34" s="248"/>
-      <c r="H34" s="165"/>
-      <c r="I34" s="166" t="s">
+      <c r="G35" s="227"/>
+      <c r="H35" s="163"/>
+      <c r="I35" s="161" t="s">
         <v>77</v>
       </c>
-      <c r="J34" s="134"/>
-      <c r="K34" s="118" t="str">
-        <f t="shared" si="3"/>
+      <c r="J35" s="131"/>
+      <c r="K35" s="116" t="str">
+        <f>IF(D35&gt;E35,"*Numerator for "&amp;C35&amp;" Cannot be more than Denominator"&amp;CHAR(10),"")</f>
         <v/>
       </c>
-      <c r="L34" s="167"/>
-      <c r="M34" s="167"/>
-      <c r="N34" s="167"/>
-      <c r="O34" s="167"/>
-      <c r="P34" s="167"/>
-      <c r="Q34" s="167"/>
-      <c r="R34" s="167"/>
-    </row>
-    <row r="35" spans="2:18" s="6" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B35" s="111">
-        <v>17.2</v>
-      </c>
-      <c r="C35" s="112" t="s">
-        <v>25</v>
-      </c>
-      <c r="D35" s="113"/>
-      <c r="E35" s="188">
-        <f>E34</f>
+      <c r="L35" s="272"/>
+      <c r="M35" s="162"/>
+      <c r="N35" s="162"/>
+      <c r="O35" s="162"/>
+      <c r="P35" s="162"/>
+      <c r="Q35" s="162"/>
+      <c r="R35" s="162"/>
+    </row>
+    <row r="36" spans="2:18" s="6" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B36" s="110">
+        <v>17.3</v>
+      </c>
+      <c r="C36" s="111" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="117">
+        <f>E32</f>
         <v>0</v>
       </c>
-      <c r="F35" s="114">
+      <c r="E36" s="117">
+        <f t="shared" ref="E36:E39" si="4">E35</f>
+        <v>0</v>
+      </c>
+      <c r="F36" s="252">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G35" s="248"/>
-      <c r="H35" s="168"/>
-      <c r="I35" s="166" t="s">
+      <c r="G36" s="227"/>
+      <c r="H36" s="164" t="s">
+        <v>47</v>
+      </c>
+      <c r="I36" s="161" t="s">
         <v>77</v>
       </c>
-      <c r="J35" s="134"/>
-      <c r="K35" s="118" t="str">
-        <f t="shared" si="3"/>
+      <c r="J36" s="131"/>
+      <c r="K36" s="116" t="str">
+        <f t="shared" ref="K36:K39" si="5">IF(D36&gt;E36,"*Numerator for "&amp;C36&amp;" Cannot be more than Denominator"&amp;CHAR(10),"")</f>
         <v/>
       </c>
-      <c r="L35" s="167"/>
-      <c r="M35" s="167"/>
-      <c r="N35" s="167"/>
-      <c r="O35" s="167"/>
-      <c r="P35" s="167"/>
-      <c r="Q35" s="167"/>
-      <c r="R35" s="167"/>
-    </row>
-    <row r="36" spans="2:18" s="6" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B36" s="111">
-        <v>17.3</v>
-      </c>
-      <c r="C36" s="112" t="s">
-        <v>26</v>
-      </c>
-      <c r="D36" s="119">
-        <f>E32</f>
+      <c r="L36" s="272"/>
+      <c r="M36" s="162"/>
+      <c r="N36" s="162"/>
+      <c r="O36" s="162"/>
+      <c r="P36" s="162"/>
+      <c r="Q36" s="162"/>
+      <c r="R36" s="162"/>
+    </row>
+    <row r="37" spans="2:18" s="6" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B37" s="110">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="C37" s="111" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="112"/>
+      <c r="E37" s="117">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E36" s="119">
-        <f t="shared" ref="E36:E39" si="4">E35</f>
-        <v>0</v>
-      </c>
-      <c r="F36" s="114">
+      <c r="F37" s="252">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G36" s="248"/>
-      <c r="H36" s="169" t="s">
-        <v>47</v>
-      </c>
-      <c r="I36" s="166" t="s">
+      <c r="G37" s="227"/>
+      <c r="H37" s="113"/>
+      <c r="I37" s="161" t="s">
         <v>77</v>
       </c>
-      <c r="J36" s="134"/>
-      <c r="K36" s="118" t="str">
-        <f t="shared" si="3"/>
+      <c r="J37" s="131"/>
+      <c r="K37" s="116" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="L36" s="167"/>
-      <c r="M36" s="167"/>
-      <c r="N36" s="167"/>
-      <c r="O36" s="167"/>
-      <c r="P36" s="167"/>
-      <c r="Q36" s="167"/>
-      <c r="R36" s="167"/>
-    </row>
-    <row r="37" spans="2:18" s="6" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B37" s="111">
-        <v>17.399999999999999</v>
-      </c>
-      <c r="C37" s="112" t="s">
-        <v>27</v>
-      </c>
-      <c r="D37" s="113"/>
-      <c r="E37" s="119">
+      <c r="L37" s="272"/>
+      <c r="M37" s="162"/>
+      <c r="N37" s="162"/>
+      <c r="O37" s="162"/>
+      <c r="P37" s="162"/>
+      <c r="Q37" s="162"/>
+      <c r="R37" s="162"/>
+    </row>
+    <row r="38" spans="2:18" s="6" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B38" s="110">
+        <v>17.5</v>
+      </c>
+      <c r="C38" s="111" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" s="112"/>
+      <c r="E38" s="117">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F37" s="114">
+      <c r="F38" s="252">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G37" s="248"/>
-      <c r="H37" s="115"/>
-      <c r="I37" s="166" t="s">
+      <c r="G38" s="227"/>
+      <c r="H38" s="151"/>
+      <c r="I38" s="161" t="s">
         <v>77</v>
       </c>
-      <c r="J37" s="134"/>
-      <c r="K37" s="118" t="str">
-        <f t="shared" si="3"/>
+      <c r="J38" s="131"/>
+      <c r="K38" s="116" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="L37" s="167"/>
-      <c r="M37" s="167"/>
-      <c r="N37" s="167"/>
-      <c r="O37" s="167"/>
-      <c r="P37" s="167"/>
-      <c r="Q37" s="167"/>
-      <c r="R37" s="167"/>
-    </row>
-    <row r="38" spans="2:18" s="6" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B38" s="111">
-        <v>17.5</v>
-      </c>
-      <c r="C38" s="112" t="s">
-        <v>28</v>
-      </c>
-      <c r="D38" s="113"/>
-      <c r="E38" s="119">
+      <c r="L38" s="272"/>
+      <c r="M38" s="162"/>
+      <c r="N38" s="162"/>
+      <c r="O38" s="162"/>
+      <c r="P38" s="162"/>
+      <c r="Q38" s="162"/>
+      <c r="R38" s="162"/>
+    </row>
+    <row r="39" spans="2:18" s="6" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
+      <c r="B39" s="132">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="C39" s="133" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" s="134"/>
+      <c r="E39" s="135">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F38" s="114">
+      <c r="F39" s="252">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G38" s="248"/>
-      <c r="H38" s="155"/>
-      <c r="I38" s="166" t="s">
+      <c r="G39" s="227"/>
+      <c r="H39" s="136"/>
+      <c r="I39" s="165" t="s">
         <v>77</v>
       </c>
-      <c r="J38" s="134"/>
-      <c r="K38" s="118" t="str">
-        <f t="shared" si="3"/>
+      <c r="J39" s="138"/>
+      <c r="K39" s="116" t="str">
+        <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="L38" s="167"/>
-      <c r="M38" s="167"/>
-      <c r="N38" s="167"/>
-      <c r="O38" s="167"/>
-      <c r="P38" s="167"/>
-      <c r="Q38" s="167"/>
-      <c r="R38" s="167"/>
-    </row>
-    <row r="39" spans="2:18" s="6" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B39" s="135">
-        <v>17.600000000000001</v>
-      </c>
-      <c r="C39" s="136" t="s">
-        <v>29</v>
-      </c>
-      <c r="D39" s="137"/>
-      <c r="E39" s="138">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F39" s="114">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G39" s="248"/>
-      <c r="H39" s="139"/>
-      <c r="I39" s="170" t="s">
-        <v>77</v>
-      </c>
-      <c r="J39" s="141"/>
-      <c r="K39" s="118" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="L39" s="167"/>
-      <c r="M39" s="167"/>
-      <c r="N39" s="167"/>
-      <c r="O39" s="167"/>
-      <c r="P39" s="167"/>
-      <c r="Q39" s="167"/>
-      <c r="R39" s="167"/>
-    </row>
-    <row r="40" spans="2:18" s="8" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B40" s="256" t="s">
+      <c r="L39" s="272"/>
+      <c r="M39" s="162"/>
+      <c r="N39" s="162"/>
+      <c r="O39" s="162"/>
+      <c r="P39" s="162"/>
+      <c r="Q39" s="162"/>
+      <c r="R39" s="162"/>
+    </row>
+    <row r="40" spans="2:18" s="8" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B40" s="235" t="s">
         <v>79</v>
       </c>
-      <c r="C40" s="256"/>
-      <c r="D40" s="256"/>
-      <c r="E40" s="256"/>
-      <c r="F40" s="256"/>
-      <c r="G40" s="248"/>
-      <c r="H40" s="243"/>
-      <c r="I40" s="243"/>
-      <c r="J40" s="243"/>
-      <c r="K40" s="171"/>
-      <c r="L40" s="171"/>
-      <c r="M40" s="171"/>
-      <c r="N40" s="171"/>
-      <c r="O40" s="171"/>
-      <c r="P40" s="171"/>
-      <c r="Q40" s="171"/>
-      <c r="R40" s="171"/>
+      <c r="C40" s="235"/>
+      <c r="D40" s="235"/>
+      <c r="E40" s="235"/>
+      <c r="F40" s="235"/>
+      <c r="G40" s="227"/>
+      <c r="H40" s="222"/>
+      <c r="I40" s="222"/>
+      <c r="J40" s="222"/>
+      <c r="K40" s="166"/>
+      <c r="L40" s="273"/>
+      <c r="M40" s="166"/>
+      <c r="N40" s="166"/>
+      <c r="O40" s="166"/>
+      <c r="P40" s="166"/>
+      <c r="Q40" s="166"/>
+      <c r="R40" s="166"/>
     </row>
   </sheetData>
   <sheetProtection password="CC71" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
-  <mergeCells count="14">
+  <mergeCells count="17">
+    <mergeCell ref="L8:L23"/>
+    <mergeCell ref="L26:L40"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B2:R2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="H3:J5"/>
     <mergeCell ref="H26:J26"/>
     <mergeCell ref="H40:J40"/>
     <mergeCell ref="B6:C6"/>
@@ -6236,139 +6784,211 @@
     <mergeCell ref="B24:F25"/>
     <mergeCell ref="H24:J25"/>
     <mergeCell ref="B40:F40"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B2:R2"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="25" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="83" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="cellIs" dxfId="24" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="78" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:F17">
-    <cfRule type="cellIs" dxfId="23" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="75" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="22" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="50" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="21" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="49" operator="equal">
       <formula>0</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="20" priority="29" operator="equal">
-      <formula>0</formula>
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>D12&lt;D10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="19" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="47" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="18" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="46" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="cellIs" dxfId="17" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="45" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="16" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="44" operator="equal">
       <formula>0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="3">
+      <formula>(SUM($D$19:$D$23)&lt;&gt;E19)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="15" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="43" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="cellIs" dxfId="14" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="42" operator="equal">
       <formula>0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="31" priority="7">
+      <formula>IF(D20&gt;0,(SUM($D$19:$D$23)&lt;&gt;E19),"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="13" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="41" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="12" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="40" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="11" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="39" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="10" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="38" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="37" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="cellIs" dxfId="8" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="36" operator="equal">
       <formula>0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="15">
+      <formula>IF(D36&gt;0,(SUM(D34,D35,D36,D37,D38,D39)&lt;&gt;E34),"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="cellIs" dxfId="7" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="35" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="cellIs" dxfId="6" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="34" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="cellIs" dxfId="5" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="33" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="cellIs" dxfId="4" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="32" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="expression" dxfId="3" priority="11">
+    <cfRule type="expression" dxfId="19" priority="30">
       <formula>D12&lt;D10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19:F23">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28:F32">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F34:F39">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:J5">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="19">
+      <formula>LEN(TRIM(H3))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule type="expression" dxfId="14" priority="18">
+      <formula>IF(D34&gt;0,(SUM(D34,D35,D36,D37,D38,D39)&lt;&gt;E34),"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="expression" dxfId="13" priority="16">
+      <formula>IF(D35&gt;0,(SUM(D34,D35,D36,D37,D38,D39)&lt;&gt;E34),"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37">
+    <cfRule type="expression" dxfId="12" priority="14">
+      <formula>IF(D37&gt;0,(SUM(D34,D35,D36,D37,D38,D39)&lt;&gt;E34),"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
+    <cfRule type="expression" dxfId="11" priority="13">
+      <formula>IF(D38&gt;0,(SUM(D34,D35,D36,D37,D38,D39)&lt;&gt;E34),"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39">
+    <cfRule type="expression" dxfId="10" priority="12">
+      <formula>IF(D35&gt;0,(SUM(D34,D35,D36,D37,D38,D39)&lt;&gt;E34),"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34">
+    <cfRule type="expression" dxfId="9" priority="11">
+      <formula>SUM(D34,D35,D36,D37,D38,D39)&lt;&gt;E34</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L8:L23">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="10">
+      <formula>LEN(TRIM(L8))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L26:L40">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="9">
+      <formula>LEN(TRIM(L26))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19">
+    <cfRule type="expression" dxfId="6" priority="8">
+      <formula>IF(D19&gt;0,(SUM($D$19:$D$23)&lt;&gt;E19),"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>IF(D21&gt;0,(SUM($D$19:$D$23)&lt;&gt;E19),"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>IF(D22&gt;0,(SUM($D$19:$D$23)&lt;&gt;E19),"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>IF(D23&gt;0,(SUM($D$19:$D$23)&lt;&gt;E19),"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
consolidated Prep Module added
</commit_message>
<xml_diff>
--- a/web/hca.xlsx
+++ b/web/hca.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="121">
   <si>
     <t>Num</t>
   </si>
@@ -485,6 +485,15 @@
   <si>
     <t>Data Error Checks</t>
   </si>
+  <si>
+    <t>Early Warnings</t>
+  </si>
+  <si>
+    <t>warnings</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
 </sst>
 </file>
 
@@ -495,7 +504,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="yyyy/mmm"/>
   </numFmts>
-  <fonts count="46">
+  <fonts count="48">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -785,8 +794,22 @@
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -895,8 +918,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="96">
+  <borders count="112">
     <border>
       <left/>
       <right/>
@@ -1799,48 +1834,24 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
+      <top style="medium">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color theme="4"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="4"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color theme="4"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
@@ -1866,32 +1877,6 @@
         <color theme="4"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color theme="4"/>
-      </right>
-      <top style="medium">
-        <color theme="4"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="8"/>
-      </left>
-      <right style="medium">
-        <color theme="8"/>
-      </right>
-      <top style="medium">
-        <color theme="8"/>
-      </top>
-      <bottom style="medium">
-        <color theme="8"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1989,26 +1974,345 @@
     </border>
     <border>
       <left style="medium">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="4"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color theme="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="8"/>
+      </top>
+      <bottom style="medium">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="8"/>
+      </top>
+      <bottom style="medium">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right style="medium">
         <color theme="8"/>
       </right>
+      <top style="medium">
+        <color theme="8"/>
+      </top>
+      <bottom style="medium">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="4"/>
+      </right>
+      <top style="medium">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="4"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color theme="8"/>
+        <color theme="4"/>
       </left>
       <right style="medium">
-        <color theme="8"/>
+        <color theme="4"/>
+      </right>
+      <top style="medium">
+        <color theme="4"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="medium">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="medium">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="medium">
+        <color theme="4"/>
+      </right>
+      <top style="medium">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="medium">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="medium">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4"/>
+      </left>
+      <right style="medium">
+        <color theme="4"/>
+      </right>
+      <top style="medium">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4"/>
+      </left>
+      <right style="medium">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4"/>
+      </left>
+      <right style="medium">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4"/>
+      </left>
+      <right style="medium">
+        <color theme="4"/>
+      </right>
+      <top style="medium">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4"/>
+      </left>
+      <right style="medium">
+        <color theme="4"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4"/>
+      </left>
+      <right style="medium">
+        <color theme="4"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color theme="8"/>
-      </bottom>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -2016,106 +2320,63 @@
         <color theme="4"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="medium">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
       </left>
       <right style="medium">
         <color theme="4"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color theme="8"/>
-      </top>
-      <bottom style="medium">
-        <color theme="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color theme="8"/>
-      </top>
-      <bottom style="medium">
-        <color theme="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color theme="8"/>
-      </right>
-      <top style="medium">
-        <color theme="8"/>
-      </top>
-      <bottom style="medium">
-        <color theme="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
       <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="4"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color theme="4"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2127,7 +2388,7 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="287">
+  <cellXfs count="302">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2425,15 +2686,6 @@
     <xf numFmtId="164" fontId="33" fillId="18" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="18" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="35" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2449,13 +2701,6 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2468,9 +2713,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2480,9 +2722,6 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2516,16 +2755,6 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2550,18 +2779,8 @@
     <xf numFmtId="164" fontId="33" fillId="17" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="17" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="17" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2569,9 +2788,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2581,15 +2797,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="36" fillId="17" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="41" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2623,12 +2830,6 @@
     <xf numFmtId="164" fontId="36" fillId="6" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2641,46 +2842,70 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="17" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="17" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="17" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="18" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="33" fillId="17" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="51" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="86" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2792,6 +3017,75 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="33" fillId="18" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2804,16 +3098,22 @@
     <xf numFmtId="164" fontId="39" fillId="17" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="38" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2831,159 +3131,163 @@
     <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="17" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="18" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="18" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="18" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="6" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="93" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="94" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="95" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="96" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="6" borderId="95" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="6" borderId="96" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="95" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="97" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="99" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="100" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="101" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="102" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="19" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="103" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="104" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="105" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="20" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="103" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="104" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="105" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="107" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="106" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="108" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="109" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="110" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="111" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="36" fillId="17" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="17" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="17" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="17" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="17" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="18" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="46" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="72" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="33" fillId="17" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="17" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="77" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="88" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="51" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="2" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="94" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="95" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2993,7 +3297,107 @@
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="60">
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -3001,6 +3405,56 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.59996337778862885"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3236,6 +3690,16 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="4" tint="0.59996337778862885"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="0"/>
       </font>
       <fill>
@@ -3381,6 +3845,16 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4135,111 +4609,111 @@
       <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.59765625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="89.3984375" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.59765625" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="155.1328125" style="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="89.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="155.140625" style="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="164" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.73046875" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.265625" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.3984375" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.42578125" style="17" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.73046875" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.265625" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.3984375" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.42578125" style="15" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.73046875" style="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.265625" style="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.3984375" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.42578125" style="15" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18" style="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.86328125" style="15"/>
+    <col min="18" max="16384" width="8.85546875" style="15"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:17" s="1" customFormat="1">
-      <c r="A2" s="186"/>
-      <c r="B2" s="186"/>
-      <c r="C2" s="186"/>
-      <c r="D2" s="186"/>
-      <c r="E2" s="186"/>
-      <c r="F2" s="186"/>
-      <c r="G2" s="186"/>
-      <c r="H2" s="186"/>
-      <c r="I2" s="186"/>
+      <c r="A2" s="177"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1">
-      <c r="A3" s="186"/>
-      <c r="B3" s="186"/>
-      <c r="C3" s="186"/>
-      <c r="D3" s="186"/>
-      <c r="E3" s="186"/>
-      <c r="F3" s="186"/>
-      <c r="G3" s="186"/>
-      <c r="H3" s="186"/>
-      <c r="I3" s="186"/>
+      <c r="A3" s="177"/>
+      <c r="B3" s="177"/>
+      <c r="C3" s="177"/>
+      <c r="D3" s="177"/>
+      <c r="E3" s="177"/>
+      <c r="F3" s="177"/>
+      <c r="G3" s="177"/>
+      <c r="H3" s="177"/>
+      <c r="I3" s="177"/>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1">
-      <c r="A4" s="186"/>
-      <c r="B4" s="186"/>
-      <c r="C4" s="186"/>
-      <c r="D4" s="186"/>
-      <c r="E4" s="186"/>
-      <c r="F4" s="186"/>
-      <c r="G4" s="186"/>
-      <c r="H4" s="186"/>
-      <c r="I4" s="186"/>
+      <c r="A4" s="177"/>
+      <c r="B4" s="177"/>
+      <c r="C4" s="177"/>
+      <c r="D4" s="177"/>
+      <c r="E4" s="177"/>
+      <c r="F4" s="177"/>
+      <c r="G4" s="177"/>
+      <c r="H4" s="177"/>
+      <c r="I4" s="177"/>
     </row>
-    <row r="6" spans="1:17" ht="25.15">
-      <c r="A6" s="195" t="s">
+    <row r="6" spans="1:17" ht="26.25">
+      <c r="A6" s="186" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="195"/>
-      <c r="C6" s="195"/>
-      <c r="D6" s="195"/>
-      <c r="E6" s="195"/>
-      <c r="F6" s="195"/>
-      <c r="G6" s="195"/>
-      <c r="H6" s="195"/>
-      <c r="I6" s="195"/>
-      <c r="J6" s="195"/>
-      <c r="K6" s="195"/>
-      <c r="L6" s="195"/>
-      <c r="M6" s="195"/>
-      <c r="N6" s="195"/>
-      <c r="O6" s="195"/>
-      <c r="P6" s="195"/>
-      <c r="Q6" s="195"/>
+      <c r="B6" s="186"/>
+      <c r="C6" s="186"/>
+      <c r="D6" s="186"/>
+      <c r="E6" s="186"/>
+      <c r="F6" s="186"/>
+      <c r="G6" s="186"/>
+      <c r="H6" s="186"/>
+      <c r="I6" s="186"/>
+      <c r="J6" s="186"/>
+      <c r="K6" s="186"/>
+      <c r="L6" s="186"/>
+      <c r="M6" s="186"/>
+      <c r="N6" s="186"/>
+      <c r="O6" s="186"/>
+      <c r="P6" s="186"/>
+      <c r="Q6" s="186"/>
     </row>
-    <row r="7" spans="1:17" ht="15.4" thickBot="1"/>
+    <row r="7" spans="1:17" ht="15.75" thickBot="1"/>
     <row r="8" spans="1:17" s="18" customFormat="1" ht="25.15" customHeight="1" thickTop="1">
       <c r="A8" s="25"/>
-      <c r="B8" s="196" t="s">
+      <c r="B8" s="187" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="196"/>
-      <c r="D8" s="196"/>
-      <c r="E8" s="196"/>
-      <c r="F8" s="197" t="s">
+      <c r="C8" s="187"/>
+      <c r="D8" s="187"/>
+      <c r="E8" s="187"/>
+      <c r="F8" s="188" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="197"/>
-      <c r="H8" s="197"/>
-      <c r="I8" s="197"/>
-      <c r="J8" s="197" t="s">
+      <c r="G8" s="188"/>
+      <c r="H8" s="188"/>
+      <c r="I8" s="188"/>
+      <c r="J8" s="188" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="197"/>
-      <c r="L8" s="197"/>
-      <c r="M8" s="197"/>
-      <c r="N8" s="197" t="s">
+      <c r="K8" s="188"/>
+      <c r="L8" s="188"/>
+      <c r="M8" s="188"/>
+      <c r="N8" s="188" t="s">
         <v>33</v>
       </c>
-      <c r="O8" s="197"/>
-      <c r="P8" s="197"/>
-      <c r="Q8" s="205"/>
+      <c r="O8" s="188"/>
+      <c r="P8" s="188"/>
+      <c r="Q8" s="196"/>
     </row>
-    <row r="9" spans="1:17" s="24" customFormat="1">
+    <row r="9" spans="1:17" s="24" customFormat="1" ht="15.75">
       <c r="A9" s="19" t="s">
         <v>17</v>
       </c>
@@ -4293,31 +4767,31 @@
       </c>
     </row>
     <row r="10" spans="1:17" s="32" customFormat="1" ht="58.15" customHeight="1">
-      <c r="A10" s="198" t="s">
+      <c r="A10" s="189" t="s">
         <v>89</v>
       </c>
-      <c r="B10" s="199"/>
-      <c r="C10" s="199"/>
-      <c r="D10" s="199"/>
-      <c r="E10" s="199"/>
-      <c r="F10" s="200" t="s">
+      <c r="B10" s="190"/>
+      <c r="C10" s="190"/>
+      <c r="D10" s="190"/>
+      <c r="E10" s="190"/>
+      <c r="F10" s="191" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="200"/>
-      <c r="H10" s="200"/>
-      <c r="I10" s="200"/>
-      <c r="J10" s="200" t="s">
+      <c r="G10" s="191"/>
+      <c r="H10" s="191"/>
+      <c r="I10" s="191"/>
+      <c r="J10" s="191" t="s">
         <v>39</v>
       </c>
-      <c r="K10" s="200"/>
-      <c r="L10" s="200"/>
-      <c r="M10" s="200"/>
-      <c r="N10" s="200" t="s">
+      <c r="K10" s="191"/>
+      <c r="L10" s="191"/>
+      <c r="M10" s="191"/>
+      <c r="N10" s="191" t="s">
         <v>40</v>
       </c>
-      <c r="O10" s="200"/>
-      <c r="P10" s="200"/>
-      <c r="Q10" s="201"/>
+      <c r="O10" s="191"/>
+      <c r="P10" s="191"/>
+      <c r="Q10" s="192"/>
     </row>
     <row r="11" spans="1:17" s="38" customFormat="1" ht="43.9" customHeight="1">
       <c r="A11" s="34">
@@ -4481,7 +4955,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="38" customFormat="1" ht="34.5">
+    <row r="15" spans="1:17" s="38" customFormat="1" ht="36">
       <c r="A15" s="34">
         <v>5</v>
       </c>
@@ -4520,7 +4994,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="38" customFormat="1" ht="17.25">
+    <row r="16" spans="1:17" s="38" customFormat="1" ht="36">
       <c r="A16" s="39">
         <v>6</v>
       </c>
@@ -4592,7 +5066,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="38" customFormat="1" ht="17.25">
+    <row r="18" spans="1:17" s="38" customFormat="1" ht="36">
       <c r="A18" s="39">
         <v>8</v>
       </c>
@@ -4625,7 +5099,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="38" customFormat="1" ht="17.25">
+    <row r="19" spans="1:17" s="38" customFormat="1" ht="36">
       <c r="A19" s="34">
         <v>9</v>
       </c>
@@ -4664,7 +5138,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="38" customFormat="1" ht="35.25">
+    <row r="20" spans="1:17" s="38" customFormat="1" ht="36">
       <c r="A20" s="34">
         <v>10</v>
       </c>
@@ -4703,7 +5177,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="33" customFormat="1" ht="20.65">
+    <row r="21" spans="1:17" s="33" customFormat="1" ht="20.25">
       <c r="A21" s="29">
         <v>11</v>
       </c>
@@ -4711,24 +5185,24 @@
         <v>48</v>
       </c>
       <c r="C21" s="31"/>
-      <c r="D21" s="206" t="s">
+      <c r="D21" s="197" t="s">
         <v>93</v>
       </c>
-      <c r="E21" s="207"/>
-      <c r="F21" s="207"/>
-      <c r="G21" s="207"/>
-      <c r="H21" s="207"/>
-      <c r="I21" s="207"/>
-      <c r="J21" s="207"/>
-      <c r="K21" s="207"/>
-      <c r="L21" s="207"/>
-      <c r="M21" s="207"/>
-      <c r="N21" s="207"/>
-      <c r="O21" s="207"/>
-      <c r="P21" s="207"/>
-      <c r="Q21" s="208"/>
+      <c r="E21" s="198"/>
+      <c r="F21" s="198"/>
+      <c r="G21" s="198"/>
+      <c r="H21" s="198"/>
+      <c r="I21" s="198"/>
+      <c r="J21" s="198"/>
+      <c r="K21" s="198"/>
+      <c r="L21" s="198"/>
+      <c r="M21" s="198"/>
+      <c r="N21" s="198"/>
+      <c r="O21" s="198"/>
+      <c r="P21" s="198"/>
+      <c r="Q21" s="199"/>
     </row>
-    <row r="22" spans="1:17" s="14" customFormat="1" ht="17.25">
+    <row r="22" spans="1:17" s="14" customFormat="1" ht="18">
       <c r="A22" s="69">
         <v>11.1</v>
       </c>
@@ -4739,7 +5213,7 @@
       <c r="D22" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="187" t="s">
+      <c r="E22" s="178" t="s">
         <v>56</v>
       </c>
       <c r="F22" s="35"/>
@@ -4767,7 +5241,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="14" customFormat="1" ht="17.25">
+    <row r="23" spans="1:17" s="14" customFormat="1" ht="18">
       <c r="A23" s="69">
         <v>11.2</v>
       </c>
@@ -4778,7 +5252,7 @@
       <c r="D23" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="218"/>
+      <c r="E23" s="209"/>
       <c r="F23" s="40" t="s">
         <v>44</v>
       </c>
@@ -4810,7 +5284,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="14" customFormat="1" ht="17.25">
+    <row r="24" spans="1:17" s="14" customFormat="1" ht="18">
       <c r="A24" s="69">
         <v>11.3</v>
       </c>
@@ -4821,7 +5295,7 @@
       <c r="D24" s="69" t="s">
         <v>82</v>
       </c>
-      <c r="E24" s="188"/>
+      <c r="E24" s="179"/>
       <c r="F24" s="35"/>
       <c r="G24" s="35" t="s">
         <v>41</v>
@@ -4847,7 +5321,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="14" customFormat="1" ht="17.25">
+    <row r="25" spans="1:17" s="14" customFormat="1" ht="36">
       <c r="A25" s="69">
         <v>11.4</v>
       </c>
@@ -4858,7 +5332,7 @@
       <c r="D25" s="69" t="s">
         <v>83</v>
       </c>
-      <c r="E25" s="187" t="s">
+      <c r="E25" s="178" t="s">
         <v>80</v>
       </c>
       <c r="F25" s="40"/>
@@ -4886,7 +5360,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="14" customFormat="1" ht="17.649999999999999" thickBot="1">
+    <row r="26" spans="1:17" s="14" customFormat="1" ht="18.75" thickBot="1">
       <c r="A26" s="69">
         <v>11.5</v>
       </c>
@@ -4897,7 +5371,7 @@
       <c r="D26" s="69" t="s">
         <v>84</v>
       </c>
-      <c r="E26" s="188"/>
+      <c r="E26" s="179"/>
       <c r="F26" s="45"/>
       <c r="G26" s="45" t="s">
         <v>41</v>
@@ -4923,51 +5397,51 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="15.75" thickTop="1" thickBot="1">
-      <c r="A27" s="202"/>
-      <c r="B27" s="203"/>
-      <c r="C27" s="203"/>
-      <c r="D27" s="203"/>
-      <c r="E27" s="203"/>
-      <c r="F27" s="203"/>
-      <c r="G27" s="203"/>
-      <c r="H27" s="203"/>
-      <c r="I27" s="203"/>
-      <c r="J27" s="203"/>
-      <c r="K27" s="203"/>
-      <c r="L27" s="203"/>
-      <c r="M27" s="203"/>
-      <c r="N27" s="203"/>
-      <c r="O27" s="203"/>
-      <c r="P27" s="203"/>
-      <c r="Q27" s="204"/>
+    <row r="27" spans="1:17" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A27" s="193"/>
+      <c r="B27" s="194"/>
+      <c r="C27" s="194"/>
+      <c r="D27" s="194"/>
+      <c r="E27" s="194"/>
+      <c r="F27" s="194"/>
+      <c r="G27" s="194"/>
+      <c r="H27" s="194"/>
+      <c r="I27" s="194"/>
+      <c r="J27" s="194"/>
+      <c r="K27" s="194"/>
+      <c r="L27" s="194"/>
+      <c r="M27" s="194"/>
+      <c r="N27" s="194"/>
+      <c r="O27" s="194"/>
+      <c r="P27" s="194"/>
+      <c r="Q27" s="195"/>
     </row>
     <row r="28" spans="1:17" s="32" customFormat="1" ht="21" thickTop="1">
-      <c r="A28" s="192" t="s">
+      <c r="A28" s="183" t="s">
         <v>90</v>
       </c>
-      <c r="B28" s="193"/>
-      <c r="C28" s="193"/>
-      <c r="D28" s="193"/>
-      <c r="E28" s="194"/>
-      <c r="F28" s="215" t="s">
+      <c r="B28" s="184"/>
+      <c r="C28" s="184"/>
+      <c r="D28" s="184"/>
+      <c r="E28" s="185"/>
+      <c r="F28" s="206" t="s">
         <v>45</v>
       </c>
-      <c r="G28" s="216"/>
-      <c r="H28" s="216"/>
-      <c r="I28" s="217"/>
-      <c r="J28" s="212" t="s">
+      <c r="G28" s="207"/>
+      <c r="H28" s="207"/>
+      <c r="I28" s="208"/>
+      <c r="J28" s="203" t="s">
         <v>45</v>
       </c>
-      <c r="K28" s="213"/>
-      <c r="L28" s="213"/>
-      <c r="M28" s="214"/>
-      <c r="N28" s="209" t="s">
+      <c r="K28" s="204"/>
+      <c r="L28" s="204"/>
+      <c r="M28" s="205"/>
+      <c r="N28" s="200" t="s">
         <v>45</v>
       </c>
-      <c r="O28" s="210"/>
-      <c r="P28" s="210"/>
-      <c r="Q28" s="211"/>
+      <c r="O28" s="201"/>
+      <c r="P28" s="201"/>
+      <c r="Q28" s="202"/>
     </row>
     <row r="29" spans="1:17" s="38" customFormat="1" ht="55.5" customHeight="1">
       <c r="A29" s="69">
@@ -5152,7 +5626,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="13" customFormat="1" ht="20.65">
+    <row r="34" spans="1:17" s="13" customFormat="1" ht="20.25">
       <c r="A34" s="29">
         <v>17</v>
       </c>
@@ -5160,22 +5634,22 @@
         <v>23</v>
       </c>
       <c r="C34" s="31"/>
-      <c r="D34" s="206" t="s">
+      <c r="D34" s="197" t="s">
         <v>93</v>
       </c>
-      <c r="E34" s="207"/>
-      <c r="F34" s="207"/>
-      <c r="G34" s="207"/>
-      <c r="H34" s="207"/>
-      <c r="I34" s="207"/>
-      <c r="J34" s="207"/>
-      <c r="K34" s="207"/>
-      <c r="L34" s="207"/>
-      <c r="M34" s="207"/>
-      <c r="N34" s="207"/>
-      <c r="O34" s="207"/>
-      <c r="P34" s="207"/>
-      <c r="Q34" s="208"/>
+      <c r="E34" s="198"/>
+      <c r="F34" s="198"/>
+      <c r="G34" s="198"/>
+      <c r="H34" s="198"/>
+      <c r="I34" s="198"/>
+      <c r="J34" s="198"/>
+      <c r="K34" s="198"/>
+      <c r="L34" s="198"/>
+      <c r="M34" s="198"/>
+      <c r="N34" s="198"/>
+      <c r="O34" s="198"/>
+      <c r="P34" s="198"/>
+      <c r="Q34" s="199"/>
     </row>
     <row r="35" spans="1:17" s="14" customFormat="1" ht="41.65" customHeight="1">
       <c r="A35" s="69">
@@ -5188,7 +5662,7 @@
       <c r="D35" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="189" t="s">
+      <c r="E35" s="180" t="s">
         <v>116</v>
       </c>
       <c r="F35" s="59"/>
@@ -5227,7 +5701,7 @@
       <c r="D36" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="E36" s="190"/>
+      <c r="E36" s="181"/>
       <c r="F36" s="61"/>
       <c r="G36" s="40" t="s">
         <v>77</v>
@@ -5264,7 +5738,7 @@
       <c r="D37" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="191"/>
+      <c r="E37" s="182"/>
       <c r="F37" s="59" t="s">
         <v>47</v>
       </c>
@@ -5307,7 +5781,7 @@
       <c r="D38" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="E38" s="189" t="s">
+      <c r="E38" s="180" t="s">
         <v>79</v>
       </c>
       <c r="F38" s="61"/>
@@ -5346,7 +5820,7 @@
       <c r="D39" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="E39" s="190"/>
+      <c r="E39" s="181"/>
       <c r="F39" s="59"/>
       <c r="G39" s="35" t="s">
         <v>77</v>
@@ -5383,7 +5857,7 @@
       <c r="D40" s="69" t="s">
         <v>85</v>
       </c>
-      <c r="E40" s="191"/>
+      <c r="E40" s="182"/>
       <c r="F40" s="63"/>
       <c r="G40" s="64" t="s">
         <v>77</v>
@@ -5409,7 +5883,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="15.4" thickTop="1"/>
+    <row r="41" spans="1:17" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="21">
     <mergeCell ref="D34:Q34"/>
@@ -5452,37 +5926,40 @@
     <tabColor rgb="FF00B050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:W40"/>
+  <dimension ref="B1:X40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane xSplit="3" ySplit="7" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.53125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.59765625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="129.265625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="17.86328125" style="72" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" style="71" customWidth="1"/>
-    <col min="6" max="6" width="12" style="257" customWidth="1"/>
-    <col min="7" max="7" width="5.59765625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.1328125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="2.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="77.265625" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="39.9296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="9.1328125" style="1"/>
-    <col min="16" max="16" width="15.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.73046875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="15.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.1328125" style="1"/>
+    <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="129.28515625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" style="72" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="71" customWidth="1"/>
+    <col min="6" max="6" width="12" style="162" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="3.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="77.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="31.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" style="1" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="30.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="1"/>
+    <col min="17" max="17" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23" s="75" customFormat="1" ht="34.35" hidden="1" customHeight="1" thickBot="1">
+    <row r="1" spans="2:24" s="75" customFormat="1" ht="34.35" hidden="1" customHeight="1" thickBot="1">
       <c r="B1" s="84" t="s">
         <v>103</v>
       </c>
@@ -5495,7 +5972,7 @@
       <c r="E1" s="87" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="250" t="s">
+      <c r="F1" s="159" t="s">
         <v>101</v>
       </c>
       <c r="G1" s="87" t="s">
@@ -5508,131 +5985,135 @@
         <v>2020</v>
       </c>
       <c r="J1" s="88"/>
-      <c r="K1" s="236" t="s">
+      <c r="K1" s="214" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="237"/>
-      <c r="M1" s="237"/>
-      <c r="N1" s="238"/>
-      <c r="O1" s="89"/>
-      <c r="P1" s="90">
+      <c r="L1" s="215"/>
+      <c r="M1" s="215"/>
+      <c r="N1" s="215"/>
+      <c r="O1" s="216"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="90">
         <f>DATE(I1,G1,"01")</f>
         <v>43862</v>
       </c>
-      <c r="Q1" s="90">
-        <f>P1-365</f>
+      <c r="R1" s="90">
+        <f>Q1-365</f>
         <v>43497</v>
       </c>
-      <c r="R1" s="91">
-        <f>Q1-365</f>
+      <c r="S1" s="91">
+        <f>R1-365</f>
         <v>43132</v>
       </c>
-      <c r="S1" s="82"/>
       <c r="T1" s="82"/>
       <c r="U1" s="82"/>
-      <c r="V1" s="73">
+      <c r="V1" s="82"/>
+      <c r="W1" s="73">
         <v>0</v>
       </c>
-      <c r="W1" s="74"/>
+      <c r="X1" s="74"/>
     </row>
-    <row r="2" spans="2:23" s="77" customFormat="1" ht="34.35" hidden="1" customHeight="1" thickBot="1">
-      <c r="B2" s="245" t="s">
+    <row r="2" spans="2:24" s="77" customFormat="1" ht="34.35" hidden="1" customHeight="1" thickBot="1">
+      <c r="B2" s="223" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="246"/>
-      <c r="D2" s="246"/>
-      <c r="E2" s="246"/>
-      <c r="F2" s="246"/>
-      <c r="G2" s="246"/>
-      <c r="H2" s="246"/>
-      <c r="I2" s="246"/>
-      <c r="J2" s="246"/>
-      <c r="K2" s="246"/>
-      <c r="L2" s="246"/>
-      <c r="M2" s="246"/>
-      <c r="N2" s="246"/>
-      <c r="O2" s="246"/>
-      <c r="P2" s="246"/>
-      <c r="Q2" s="246"/>
-      <c r="R2" s="247"/>
-      <c r="S2" s="76"/>
-      <c r="V2" s="73">
+      <c r="C2" s="224"/>
+      <c r="D2" s="224"/>
+      <c r="E2" s="224"/>
+      <c r="F2" s="224"/>
+      <c r="G2" s="224"/>
+      <c r="H2" s="224"/>
+      <c r="I2" s="224"/>
+      <c r="J2" s="224"/>
+      <c r="K2" s="224"/>
+      <c r="L2" s="224"/>
+      <c r="M2" s="224"/>
+      <c r="N2" s="224"/>
+      <c r="O2" s="224"/>
+      <c r="P2" s="224"/>
+      <c r="Q2" s="224"/>
+      <c r="R2" s="224"/>
+      <c r="S2" s="225"/>
+      <c r="T2" s="76"/>
+      <c r="W2" s="73">
         <v>1</v>
       </c>
-      <c r="W2" s="78"/>
+      <c r="X2" s="78"/>
     </row>
-    <row r="3" spans="2:23" s="77" customFormat="1" ht="48" customHeight="1" thickBot="1">
-      <c r="B3" s="170"/>
-      <c r="C3" s="171"/>
-      <c r="D3" s="171"/>
-      <c r="E3" s="171"/>
-      <c r="F3" s="172"/>
+    <row r="3" spans="2:24" s="77" customFormat="1" ht="48" customHeight="1" thickBot="1">
+      <c r="B3" s="151"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
+      <c r="F3" s="153"/>
       <c r="G3" s="92"/>
-      <c r="H3" s="258" t="str">
+      <c r="H3" s="228" t="str">
         <f>IF(LEN(L8&amp;L26)&lt;1,"","Form Has Data Errors, Please correct before submitting or uploading")</f>
         <v/>
       </c>
-      <c r="I3" s="259"/>
-      <c r="J3" s="260"/>
+      <c r="I3" s="229"/>
+      <c r="J3" s="230"/>
       <c r="K3" s="92"/>
       <c r="L3" s="92"/>
-      <c r="M3" s="92"/>
+      <c r="M3" s="158"/>
       <c r="N3" s="92"/>
       <c r="O3" s="92"/>
       <c r="P3" s="92"/>
       <c r="Q3" s="92"/>
       <c r="R3" s="92"/>
-      <c r="S3" s="76"/>
-      <c r="V3" s="73"/>
-      <c r="W3" s="78"/>
+      <c r="S3" s="92"/>
+      <c r="T3" s="76"/>
+      <c r="W3" s="73"/>
+      <c r="X3" s="78"/>
     </row>
-    <row r="4" spans="2:23" s="77" customFormat="1" ht="24" customHeight="1" thickBot="1">
-      <c r="B4" s="242" t="str">
+    <row r="4" spans="2:24" s="77" customFormat="1" ht="24" customHeight="1" thickBot="1">
+      <c r="B4" s="220" t="str">
         <f>B1&amp;" : "&amp;C1&amp;"                                                           MFLCode : "&amp;E1&amp;"                                                    Reporting Month :   "&amp;G1&amp;"                                             Reporting Year: "&amp;I1</f>
         <v>Health Facility : Likii Dispensary                                                           MFLCode : 15035                                                    Reporting Month :   02                                             Reporting Year: 2020</v>
       </c>
-      <c r="C4" s="243"/>
-      <c r="D4" s="243"/>
-      <c r="E4" s="243"/>
-      <c r="F4" s="244"/>
+      <c r="C4" s="221"/>
+      <c r="D4" s="221"/>
+      <c r="E4" s="221"/>
+      <c r="F4" s="222"/>
       <c r="G4" s="93"/>
-      <c r="H4" s="261"/>
-      <c r="I4" s="262"/>
-      <c r="J4" s="263"/>
+      <c r="H4" s="231"/>
+      <c r="I4" s="232"/>
+      <c r="J4" s="233"/>
       <c r="K4" s="94"/>
       <c r="L4" s="94"/>
       <c r="M4" s="94"/>
       <c r="N4" s="94"/>
       <c r="O4" s="94"/>
-      <c r="P4" s="95" t="s">
+      <c r="P4" s="94"/>
+      <c r="Q4" s="95" t="s">
         <v>112</v>
       </c>
-      <c r="Q4" s="94" t="s">
+      <c r="R4" s="94" t="s">
         <v>113</v>
       </c>
-      <c r="R4" s="96" t="s">
+      <c r="S4" s="96" t="s">
         <v>114</v>
       </c>
-      <c r="S4" s="79"/>
-      <c r="V4" s="73">
+      <c r="T4" s="79"/>
+      <c r="W4" s="73">
         <v>2</v>
       </c>
-      <c r="W4" s="78"/>
+      <c r="X4" s="78"/>
     </row>
-    <row r="5" spans="2:23" s="81" customFormat="1" ht="30.75" customHeight="1" thickBot="1">
-      <c r="B5" s="248" t="s">
+    <row r="5" spans="2:24" s="81" customFormat="1" ht="30.75" customHeight="1" thickBot="1">
+      <c r="B5" s="226" t="s">
         <v>110</v>
       </c>
-      <c r="C5" s="249"/>
-      <c r="D5" s="239" t="s">
+      <c r="C5" s="227"/>
+      <c r="D5" s="217" t="s">
         <v>111</v>
       </c>
-      <c r="E5" s="240"/>
-      <c r="F5" s="241"/>
+      <c r="E5" s="218"/>
+      <c r="F5" s="219"/>
       <c r="G5" s="97"/>
-      <c r="H5" s="264"/>
-      <c r="I5" s="265"/>
-      <c r="J5" s="266"/>
+      <c r="H5" s="234"/>
+      <c r="I5" s="235"/>
+      <c r="J5" s="236"/>
       <c r="K5" s="97"/>
       <c r="L5" s="97"/>
       <c r="M5" s="97"/>
@@ -5641,33 +6122,34 @@
       <c r="P5" s="97"/>
       <c r="Q5" s="97"/>
       <c r="R5" s="97"/>
-      <c r="S5" s="83"/>
+      <c r="S5" s="97"/>
       <c r="T5" s="83"/>
       <c r="U5" s="83"/>
-      <c r="V5" s="73">
+      <c r="V5" s="83"/>
+      <c r="W5" s="73">
         <v>3</v>
       </c>
-      <c r="W5" s="80"/>
+      <c r="X5" s="80"/>
     </row>
-    <row r="6" spans="2:23" s="2" customFormat="1" ht="27.75" customHeight="1" thickBot="1">
-      <c r="B6" s="223" t="s">
+    <row r="6" spans="2:24" s="2" customFormat="1" ht="27.75" customHeight="1" thickBot="1">
+      <c r="B6" s="237" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="224"/>
+      <c r="C6" s="238"/>
       <c r="D6" s="98" t="s">
         <v>115</v>
       </c>
       <c r="E6" s="99">
-        <f>Q1</f>
+        <f>R1</f>
         <v>43497</v>
       </c>
-      <c r="F6" s="251"/>
-      <c r="G6" s="227"/>
-      <c r="H6" s="275" t="s">
+      <c r="F6" s="160"/>
+      <c r="G6" s="244"/>
+      <c r="H6" s="241" t="s">
         <v>86</v>
       </c>
-      <c r="I6" s="276"/>
-      <c r="J6" s="277"/>
+      <c r="I6" s="242"/>
+      <c r="J6" s="243"/>
       <c r="K6" s="100"/>
       <c r="L6" s="100"/>
       <c r="M6" s="100"/>
@@ -5676,1107 +6158,1179 @@
       <c r="P6" s="100"/>
       <c r="Q6" s="100"/>
       <c r="R6" s="100"/>
+      <c r="S6" s="100"/>
     </row>
-    <row r="7" spans="2:23" s="70" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
+    <row r="7" spans="2:24" s="70" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
       <c r="B7" s="101" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="103" t="s">
+      <c r="D7" s="259" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="104" t="s">
+      <c r="E7" s="260" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="105" t="s">
+      <c r="F7" s="261" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="227"/>
-      <c r="H7" s="282" t="s">
+      <c r="G7" s="244"/>
+      <c r="H7" s="168" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="283" t="s">
+      <c r="I7" s="169" t="s">
         <v>1</v>
       </c>
-      <c r="J7" s="281" t="s">
+      <c r="J7" s="167" t="s">
         <v>2</v>
       </c>
-      <c r="K7" s="109"/>
-      <c r="L7" s="274" t="s">
+      <c r="K7" s="106"/>
+      <c r="L7" s="285" t="s">
         <v>117</v>
       </c>
-      <c r="M7" s="109"/>
-      <c r="N7" s="109"/>
-      <c r="O7" s="109"/>
-      <c r="P7" s="109"/>
-      <c r="Q7" s="109"/>
-      <c r="R7" s="109"/>
+      <c r="M7" s="172" t="s">
+        <v>119</v>
+      </c>
+      <c r="N7" s="279" t="s">
+        <v>118</v>
+      </c>
+      <c r="O7" s="106"/>
+      <c r="P7" s="106"/>
+      <c r="Q7" s="106"/>
+      <c r="R7" s="106"/>
+      <c r="S7" s="106"/>
     </row>
-    <row r="8" spans="2:23" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B8" s="110">
+    <row r="8" spans="2:24" s="3" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B8" s="107">
         <v>1</v>
       </c>
-      <c r="C8" s="111" t="s">
+      <c r="C8" s="154" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="112"/>
-      <c r="E8" s="112"/>
-      <c r="F8" s="252">
+      <c r="D8" s="265"/>
+      <c r="E8" s="266"/>
+      <c r="F8" s="267">
         <f>IFERROR(D8/E8,)</f>
         <v>0</v>
       </c>
-      <c r="G8" s="227"/>
-      <c r="H8" s="278"/>
-      <c r="I8" s="279" t="s">
+      <c r="G8" s="244"/>
+      <c r="H8" s="164"/>
+      <c r="I8" s="165" t="s">
         <v>41</v>
       </c>
-      <c r="J8" s="280"/>
-      <c r="K8" s="116" t="str">
+      <c r="J8" s="166"/>
+      <c r="K8" s="111" t="str">
         <f>IF(D8&gt;E8,"*Numerator for "&amp;C8&amp;" Cannot be more than Denominator"&amp;CHAR(10),"")</f>
         <v/>
       </c>
-      <c r="L8" s="268" t="str">
+      <c r="L8" s="286" t="str">
         <f>CONCATENATE(K8,K9,K10,K11,K12,K13,K14,K15,K16,K17,K18,K19,K20,K21,K22,K23,K24)</f>
         <v/>
       </c>
-      <c r="M8" s="116"/>
-      <c r="N8" s="116"/>
-      <c r="O8" s="116"/>
-      <c r="P8" s="116"/>
-      <c r="Q8" s="116"/>
-      <c r="R8" s="116"/>
+      <c r="M8" s="170"/>
+      <c r="N8" s="276" t="str">
+        <f>CONCATENATE(M8,M9,M10,M11,M12,M13,M14,M15,M16,M17,M18,M19,M20,M21,M22,M23)</f>
+        <v/>
+      </c>
+      <c r="O8" s="173"/>
+      <c r="P8" s="111"/>
+      <c r="Q8" s="111"/>
+      <c r="R8" s="111"/>
+      <c r="S8" s="111"/>
     </row>
-    <row r="9" spans="2:23" s="4" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B9" s="110">
+    <row r="9" spans="2:24" s="4" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B9" s="107">
         <v>2</v>
       </c>
-      <c r="C9" s="111" t="s">
+      <c r="C9" s="154" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="175"/>
-      <c r="E9" s="185">
+      <c r="D9" s="268"/>
+      <c r="E9" s="253">
         <f>E8</f>
         <v>0</v>
       </c>
-      <c r="F9" s="252">
+      <c r="F9" s="269">
         <f t="shared" ref="F9:F23" si="0">IFERROR(D9/E9,)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="227"/>
-      <c r="H9" s="113"/>
-      <c r="I9" s="114" t="s">
+      <c r="G9" s="244"/>
+      <c r="H9" s="108"/>
+      <c r="I9" s="109" t="s">
         <v>41</v>
       </c>
-      <c r="J9" s="115"/>
-      <c r="K9" s="116" t="str">
+      <c r="J9" s="110"/>
+      <c r="K9" s="111" t="str">
         <f t="shared" ref="K9:K23" si="1">IF(D9&gt;E9,"*Numerator for "&amp;C9&amp;" Cannot be more than Denominator"&amp;CHAR(10),"")</f>
         <v/>
       </c>
-      <c r="L9" s="269"/>
-      <c r="M9" s="118"/>
-      <c r="N9" s="118"/>
-      <c r="O9" s="118"/>
-      <c r="P9" s="118"/>
-      <c r="Q9" s="118"/>
-      <c r="R9" s="118"/>
+      <c r="L9" s="287"/>
+      <c r="M9" s="170"/>
+      <c r="N9" s="277"/>
+      <c r="O9" s="174"/>
+      <c r="P9" s="112"/>
+      <c r="Q9" s="112"/>
+      <c r="R9" s="112"/>
+      <c r="S9" s="112"/>
     </row>
-    <row r="10" spans="2:23" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B10" s="110">
+    <row r="10" spans="2:24" s="3" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B10" s="107">
         <v>3</v>
       </c>
-      <c r="C10" s="173" t="s">
+      <c r="C10" s="154" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="284"/>
-      <c r="E10" s="286">
+      <c r="D10" s="268"/>
+      <c r="E10" s="253">
         <f>E8</f>
         <v>0</v>
       </c>
-      <c r="F10" s="285">
+      <c r="F10" s="269">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G10" s="227"/>
-      <c r="H10" s="119" t="s">
+      <c r="G10" s="244"/>
+      <c r="H10" s="113" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="114" t="s">
+      <c r="I10" s="109" t="s">
         <v>41</v>
       </c>
-      <c r="J10" s="115"/>
-      <c r="K10" s="116" t="str">
+      <c r="J10" s="110"/>
+      <c r="K10" s="111" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="L10" s="269"/>
-      <c r="M10" s="116"/>
-      <c r="N10" s="116"/>
-      <c r="O10" s="116"/>
-      <c r="P10" s="116"/>
-      <c r="Q10" s="116"/>
-      <c r="R10" s="116"/>
+      <c r="L10" s="287"/>
+      <c r="M10" s="170" t="str">
+        <f>IF(E10&gt;0,IF(D10/E10&lt;0.85,"*Early Testing Rate is below 85%"&amp;CHAR(10),""),"")</f>
+        <v/>
+      </c>
+      <c r="N10" s="277"/>
+      <c r="O10" s="173"/>
+      <c r="P10" s="111"/>
+      <c r="Q10" s="111"/>
+      <c r="R10" s="111"/>
+      <c r="S10" s="111"/>
     </row>
-    <row r="11" spans="2:23" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B11" s="110">
+    <row r="11" spans="2:24" s="3" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B11" s="107">
         <v>4</v>
       </c>
-      <c r="C11" s="111" t="s">
+      <c r="C11" s="154" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="147"/>
-      <c r="E11" s="182">
+      <c r="D11" s="268"/>
+      <c r="E11" s="253">
         <f>D10</f>
         <v>0</v>
       </c>
-      <c r="F11" s="252">
+      <c r="F11" s="269">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G11" s="227"/>
-      <c r="H11" s="113"/>
-      <c r="I11" s="120" t="s">
+      <c r="G11" s="244"/>
+      <c r="H11" s="108"/>
+      <c r="I11" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="J11" s="115"/>
-      <c r="K11" s="116" t="str">
+      <c r="J11" s="110"/>
+      <c r="K11" s="111" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="L11" s="269"/>
-      <c r="M11" s="116"/>
-      <c r="N11" s="116"/>
-      <c r="O11" s="116"/>
-      <c r="P11" s="116"/>
-      <c r="Q11" s="116"/>
-      <c r="R11" s="116"/>
+      <c r="L11" s="287"/>
+      <c r="M11" s="170"/>
+      <c r="N11" s="277"/>
+      <c r="O11" s="173"/>
+      <c r="P11" s="111"/>
+      <c r="Q11" s="111"/>
+      <c r="R11" s="111"/>
+      <c r="S11" s="111"/>
     </row>
-    <row r="12" spans="2:23" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B12" s="110">
+    <row r="12" spans="2:24" s="3" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B12" s="107">
         <v>5</v>
       </c>
-      <c r="C12" s="121" t="s">
+      <c r="C12" s="256" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="112"/>
-      <c r="E12" s="117">
+      <c r="D12" s="268"/>
+      <c r="E12" s="253">
         <f>E8</f>
         <v>0</v>
       </c>
-      <c r="F12" s="252">
+      <c r="F12" s="269">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G12" s="227"/>
-      <c r="H12" s="122" t="s">
+      <c r="G12" s="244"/>
+      <c r="H12" s="115" t="s">
         <v>91</v>
       </c>
-      <c r="I12" s="114" t="s">
+      <c r="I12" s="109" t="s">
         <v>41</v>
       </c>
-      <c r="J12" s="115"/>
-      <c r="K12" s="116" t="str">
+      <c r="J12" s="110"/>
+      <c r="K12" s="111" t="str">
         <f>IF(D12&gt;E12,"*Numerator for HEI tested with First DNA PCR at 6-8wks or at First contact and results available between 0 and 12 months Cannot be more than Denominator"&amp;CHAR(10)&amp;CHAR(10),"")</f>
         <v/>
       </c>
-      <c r="L12" s="269"/>
-      <c r="M12" s="116"/>
-      <c r="N12" s="116"/>
-      <c r="O12" s="116"/>
-      <c r="P12" s="116"/>
-      <c r="Q12" s="116"/>
-      <c r="R12" s="116"/>
+      <c r="L12" s="287"/>
+      <c r="M12" s="170" t="str">
+        <f>IF(E12&gt;0,IF(D12/E12&lt;0.95,"*Testing Rate is below 95%"&amp;CHAR(10),""),"")</f>
+        <v/>
+      </c>
+      <c r="N12" s="277"/>
+      <c r="O12" s="175"/>
+      <c r="P12" s="111"/>
+      <c r="Q12" s="111"/>
+      <c r="R12" s="111"/>
+      <c r="S12" s="111"/>
     </row>
-    <row r="13" spans="2:23" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B13" s="110">
+    <row r="13" spans="2:24" s="3" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B13" s="107">
         <v>6</v>
       </c>
-      <c r="C13" s="111" t="s">
+      <c r="C13" s="154" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="175"/>
-      <c r="E13" s="112"/>
-      <c r="F13" s="252">
+      <c r="D13" s="268"/>
+      <c r="E13" s="253">
+        <f>E8</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="269">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G13" s="227"/>
-      <c r="H13" s="123"/>
-      <c r="I13" s="124"/>
-      <c r="J13" s="115"/>
-      <c r="K13" s="116" t="str">
+      <c r="G13" s="244"/>
+      <c r="H13" s="116"/>
+      <c r="I13" s="117"/>
+      <c r="J13" s="110"/>
+      <c r="K13" s="111" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="L13" s="269"/>
-      <c r="M13" s="116"/>
-      <c r="N13" s="116"/>
-      <c r="O13" s="116"/>
-      <c r="P13" s="116"/>
-      <c r="Q13" s="116"/>
-      <c r="R13" s="116"/>
+      <c r="L13" s="287"/>
+      <c r="M13" s="170"/>
+      <c r="N13" s="277"/>
+      <c r="O13" s="173"/>
+      <c r="P13" s="111"/>
+      <c r="Q13" s="111"/>
+      <c r="R13" s="111"/>
+      <c r="S13" s="111"/>
     </row>
-    <row r="14" spans="2:23" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B14" s="110">
+    <row r="14" spans="2:24" s="3" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B14" s="107">
         <v>7</v>
       </c>
-      <c r="C14" s="173" t="s">
+      <c r="C14" s="154" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="176"/>
-      <c r="E14" s="174">
+      <c r="D14" s="268"/>
+      <c r="E14" s="253">
         <f>E8</f>
         <v>0</v>
       </c>
-      <c r="F14" s="252">
+      <c r="F14" s="269">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G14" s="227"/>
-      <c r="H14" s="125" t="s">
+      <c r="G14" s="244"/>
+      <c r="H14" s="118" t="s">
         <v>44</v>
       </c>
-      <c r="I14" s="114" t="s">
+      <c r="I14" s="109" t="s">
         <v>41</v>
       </c>
-      <c r="J14" s="115"/>
-      <c r="K14" s="116" t="str">
+      <c r="J14" s="110"/>
+      <c r="K14" s="111" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="L14" s="269"/>
-      <c r="M14" s="116"/>
-      <c r="N14" s="116"/>
-      <c r="O14" s="116"/>
-      <c r="P14" s="116"/>
-      <c r="Q14" s="116"/>
-      <c r="R14" s="116"/>
+      <c r="L14" s="287"/>
+      <c r="M14" s="170"/>
+      <c r="N14" s="277"/>
+      <c r="O14" s="173"/>
+      <c r="P14" s="111"/>
+      <c r="Q14" s="111"/>
+      <c r="R14" s="111"/>
+      <c r="S14" s="111"/>
     </row>
-    <row r="15" spans="2:23" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B15" s="110">
+    <row r="15" spans="2:24" s="3" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B15" s="107">
         <v>8</v>
       </c>
-      <c r="C15" s="111" t="s">
+      <c r="C15" s="154" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="147"/>
-      <c r="E15" s="112"/>
-      <c r="F15" s="252">
+      <c r="D15" s="268"/>
+      <c r="E15" s="253">
+        <f>E9</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="269">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G15" s="227"/>
-      <c r="H15" s="113"/>
-      <c r="I15" s="124"/>
-      <c r="J15" s="115"/>
-      <c r="K15" s="116" t="str">
+      <c r="G15" s="244"/>
+      <c r="H15" s="108"/>
+      <c r="I15" s="117"/>
+      <c r="J15" s="110"/>
+      <c r="K15" s="111" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="L15" s="269"/>
-      <c r="M15" s="116"/>
-      <c r="N15" s="116"/>
-      <c r="O15" s="116"/>
-      <c r="P15" s="116"/>
-      <c r="Q15" s="116"/>
-      <c r="R15" s="116"/>
+      <c r="L15" s="287"/>
+      <c r="M15" s="170" t="str">
+        <f>IF(E15&gt;0,IF(D15/E15&lt;0.85,"*Exclusive Breastfeeding Rate at 6 months is below 85%"&amp;CHAR(10),""),"")</f>
+        <v/>
+      </c>
+      <c r="N15" s="277"/>
+      <c r="O15" s="173"/>
+      <c r="P15" s="111"/>
+      <c r="Q15" s="111"/>
+      <c r="R15" s="111"/>
+      <c r="S15" s="111"/>
     </row>
-    <row r="16" spans="2:23" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B16" s="110">
+    <row r="16" spans="2:24" s="3" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B16" s="107">
         <v>9</v>
       </c>
-      <c r="C16" s="111" t="s">
+      <c r="C16" s="154" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="112"/>
-      <c r="E16" s="117">
+      <c r="D16" s="268"/>
+      <c r="E16" s="253">
         <f>D14</f>
         <v>0</v>
       </c>
-      <c r="F16" s="252">
+      <c r="F16" s="269">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G16" s="227"/>
-      <c r="H16" s="113"/>
-      <c r="I16" s="126" t="s">
+      <c r="G16" s="244"/>
+      <c r="H16" s="108"/>
+      <c r="I16" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="J16" s="115"/>
-      <c r="K16" s="116" t="str">
+      <c r="J16" s="110"/>
+      <c r="K16" s="111" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="L16" s="269"/>
-      <c r="M16" s="116"/>
-      <c r="N16" s="116"/>
-      <c r="O16" s="116"/>
-      <c r="P16" s="116"/>
-      <c r="Q16" s="116"/>
-      <c r="R16" s="116"/>
+      <c r="L16" s="287"/>
+      <c r="M16" s="170" t="str">
+        <f>IF(E16&gt;0,IF(D16/E16&lt;0.95,"*Linkage Rate amongest positive infants identified between 0 and 12 months is below 95%"&amp;CHAR(10),""),"")</f>
+        <v/>
+      </c>
+      <c r="N16" s="277"/>
+      <c r="O16" s="175"/>
+      <c r="P16" s="111"/>
+      <c r="Q16" s="111"/>
+      <c r="R16" s="111"/>
+      <c r="S16" s="111"/>
     </row>
-    <row r="17" spans="2:18" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B17" s="110">
+    <row r="17" spans="2:19" s="3" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B17" s="107">
         <v>10</v>
       </c>
-      <c r="C17" s="111" t="s">
+      <c r="C17" s="154" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="112"/>
-      <c r="E17" s="117">
+      <c r="D17" s="268"/>
+      <c r="E17" s="253">
         <f>D14</f>
         <v>0</v>
       </c>
-      <c r="F17" s="252">
+      <c r="F17" s="269">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G17" s="227"/>
-      <c r="H17" s="113"/>
-      <c r="I17" s="126" t="s">
+      <c r="G17" s="244"/>
+      <c r="H17" s="108"/>
+      <c r="I17" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="J17" s="115"/>
-      <c r="K17" s="116" t="str">
+      <c r="J17" s="110"/>
+      <c r="K17" s="111" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="L17" s="269"/>
-      <c r="M17" s="116"/>
-      <c r="N17" s="116"/>
-      <c r="O17" s="116"/>
-      <c r="P17" s="116"/>
-      <c r="Q17" s="116"/>
-      <c r="R17" s="116"/>
+      <c r="L17" s="287"/>
+      <c r="M17" s="170"/>
+      <c r="N17" s="277"/>
+      <c r="O17" s="173"/>
+      <c r="P17" s="111"/>
+      <c r="Q17" s="111"/>
+      <c r="R17" s="111"/>
+      <c r="S17" s="111"/>
     </row>
-    <row r="18" spans="2:18" ht="18.75" customHeight="1">
-      <c r="B18" s="167">
+    <row r="18" spans="2:19" ht="18.75" customHeight="1">
+      <c r="B18" s="150">
         <v>11</v>
       </c>
-      <c r="C18" s="168" t="s">
+      <c r="C18" s="257" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="169"/>
-      <c r="E18" s="169"/>
-      <c r="F18" s="253"/>
-      <c r="G18" s="227"/>
-      <c r="H18" s="127"/>
-      <c r="I18" s="128"/>
-      <c r="J18" s="129"/>
-      <c r="K18" s="116" t="str">
+      <c r="D18" s="270"/>
+      <c r="E18" s="264"/>
+      <c r="F18" s="271"/>
+      <c r="G18" s="244"/>
+      <c r="H18" s="120"/>
+      <c r="I18" s="121"/>
+      <c r="J18" s="122"/>
+      <c r="K18" s="111" t="str">
         <f>IF(D12&lt;E11,"*Numerator for "&amp;C12&amp;" Cannot be less than Denominator for "&amp;C11&amp;CHAR(10)&amp;CHAR(10),"")</f>
         <v/>
       </c>
-      <c r="L18" s="269"/>
-      <c r="M18" s="130"/>
-      <c r="N18" s="130"/>
-      <c r="O18" s="130"/>
-      <c r="P18" s="130"/>
-      <c r="Q18" s="130"/>
-      <c r="R18" s="130"/>
+      <c r="L18" s="287"/>
+      <c r="M18" s="170"/>
+      <c r="N18" s="277"/>
+      <c r="O18" s="176"/>
+      <c r="P18" s="123"/>
+      <c r="Q18" s="123"/>
+      <c r="R18" s="123"/>
+      <c r="S18" s="123"/>
     </row>
-    <row r="19" spans="2:18" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B19" s="110">
+    <row r="19" spans="2:19" s="3" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B19" s="107">
         <v>11.1</v>
       </c>
-      <c r="C19" s="111" t="s">
+      <c r="C19" s="154" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="112"/>
-      <c r="E19" s="117">
+      <c r="D19" s="268"/>
+      <c r="E19" s="253">
         <f>E8</f>
         <v>0</v>
       </c>
-      <c r="F19" s="252">
+      <c r="F19" s="269">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G19" s="227"/>
-      <c r="H19" s="113"/>
-      <c r="I19" s="114" t="s">
+      <c r="G19" s="244"/>
+      <c r="H19" s="108"/>
+      <c r="I19" s="109" t="s">
         <v>41</v>
       </c>
-      <c r="J19" s="131"/>
-      <c r="K19" s="116" t="str">
+      <c r="J19" s="124"/>
+      <c r="K19" s="111" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="L19" s="269"/>
-      <c r="M19" s="116"/>
-      <c r="N19" s="116"/>
-      <c r="O19" s="116"/>
-      <c r="P19" s="116"/>
-      <c r="Q19" s="116"/>
-      <c r="R19" s="116"/>
+      <c r="L19" s="287"/>
+      <c r="M19" s="170"/>
+      <c r="N19" s="277"/>
+      <c r="O19" s="173"/>
+      <c r="P19" s="111"/>
+      <c r="Q19" s="111"/>
+      <c r="R19" s="111"/>
+      <c r="S19" s="111"/>
     </row>
-    <row r="20" spans="2:18" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B20" s="110">
+    <row r="20" spans="2:19" s="3" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B20" s="107">
         <v>11.2</v>
       </c>
-      <c r="C20" s="111" t="s">
+      <c r="C20" s="154" t="s">
         <v>87</v>
       </c>
-      <c r="D20" s="117">
+      <c r="D20" s="272">
         <f>D14</f>
         <v>0</v>
       </c>
-      <c r="E20" s="117">
+      <c r="E20" s="253">
         <f>E8</f>
         <v>0</v>
       </c>
-      <c r="F20" s="252">
+      <c r="F20" s="269">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G20" s="227"/>
-      <c r="H20" s="125" t="s">
+      <c r="G20" s="244"/>
+      <c r="H20" s="118" t="s">
         <v>44</v>
       </c>
-      <c r="I20" s="114" t="s">
+      <c r="I20" s="109" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="131"/>
-      <c r="K20" s="116" t="str">
+      <c r="J20" s="124"/>
+      <c r="K20" s="111" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="L20" s="269"/>
-      <c r="M20" s="116"/>
-      <c r="N20" s="116"/>
-      <c r="O20" s="116"/>
-      <c r="P20" s="116"/>
-      <c r="Q20" s="116"/>
-      <c r="R20" s="116"/>
+      <c r="L20" s="287"/>
+      <c r="M20" s="170" t="str">
+        <f>IF(E20&gt;0,IF(D20/E20&gt;0.05,"*EID Mother To Child Transmission rate is above 5%"&amp;CHAR(10),""),"")</f>
+        <v/>
+      </c>
+      <c r="N20" s="277"/>
+      <c r="O20" s="173"/>
+      <c r="P20" s="111"/>
+      <c r="Q20" s="111"/>
+      <c r="R20" s="111"/>
+      <c r="S20" s="111"/>
     </row>
-    <row r="21" spans="2:18" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B21" s="110">
+    <row r="21" spans="2:19" s="3" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B21" s="107">
         <v>11.3</v>
       </c>
-      <c r="C21" s="111" t="s">
+      <c r="C21" s="154" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="112"/>
-      <c r="E21" s="117">
+      <c r="D21" s="268"/>
+      <c r="E21" s="253">
         <f>E8</f>
         <v>0</v>
       </c>
-      <c r="F21" s="252">
+      <c r="F21" s="269">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G21" s="227"/>
-      <c r="H21" s="113"/>
-      <c r="I21" s="114" t="s">
+      <c r="G21" s="244"/>
+      <c r="H21" s="108"/>
+      <c r="I21" s="109" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="131"/>
-      <c r="K21" s="116" t="str">
+      <c r="J21" s="124"/>
+      <c r="K21" s="111" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="L21" s="269"/>
-      <c r="M21" s="116"/>
-      <c r="N21" s="116"/>
-      <c r="O21" s="116"/>
-      <c r="P21" s="116"/>
-      <c r="Q21" s="116"/>
-      <c r="R21" s="116"/>
+      <c r="L21" s="287"/>
+      <c r="M21" s="170"/>
+      <c r="N21" s="277"/>
+      <c r="O21" s="173"/>
+      <c r="P21" s="111"/>
+      <c r="Q21" s="111"/>
+      <c r="R21" s="111"/>
+      <c r="S21" s="111"/>
     </row>
-    <row r="22" spans="2:18" s="3" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B22" s="110">
+    <row r="22" spans="2:19" s="3" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B22" s="107">
         <v>11.4</v>
       </c>
-      <c r="C22" s="111" t="s">
+      <c r="C22" s="154" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="112"/>
-      <c r="E22" s="117">
+      <c r="D22" s="268"/>
+      <c r="E22" s="253">
         <f>E8</f>
         <v>0</v>
       </c>
-      <c r="F22" s="252">
+      <c r="F22" s="269">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G22" s="227"/>
-      <c r="H22" s="113"/>
-      <c r="I22" s="114" t="s">
+      <c r="G22" s="244"/>
+      <c r="H22" s="108"/>
+      <c r="I22" s="109" t="s">
         <v>41</v>
       </c>
-      <c r="J22" s="131"/>
-      <c r="K22" s="116" t="str">
+      <c r="J22" s="124"/>
+      <c r="K22" s="111" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="L22" s="269"/>
-      <c r="M22" s="116"/>
-      <c r="N22" s="116"/>
-      <c r="O22" s="116"/>
-      <c r="P22" s="116"/>
-      <c r="Q22" s="116"/>
-      <c r="R22" s="116"/>
+      <c r="L22" s="287"/>
+      <c r="M22" s="170"/>
+      <c r="N22" s="277"/>
+      <c r="O22" s="173"/>
+      <c r="P22" s="111"/>
+      <c r="Q22" s="111"/>
+      <c r="R22" s="111"/>
+      <c r="S22" s="111"/>
     </row>
-    <row r="23" spans="2:18" s="3" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B23" s="183">
+    <row r="23" spans="2:19" s="3" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
+      <c r="B23" s="157">
         <v>11.5</v>
       </c>
-      <c r="C23" s="184" t="s">
+      <c r="C23" s="258" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="175"/>
-      <c r="E23" s="185">
+      <c r="D23" s="273"/>
+      <c r="E23" s="274">
         <f>E8</f>
         <v>0</v>
       </c>
-      <c r="F23" s="254">
+      <c r="F23" s="275">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="227"/>
-      <c r="H23" s="136"/>
-      <c r="I23" s="137" t="s">
+      <c r="G23" s="244"/>
+      <c r="H23" s="126"/>
+      <c r="I23" s="127" t="s">
         <v>41</v>
       </c>
-      <c r="J23" s="138"/>
-      <c r="K23" s="116" t="str">
+      <c r="J23" s="128"/>
+      <c r="K23" s="111" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="L23" s="270"/>
-      <c r="M23" s="116"/>
-      <c r="N23" s="116"/>
-      <c r="O23" s="116"/>
-      <c r="P23" s="116"/>
-      <c r="Q23" s="116"/>
-      <c r="R23" s="116"/>
+      <c r="L23" s="288"/>
+      <c r="M23" s="170"/>
+      <c r="N23" s="278"/>
+      <c r="O23" s="173"/>
+      <c r="P23" s="111"/>
+      <c r="Q23" s="111"/>
+      <c r="R23" s="111"/>
+      <c r="S23" s="111"/>
     </row>
-    <row r="24" spans="2:18" ht="16.5" customHeight="1">
-      <c r="B24" s="228" t="s">
+    <row r="24" spans="2:19" ht="16.5" customHeight="1">
+      <c r="B24" s="245" t="s">
         <v>80</v>
       </c>
-      <c r="C24" s="229"/>
-      <c r="D24" s="229"/>
-      <c r="E24" s="229"/>
-      <c r="F24" s="230"/>
-      <c r="G24" s="227"/>
-      <c r="H24" s="234"/>
-      <c r="I24" s="234"/>
-      <c r="J24" s="234"/>
-      <c r="K24" s="130" t="str">
+      <c r="C24" s="246"/>
+      <c r="D24" s="262"/>
+      <c r="E24" s="262"/>
+      <c r="F24" s="263"/>
+      <c r="G24" s="244"/>
+      <c r="H24" s="250"/>
+      <c r="I24" s="250"/>
+      <c r="J24" s="250"/>
+      <c r="K24" s="123" t="str">
         <f>IF(SUM(D19:D23)&lt;&gt;E19,"* Sum of Numerator  11.1,11.2,11.3,11.4 and 11.5 should be equal to Denominator for 11.1","")</f>
         <v/>
       </c>
-      <c r="L24" s="130"/>
-      <c r="M24" s="130"/>
-      <c r="N24" s="130"/>
-      <c r="O24" s="130"/>
-      <c r="P24" s="130"/>
-      <c r="Q24" s="130"/>
-      <c r="R24" s="130"/>
+      <c r="L24" s="123"/>
+      <c r="M24" s="123"/>
+      <c r="N24" s="123"/>
+      <c r="O24" s="176"/>
+      <c r="P24" s="123"/>
+      <c r="Q24" s="123"/>
+      <c r="R24" s="123"/>
+      <c r="S24" s="123"/>
     </row>
-    <row r="25" spans="2:18" ht="9.75" customHeight="1" thickBot="1">
-      <c r="B25" s="231"/>
-      <c r="C25" s="232"/>
-      <c r="D25" s="232"/>
-      <c r="E25" s="232"/>
-      <c r="F25" s="233"/>
-      <c r="G25" s="227"/>
-      <c r="H25" s="234"/>
-      <c r="I25" s="234"/>
-      <c r="J25" s="234"/>
-      <c r="K25" s="130"/>
-      <c r="L25" s="130"/>
-      <c r="M25" s="130"/>
-      <c r="N25" s="130"/>
-      <c r="O25" s="130"/>
-      <c r="P25" s="130"/>
-      <c r="Q25" s="130"/>
-      <c r="R25" s="130"/>
+    <row r="25" spans="2:19" ht="9.75" customHeight="1" thickBot="1">
+      <c r="B25" s="247"/>
+      <c r="C25" s="248"/>
+      <c r="D25" s="248"/>
+      <c r="E25" s="248"/>
+      <c r="F25" s="249"/>
+      <c r="G25" s="244"/>
+      <c r="H25" s="250"/>
+      <c r="I25" s="250"/>
+      <c r="J25" s="250"/>
+      <c r="K25" s="123"/>
+      <c r="L25" s="123"/>
+      <c r="M25" s="123"/>
+      <c r="N25" s="123"/>
+      <c r="O25" s="176"/>
+      <c r="P25" s="123"/>
+      <c r="Q25" s="123"/>
+      <c r="R25" s="123"/>
+      <c r="S25" s="123"/>
     </row>
-    <row r="26" spans="2:18" s="5" customFormat="1" ht="32.25" customHeight="1" thickBot="1">
-      <c r="B26" s="225" t="s">
+    <row r="26" spans="2:19" s="5" customFormat="1" ht="32.25" customHeight="1" thickBot="1">
+      <c r="B26" s="239" t="s">
         <v>90</v>
       </c>
-      <c r="C26" s="226"/>
-      <c r="D26" s="139" t="s">
+      <c r="C26" s="240"/>
+      <c r="D26" s="129" t="s">
         <v>115</v>
       </c>
-      <c r="E26" s="140">
-        <f>R1</f>
+      <c r="E26" s="130">
+        <f>S1</f>
         <v>43132</v>
       </c>
-      <c r="F26" s="255"/>
-      <c r="G26" s="227"/>
-      <c r="H26" s="219" t="s">
+      <c r="F26" s="161"/>
+      <c r="G26" s="244"/>
+      <c r="H26" s="210" t="s">
         <v>86</v>
       </c>
-      <c r="I26" s="220"/>
-      <c r="J26" s="221"/>
-      <c r="K26" s="141"/>
-      <c r="L26" s="271" t="str">
+      <c r="I26" s="211"/>
+      <c r="J26" s="212"/>
+      <c r="K26" s="131"/>
+      <c r="L26" s="281" t="str">
         <f>CONCATENATE(K28,K29,K30,K31,K32,K33,K34,K35,K36,K37,K38,K39)</f>
         <v/>
       </c>
-      <c r="M26" s="141"/>
-      <c r="N26" s="141"/>
-      <c r="O26" s="141"/>
-      <c r="P26" s="141"/>
-      <c r="Q26" s="141"/>
-      <c r="R26" s="141"/>
+      <c r="M26" s="171"/>
+      <c r="N26" s="281" t="str">
+        <f>CONCATENATE(M28,M29,M30,M31,M32,M33,M34,M35,M36,M37,M38,M39,M40)</f>
+        <v/>
+      </c>
+      <c r="O26" s="176"/>
+      <c r="P26" s="131"/>
+      <c r="Q26" s="131"/>
+      <c r="R26" s="131"/>
+      <c r="S26" s="131"/>
     </row>
-    <row r="27" spans="2:18" s="70" customFormat="1" ht="22.9" customHeight="1" thickBot="1">
-      <c r="B27" s="142" t="s">
+    <row r="27" spans="2:19" s="70" customFormat="1" ht="22.9" customHeight="1" thickBot="1">
+      <c r="B27" s="132" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="143" t="s">
+      <c r="C27" s="133" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="179" t="s">
+      <c r="D27" s="156" t="s">
         <v>19</v>
       </c>
-      <c r="E27" s="144" t="s">
+      <c r="E27" s="156" t="s">
         <v>20</v>
       </c>
-      <c r="F27" s="145" t="s">
+      <c r="F27" s="255" t="s">
         <v>2</v>
       </c>
-      <c r="G27" s="227"/>
-      <c r="H27" s="106" t="s">
+      <c r="G27" s="244"/>
+      <c r="H27" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="I27" s="107" t="s">
+      <c r="I27" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="J27" s="108" t="s">
+      <c r="J27" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="K27" s="109"/>
-      <c r="L27" s="272"/>
-      <c r="M27" s="109"/>
-      <c r="N27" s="109"/>
-      <c r="O27" s="109"/>
-      <c r="P27" s="109"/>
-      <c r="Q27" s="109"/>
-      <c r="R27" s="109"/>
+      <c r="K27" s="106"/>
+      <c r="L27" s="282"/>
+      <c r="M27" s="171"/>
+      <c r="N27" s="282"/>
+      <c r="O27" s="175"/>
+      <c r="P27" s="106"/>
+      <c r="Q27" s="106"/>
+      <c r="R27" s="106"/>
+      <c r="S27" s="106"/>
     </row>
-    <row r="28" spans="2:18" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B28" s="146">
+    <row r="28" spans="2:19" s="11" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B28" s="134">
         <v>12</v>
       </c>
-      <c r="C28" s="177" t="s">
+      <c r="C28" s="155" t="s">
         <v>92</v>
       </c>
-      <c r="D28" s="176"/>
-      <c r="E28" s="178"/>
-      <c r="F28" s="252">
+      <c r="D28" s="265"/>
+      <c r="E28" s="266"/>
+      <c r="F28" s="267">
         <f t="shared" ref="F28:F39" si="2">IFERROR(D28/E28,)</f>
         <v>0</v>
       </c>
-      <c r="G28" s="227"/>
-      <c r="H28" s="113" t="s">
+      <c r="G28" s="244"/>
+      <c r="H28" s="108" t="s">
         <v>46</v>
       </c>
-      <c r="I28" s="148"/>
-      <c r="J28" s="131"/>
-      <c r="K28" s="116" t="str">
+      <c r="I28" s="135"/>
+      <c r="J28" s="124"/>
+      <c r="K28" s="111" t="str">
         <f>IF(D28&gt;E28,"*Numerator for "&amp;C28&amp;" Cannot be more than Denominator"&amp;CHAR(10),"")</f>
         <v/>
       </c>
-      <c r="L28" s="272"/>
-      <c r="M28" s="149"/>
-      <c r="N28" s="149"/>
-      <c r="O28" s="149"/>
-      <c r="P28" s="149"/>
-      <c r="Q28" s="149"/>
-      <c r="R28" s="149"/>
+      <c r="L28" s="282"/>
+      <c r="M28" s="171"/>
+      <c r="N28" s="282"/>
+      <c r="O28" s="175"/>
+      <c r="P28" s="136"/>
+      <c r="Q28" s="136"/>
+      <c r="R28" s="136"/>
+      <c r="S28" s="136"/>
     </row>
-    <row r="29" spans="2:18" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B29" s="110">
+    <row r="29" spans="2:19" s="11" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B29" s="107">
         <v>13</v>
       </c>
-      <c r="C29" s="150" t="s">
+      <c r="C29" s="254" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="147"/>
-      <c r="E29" s="117">
+      <c r="D29" s="268"/>
+      <c r="E29" s="253">
         <f>D28</f>
         <v>0</v>
       </c>
-      <c r="F29" s="252">
+      <c r="F29" s="269">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G29" s="227"/>
-      <c r="H29" s="113"/>
-      <c r="I29" s="148" t="s">
+      <c r="G29" s="244"/>
+      <c r="H29" s="108" t="s">
+        <v>120</v>
+      </c>
+      <c r="I29" s="135" t="s">
         <v>46</v>
       </c>
-      <c r="J29" s="131"/>
-      <c r="K29" s="116" t="str">
+      <c r="J29" s="124"/>
+      <c r="K29" s="111" t="str">
         <f t="shared" ref="K29:K32" si="3">IF(D29&gt;E29,"*Numerator for "&amp;C29&amp;" Cannot be more than Denominator"&amp;CHAR(10),"")</f>
         <v/>
       </c>
-      <c r="L29" s="272"/>
-      <c r="M29" s="149"/>
-      <c r="N29" s="149"/>
-      <c r="O29" s="149"/>
-      <c r="P29" s="149"/>
-      <c r="Q29" s="149"/>
-      <c r="R29" s="149"/>
+      <c r="L29" s="282"/>
+      <c r="M29" s="171"/>
+      <c r="N29" s="282"/>
+      <c r="O29" s="175"/>
+      <c r="P29" s="136"/>
+      <c r="Q29" s="136"/>
+      <c r="R29" s="136"/>
+      <c r="S29" s="136"/>
     </row>
-    <row r="30" spans="2:18" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B30" s="110">
+    <row r="30" spans="2:19" s="11" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B30" s="107">
         <v>14</v>
       </c>
-      <c r="C30" s="150" t="s">
+      <c r="C30" s="254" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="112"/>
-      <c r="E30" s="112"/>
-      <c r="F30" s="252">
+      <c r="D30" s="268"/>
+      <c r="E30" s="253">
+        <f>D29</f>
+        <v>0</v>
+      </c>
+      <c r="F30" s="269">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G30" s="227"/>
-      <c r="H30" s="113"/>
-      <c r="I30" s="148"/>
-      <c r="J30" s="131"/>
-      <c r="K30" s="116" t="str">
+      <c r="G30" s="244"/>
+      <c r="H30" s="108"/>
+      <c r="I30" s="135" t="s">
+        <v>120</v>
+      </c>
+      <c r="J30" s="124"/>
+      <c r="K30" s="111" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L30" s="272"/>
-      <c r="M30" s="149"/>
-      <c r="N30" s="149"/>
-      <c r="O30" s="149"/>
-      <c r="P30" s="149"/>
-      <c r="Q30" s="149"/>
-      <c r="R30" s="149"/>
+      <c r="L30" s="282"/>
+      <c r="M30" s="171"/>
+      <c r="N30" s="282"/>
+      <c r="O30" s="175"/>
+      <c r="P30" s="136"/>
+      <c r="Q30" s="136"/>
+      <c r="R30" s="136"/>
+      <c r="S30" s="136"/>
     </row>
-    <row r="31" spans="2:18" s="11" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B31" s="110">
+    <row r="31" spans="2:19" s="11" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B31" s="107">
         <v>15</v>
       </c>
-      <c r="C31" s="150" t="s">
+      <c r="C31" s="254" t="s">
         <v>88</v>
       </c>
-      <c r="D31" s="112"/>
-      <c r="E31" s="175"/>
-      <c r="F31" s="252">
+      <c r="D31" s="268"/>
+      <c r="E31" s="253">
+        <f>E28</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="269">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G31" s="227"/>
-      <c r="H31" s="151"/>
-      <c r="I31" s="152"/>
-      <c r="J31" s="131"/>
-      <c r="K31" s="116" t="str">
+      <c r="G31" s="244"/>
+      <c r="H31" s="137"/>
+      <c r="I31" s="138"/>
+      <c r="J31" s="124"/>
+      <c r="K31" s="111" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L31" s="272"/>
-      <c r="M31" s="149"/>
-      <c r="N31" s="149"/>
-      <c r="O31" s="149"/>
-      <c r="P31" s="149"/>
-      <c r="Q31" s="149"/>
-      <c r="R31" s="149"/>
+      <c r="L31" s="282"/>
+      <c r="M31" s="171"/>
+      <c r="N31" s="282"/>
+      <c r="O31" s="175"/>
+      <c r="P31" s="136"/>
+      <c r="Q31" s="136"/>
+      <c r="R31" s="136"/>
+      <c r="S31" s="136"/>
     </row>
-    <row r="32" spans="2:18" s="12" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B32" s="110">
+    <row r="32" spans="2:19" s="12" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
+      <c r="B32" s="157">
         <v>16</v>
       </c>
-      <c r="C32" s="150" t="s">
+      <c r="C32" s="289" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="180"/>
-      <c r="E32" s="176"/>
-      <c r="F32" s="252">
+      <c r="D32" s="290"/>
+      <c r="E32" s="291"/>
+      <c r="F32" s="292">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G32" s="227"/>
-      <c r="H32" s="113"/>
-      <c r="I32" s="148" t="s">
+      <c r="G32" s="244"/>
+      <c r="H32" s="108"/>
+      <c r="I32" s="135" t="s">
         <v>47</v>
       </c>
-      <c r="J32" s="131"/>
-      <c r="K32" s="116" t="str">
+      <c r="J32" s="124"/>
+      <c r="K32" s="111" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="L32" s="272"/>
-      <c r="M32" s="153"/>
-      <c r="N32" s="153"/>
-      <c r="O32" s="153"/>
-      <c r="P32" s="153"/>
-      <c r="Q32" s="153"/>
-      <c r="R32" s="153"/>
+      <c r="L32" s="282"/>
+      <c r="M32" s="284" t="str">
+        <f>IF(E32&gt;0,IF(D32/E32&lt;0.95,"*Linkage Rate amongest positive infants identified is below 95%"&amp;CHAR(10),""),"")</f>
+        <v/>
+      </c>
+      <c r="N32" s="282"/>
+      <c r="O32" s="175"/>
+      <c r="P32" s="139"/>
+      <c r="Q32" s="139"/>
+      <c r="R32" s="139"/>
+      <c r="S32" s="139"/>
     </row>
-    <row r="33" spans="2:18" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="B33" s="154">
+    <row r="33" spans="2:19" s="5" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="B33" s="297">
         <v>17</v>
       </c>
-      <c r="C33" s="155" t="s">
+      <c r="C33" s="298" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="156"/>
-      <c r="E33" s="181"/>
-      <c r="F33" s="256"/>
-      <c r="G33" s="227"/>
-      <c r="H33" s="157"/>
-      <c r="I33" s="158"/>
-      <c r="J33" s="159"/>
-      <c r="K33" s="141"/>
-      <c r="L33" s="272"/>
-      <c r="M33" s="141"/>
-      <c r="N33" s="141"/>
-      <c r="O33" s="141"/>
-      <c r="P33" s="141"/>
-      <c r="Q33" s="141"/>
-      <c r="R33" s="141"/>
+      <c r="D33" s="299"/>
+      <c r="E33" s="300"/>
+      <c r="F33" s="301"/>
+      <c r="G33" s="244"/>
+      <c r="H33" s="140"/>
+      <c r="I33" s="141"/>
+      <c r="J33" s="142"/>
+      <c r="K33" s="131"/>
+      <c r="L33" s="282"/>
+      <c r="M33" s="171"/>
+      <c r="N33" s="282"/>
+      <c r="O33" s="176"/>
+      <c r="P33" s="131"/>
+      <c r="Q33" s="131"/>
+      <c r="R33" s="131"/>
+      <c r="S33" s="131"/>
     </row>
-    <row r="34" spans="2:18" s="6" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B34" s="110">
+    <row r="34" spans="2:19" s="6" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B34" s="134">
         <v>17.100000000000001</v>
       </c>
-      <c r="C34" s="111" t="s">
+      <c r="C34" s="293" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="180"/>
-      <c r="E34" s="176"/>
-      <c r="F34" s="252">
+      <c r="D34" s="294"/>
+      <c r="E34" s="295"/>
+      <c r="F34" s="296">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G34" s="227"/>
-      <c r="H34" s="160"/>
-      <c r="I34" s="161" t="s">
+      <c r="G34" s="244"/>
+      <c r="H34" s="143"/>
+      <c r="I34" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="J34" s="131"/>
-      <c r="K34" s="267" t="str">
+      <c r="J34" s="124"/>
+      <c r="K34" s="163" t="str">
         <f>IF(SUM(D34:D39)&lt;&gt;E34,"*Sum of Numerator  17.1,17.2,17.3,17.4,17.5 and 17.6 should be equal to Denominator for 17.1","")</f>
         <v/>
       </c>
-      <c r="L34" s="272"/>
-      <c r="M34" s="162"/>
-      <c r="N34" s="162"/>
-      <c r="O34" s="162"/>
-      <c r="P34" s="162"/>
-      <c r="Q34" s="162"/>
-      <c r="R34" s="162"/>
+      <c r="L34" s="282"/>
+      <c r="M34" s="171"/>
+      <c r="N34" s="282"/>
+      <c r="O34" s="173"/>
+      <c r="P34" s="145"/>
+      <c r="Q34" s="145"/>
+      <c r="R34" s="145"/>
+      <c r="S34" s="145"/>
     </row>
-    <row r="35" spans="2:18" s="6" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B35" s="110">
+    <row r="35" spans="2:19" s="6" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B35" s="107">
         <v>17.2</v>
       </c>
-      <c r="C35" s="111" t="s">
+      <c r="C35" s="154" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="112"/>
-      <c r="E35" s="182">
+      <c r="D35" s="268"/>
+      <c r="E35" s="253">
         <f>E34</f>
         <v>0</v>
       </c>
-      <c r="F35" s="252">
+      <c r="F35" s="269">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G35" s="227"/>
-      <c r="H35" s="163"/>
-      <c r="I35" s="161" t="s">
+      <c r="G35" s="244"/>
+      <c r="H35" s="146"/>
+      <c r="I35" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="J35" s="131"/>
-      <c r="K35" s="116" t="str">
+      <c r="J35" s="124"/>
+      <c r="K35" s="111" t="str">
         <f>IF(D35&gt;E35,"*Numerator for "&amp;C35&amp;" Cannot be more than Denominator"&amp;CHAR(10),"")</f>
         <v/>
       </c>
-      <c r="L35" s="272"/>
-      <c r="M35" s="162"/>
-      <c r="N35" s="162"/>
-      <c r="O35" s="162"/>
-      <c r="P35" s="162"/>
-      <c r="Q35" s="162"/>
-      <c r="R35" s="162"/>
+      <c r="L35" s="282"/>
+      <c r="M35" s="171"/>
+      <c r="N35" s="282"/>
+      <c r="O35" s="173"/>
+      <c r="P35" s="145"/>
+      <c r="Q35" s="145"/>
+      <c r="R35" s="145"/>
+      <c r="S35" s="145"/>
     </row>
-    <row r="36" spans="2:18" s="6" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B36" s="110">
+    <row r="36" spans="2:19" s="6" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B36" s="107">
         <v>17.3</v>
       </c>
-      <c r="C36" s="111" t="s">
+      <c r="C36" s="154" t="s">
         <v>26</v>
       </c>
-      <c r="D36" s="117">
+      <c r="D36" s="272">
         <f>E32</f>
         <v>0</v>
       </c>
-      <c r="E36" s="117">
+      <c r="E36" s="253">
         <f t="shared" ref="E36:E39" si="4">E35</f>
         <v>0</v>
       </c>
-      <c r="F36" s="252">
+      <c r="F36" s="269">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G36" s="227"/>
-      <c r="H36" s="164" t="s">
+      <c r="G36" s="244"/>
+      <c r="H36" s="147" t="s">
         <v>47</v>
       </c>
-      <c r="I36" s="161" t="s">
+      <c r="I36" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="J36" s="131"/>
-      <c r="K36" s="116" t="str">
+      <c r="J36" s="124"/>
+      <c r="K36" s="111" t="str">
         <f t="shared" ref="K36:K39" si="5">IF(D36&gt;E36,"*Numerator for "&amp;C36&amp;" Cannot be more than Denominator"&amp;CHAR(10),"")</f>
         <v/>
       </c>
-      <c r="L36" s="272"/>
-      <c r="M36" s="162"/>
-      <c r="N36" s="162"/>
-      <c r="O36" s="162"/>
-      <c r="P36" s="162"/>
-      <c r="Q36" s="162"/>
-      <c r="R36" s="162"/>
+      <c r="L36" s="282"/>
+      <c r="M36" s="284" t="str">
+        <f>IF(E36&gt;0,IF(D36/E36&gt;0.05,"*EID Mother To Child Transmission rate is above 5%"&amp;CHAR(10),""),"")</f>
+        <v/>
+      </c>
+      <c r="N36" s="282"/>
+      <c r="O36" s="173"/>
+      <c r="P36" s="145"/>
+      <c r="Q36" s="145"/>
+      <c r="R36" s="145"/>
+      <c r="S36" s="145"/>
     </row>
-    <row r="37" spans="2:18" s="6" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B37" s="110">
+    <row r="37" spans="2:19" s="6" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B37" s="107">
         <v>17.399999999999999</v>
       </c>
-      <c r="C37" s="111" t="s">
+      <c r="C37" s="154" t="s">
         <v>27</v>
       </c>
-      <c r="D37" s="112"/>
-      <c r="E37" s="117">
+      <c r="D37" s="268"/>
+      <c r="E37" s="253">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F37" s="252">
+      <c r="F37" s="269">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G37" s="227"/>
-      <c r="H37" s="113"/>
-      <c r="I37" s="161" t="s">
+      <c r="G37" s="244"/>
+      <c r="H37" s="108"/>
+      <c r="I37" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="J37" s="131"/>
-      <c r="K37" s="116" t="str">
+      <c r="J37" s="124"/>
+      <c r="K37" s="111" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="L37" s="272"/>
-      <c r="M37" s="162"/>
-      <c r="N37" s="162"/>
-      <c r="O37" s="162"/>
-      <c r="P37" s="162"/>
-      <c r="Q37" s="162"/>
-      <c r="R37" s="162"/>
+      <c r="L37" s="282"/>
+      <c r="M37" s="171"/>
+      <c r="N37" s="282"/>
+      <c r="O37" s="173"/>
+      <c r="P37" s="145"/>
+      <c r="Q37" s="145"/>
+      <c r="R37" s="145"/>
+      <c r="S37" s="145"/>
     </row>
-    <row r="38" spans="2:18" s="6" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B38" s="110">
+    <row r="38" spans="2:19" s="6" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B38" s="107">
         <v>17.5</v>
       </c>
-      <c r="C38" s="111" t="s">
+      <c r="C38" s="154" t="s">
         <v>28</v>
       </c>
-      <c r="D38" s="112"/>
-      <c r="E38" s="117">
+      <c r="D38" s="268"/>
+      <c r="E38" s="253">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F38" s="252">
+      <c r="F38" s="269">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G38" s="227"/>
-      <c r="H38" s="151"/>
-      <c r="I38" s="161" t="s">
+      <c r="G38" s="244"/>
+      <c r="H38" s="137"/>
+      <c r="I38" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="J38" s="131"/>
-      <c r="K38" s="116" t="str">
+      <c r="J38" s="124"/>
+      <c r="K38" s="111" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="L38" s="272"/>
-      <c r="M38" s="162"/>
-      <c r="N38" s="162"/>
-      <c r="O38" s="162"/>
-      <c r="P38" s="162"/>
-      <c r="Q38" s="162"/>
-      <c r="R38" s="162"/>
+      <c r="L38" s="282"/>
+      <c r="M38" s="171"/>
+      <c r="N38" s="282"/>
+      <c r="O38" s="173"/>
+      <c r="P38" s="145"/>
+      <c r="Q38" s="145"/>
+      <c r="R38" s="145"/>
+      <c r="S38" s="145"/>
     </row>
-    <row r="39" spans="2:18" s="6" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B39" s="132">
+    <row r="39" spans="2:19" s="6" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
+      <c r="B39" s="125">
         <v>17.600000000000001</v>
       </c>
-      <c r="C39" s="133" t="s">
+      <c r="C39" s="252" t="s">
         <v>29</v>
       </c>
-      <c r="D39" s="134"/>
-      <c r="E39" s="135">
+      <c r="D39" s="273"/>
+      <c r="E39" s="274">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F39" s="252">
+      <c r="F39" s="275">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G39" s="227"/>
-      <c r="H39" s="136"/>
-      <c r="I39" s="165" t="s">
+      <c r="G39" s="244"/>
+      <c r="H39" s="126"/>
+      <c r="I39" s="148" t="s">
         <v>77</v>
       </c>
-      <c r="J39" s="138"/>
-      <c r="K39" s="116" t="str">
+      <c r="J39" s="128"/>
+      <c r="K39" s="111" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="L39" s="272"/>
-      <c r="M39" s="162"/>
-      <c r="N39" s="162"/>
-      <c r="O39" s="162"/>
-      <c r="P39" s="162"/>
-      <c r="Q39" s="162"/>
-      <c r="R39" s="162"/>
+      <c r="L39" s="283"/>
+      <c r="M39" s="171"/>
+      <c r="N39" s="283"/>
+      <c r="O39" s="173"/>
+      <c r="P39" s="145"/>
+      <c r="Q39" s="145"/>
+      <c r="R39" s="145"/>
+      <c r="S39" s="145"/>
     </row>
-    <row r="40" spans="2:18" s="8" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B40" s="235" t="s">
+    <row r="40" spans="2:19" s="8" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B40" s="251" t="s">
         <v>79</v>
       </c>
-      <c r="C40" s="235"/>
-      <c r="D40" s="235"/>
-      <c r="E40" s="235"/>
-      <c r="F40" s="235"/>
-      <c r="G40" s="227"/>
-      <c r="H40" s="222"/>
-      <c r="I40" s="222"/>
-      <c r="J40" s="222"/>
-      <c r="K40" s="166"/>
-      <c r="L40" s="273"/>
-      <c r="M40" s="166"/>
-      <c r="N40" s="166"/>
-      <c r="O40" s="166"/>
-      <c r="P40" s="166"/>
-      <c r="Q40" s="166"/>
-      <c r="R40" s="166"/>
+      <c r="C40" s="251"/>
+      <c r="D40" s="251"/>
+      <c r="E40" s="251"/>
+      <c r="F40" s="251"/>
+      <c r="G40" s="244"/>
+      <c r="H40" s="213"/>
+      <c r="I40" s="213"/>
+      <c r="J40" s="213"/>
+      <c r="K40" s="149"/>
+      <c r="L40" s="280"/>
+      <c r="M40" s="171"/>
+      <c r="N40" s="280"/>
+      <c r="O40" s="149"/>
+      <c r="P40" s="149"/>
+      <c r="Q40" s="149"/>
+      <c r="R40" s="149"/>
+      <c r="S40" s="149"/>
     </row>
   </sheetData>
   <sheetProtection password="CC71" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
-  <mergeCells count="17">
-    <mergeCell ref="L8:L23"/>
-    <mergeCell ref="L26:L40"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B2:R2"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="H3:J5"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="H40:J40"/>
+  <mergeCells count="19">
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="H6:J6"/>
@@ -6784,212 +7338,309 @@
     <mergeCell ref="B24:F25"/>
     <mergeCell ref="H24:J25"/>
     <mergeCell ref="B40:F40"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B2:S2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="H3:J5"/>
+    <mergeCell ref="N8:N23"/>
+    <mergeCell ref="L8:L23"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="L26:L39"/>
+    <mergeCell ref="N26:N39"/>
   </mergeCells>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="42" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="100" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="cellIs" dxfId="41" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="95" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:F17">
-    <cfRule type="cellIs" dxfId="40" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="92" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="39" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="67" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="1" priority="49" operator="equal">
+    <cfRule type="expression" dxfId="55" priority="18">
+      <formula>D12&lt;D10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="66" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>D12&lt;D10</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="38" priority="47" operator="equal">
+  <conditionalFormatting sqref="E13:E15">
+    <cfRule type="cellIs" dxfId="53" priority="64" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="37" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="63" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="cellIs" dxfId="36" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="62" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="35" priority="44" operator="equal">
+    <cfRule type="expression" dxfId="50" priority="20">
+      <formula>(SUM($D$19:$D$23)&lt;&gt;E19)</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="61" operator="equal">
       <formula>0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="3">
-      <formula>(SUM($D$19:$D$23)&lt;&gt;E19)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="33" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="60" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="cellIs" dxfId="32" priority="42" operator="equal">
+    <cfRule type="expression" dxfId="47" priority="24">
+      <formula>IF(D20&gt;0,(SUM($D$19:$D$23)&lt;&gt;E19),"")</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="59" operator="equal">
       <formula>0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="31" priority="7">
-      <formula>IF(D20&gt;0,(SUM($D$19:$D$23)&lt;&gt;E19),"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="30" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="58" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="29" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="57" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="28" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="56" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="27" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="55" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="cellIs" dxfId="26" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="54" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="cellIs" dxfId="25" priority="36" operator="equal">
+    <cfRule type="expression" dxfId="40" priority="32">
+      <formula>IF(D36&gt;0,(SUM(D34,D35,D36,D37,D38,D39)&lt;&gt;E34),"")</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="53" operator="equal">
       <formula>0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="15">
-      <formula>IF(D36&gt;0,(SUM(D34,D35,D36,D37,D38,D39)&lt;&gt;E34),"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="cellIs" dxfId="23" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="52" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="cellIs" dxfId="22" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="51" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="cellIs" dxfId="21" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="50" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="cellIs" dxfId="20" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="49" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="expression" dxfId="19" priority="30">
+    <cfRule type="expression" dxfId="34" priority="47">
       <formula>D12&lt;D10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F19:F23">
-    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
+  <conditionalFormatting sqref="F19 F21:F23">
+    <cfRule type="cellIs" dxfId="33" priority="39" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F28:F32">
-    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
+  <conditionalFormatting sqref="F28:F31">
+    <cfRule type="cellIs" dxfId="32" priority="38" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F34:F39">
-    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
+  <conditionalFormatting sqref="F34:F35 F37:F39">
+    <cfRule type="cellIs" dxfId="31" priority="37" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:J5">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="19">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="36">
       <formula>LEN(TRIM(H3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
-    <cfRule type="expression" dxfId="14" priority="18">
+    <cfRule type="expression" dxfId="29" priority="35">
       <formula>IF(D34&gt;0,(SUM(D34,D35,D36,D37,D38,D39)&lt;&gt;E34),"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="expression" dxfId="13" priority="16">
+    <cfRule type="expression" dxfId="28" priority="33">
       <formula>IF(D35&gt;0,(SUM(D34,D35,D36,D37,D38,D39)&lt;&gt;E34),"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37">
-    <cfRule type="expression" dxfId="12" priority="14">
+    <cfRule type="expression" dxfId="27" priority="31">
       <formula>IF(D37&gt;0,(SUM(D34,D35,D36,D37,D38,D39)&lt;&gt;E34),"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38">
-    <cfRule type="expression" dxfId="11" priority="13">
+    <cfRule type="expression" dxfId="26" priority="30">
       <formula>IF(D38&gt;0,(SUM(D34,D35,D36,D37,D38,D39)&lt;&gt;E34),"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39">
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="25" priority="29">
       <formula>IF(D35&gt;0,(SUM(D34,D35,D36,D37,D38,D39)&lt;&gt;E34),"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="expression" dxfId="9" priority="11">
+    <cfRule type="expression" dxfId="24" priority="28">
       <formula>SUM(D34,D35,D36,D37,D38,D39)&lt;&gt;E34</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:L23">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="10">
+  <conditionalFormatting sqref="L8:M19 L21:M23 L20">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="27">
       <formula>LEN(TRIM(L8))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L26:L40">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="9">
+  <conditionalFormatting sqref="L26:M26 M33:M35 L40:M40 M37:M39 M27:M31">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="26">
       <formula>LEN(TRIM(L26))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="21" priority="25">
       <formula>IF(D19&gt;0,(SUM($D$19:$D$23)&lt;&gt;E19),"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="20" priority="23">
       <formula>IF(D21&gt;0,(SUM($D$19:$D$23)&lt;&gt;E19),"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="19" priority="22">
       <formula>IF(D22&gt;0,(SUM($D$19:$D$23)&lt;&gt;E19),"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="18" priority="21">
       <formula>IF(D23&gt;0,(SUM($D$19:$D$23)&lt;&gt;E19),"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
       <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N8:N23">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="15">
+      <formula>LEN(TRIM(N8))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M32">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="14">
+      <formula>LEN(TRIM(M32))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M36">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="13">
+      <formula>LEN(TRIM(M36))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N26 N40">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="12">
+      <formula>LEN(TRIM(N26))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M20">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="11">
+      <formula>LEN(TRIM(M20))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10">
+    <cfRule type="expression" dxfId="9" priority="10">
+      <formula>E10&gt;0&amp;F10&lt;0.85</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12">
+    <cfRule type="expression" dxfId="8" priority="9">
+      <formula>E12&gt;0&amp;F12&lt;0.95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F15">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>E15&gt;0&amp;F15&lt;0.85</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>E16&gt;0&amp;F16&lt;0.95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20">
+    <cfRule type="expression" dxfId="2" priority="5">
+      <formula>E20&gt;0&amp;F20&gt;0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F32">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F32">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>E32&gt;0&amp;F32&lt;0.95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F36">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F36">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>E36&gt;0&amp;F36&gt;0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>

</xml_diff>